<commit_message>
Alinhamento com professor dia 18/10
</commit_message>
<xml_diff>
--- a/Planilha de Monitoramento_Revisada_Luciene_Manhumirim.xlsx
+++ b/Planilha de Monitoramento_Revisada_Luciene_Manhumirim.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/df9355e39e7ae21c/Área de Trabalho/ProjetoBancosDeDados/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="22" documentId="11_2BF06DF04E5DE4C71D5F5451B3019729361D1167" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6E89DF9F-FF41-47B2-99A0-3F390BA5AFD1}"/>
+  <xr:revisionPtr revIDLastSave="45" documentId="11_2BF06DF04E5DE4C71D5F5451B3019729361D1167" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{714BD54E-7AAD-4F62-9565-7CF4CF0CBD34}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1066,17 +1066,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="165" fontId="6" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1104,6 +1093,17 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hiperlink" xfId="1" builtinId="8"/>
@@ -1344,6 +1344,158 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>1121075</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>96762</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>864241</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>71436</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="CaixaDeTexto 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4BCC385E-5470-C316-FBFA-EDB86A4C1D4B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="23814388" y="2966168"/>
+          <a:ext cx="4862853" cy="2474987"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="1100"/>
+            <a:t>DATA</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="1100" baseline="0"/>
+            <a:t> ATRIBUTO DO RELACIONAMENTO OCORRENCIA</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="pt-BR" sz="1100" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="1100" baseline="0"/>
+            <a:t>EQUIPE COMO ENTIDADE</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="pt-BR" sz="1100" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="1100" baseline="0"/>
+            <a:t>RO ANTERIORES - RELACIONAMENTO RECURSIV</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="pt-BR" sz="1100" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="1100" baseline="0"/>
+            <a:t>OFÍCIO FORMALIZA COMUNICAÇÃO ENTRE SETORES. PODE SER NOME OU EMAIL. OFICIO COMO ENTIDADE</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="pt-BR" sz="1100" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="1100" baseline="0"/>
+            <a:t>ORGAO DE DESTINO COMO ENTIDADE</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="pt-BR" sz="1100" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="1100" baseline="0"/>
+            <a:t>ORGAO DE DESTINO DO OFICIO TEM RELAÇÃO COM REGIONAL</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="pt-BR" sz="1100" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="pt-BR" sz="1100" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="pt-BR" sz="1100" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="pt-BR" sz="1100" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="pt-BR" sz="1100" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="pt-BR" sz="1100" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="pt-BR" sz="1100" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="pt-BR" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1606,8 +1758,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:U1003"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="O14" sqref="O14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75"/>
@@ -1720,7 +1872,7 @@
       <c r="G2" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="H2" s="25" t="s">
+      <c r="H2" s="20" t="s">
         <v>25</v>
       </c>
       <c r="I2" s="10">
@@ -1744,16 +1896,16 @@
         <v>28</v>
       </c>
       <c r="Q2" s="6"/>
-      <c r="R2" s="19">
+      <c r="R2" s="14">
         <v>-19.879231999999998</v>
       </c>
-      <c r="S2" s="26">
+      <c r="S2" s="21">
         <v>-44.142362800000001</v>
       </c>
-      <c r="T2" s="20" t="s">
+      <c r="T2" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="U2" s="20" t="s">
+      <c r="U2" s="15" t="s">
         <v>30</v>
       </c>
     </row>
@@ -1779,7 +1931,7 @@
       <c r="G3" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="H3" s="21" t="s">
+      <c r="H3" s="16" t="s">
         <v>34</v>
       </c>
       <c r="I3" s="11">
@@ -1804,17 +1956,17 @@
       <c r="P3" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="Q3" s="22">
+      <c r="Q3" s="17">
         <v>45127</v>
       </c>
-      <c r="R3" s="19">
+      <c r="R3" s="14">
         <v>-19.825268999999999</v>
       </c>
-      <c r="S3" s="26">
+      <c r="S3" s="21">
         <v>-44.156440000000003</v>
       </c>
-      <c r="T3" s="23"/>
-      <c r="U3" s="23" t="s">
+      <c r="T3" s="18"/>
+      <c r="U3" s="18" t="s">
         <v>38</v>
       </c>
     </row>
@@ -1840,7 +1992,7 @@
       <c r="G4" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="H4" s="25" t="s">
+      <c r="H4" s="20" t="s">
         <v>25</v>
       </c>
       <c r="I4" s="11">
@@ -1866,14 +2018,14 @@
         <v>28</v>
       </c>
       <c r="Q4" s="8"/>
-      <c r="R4" s="19">
+      <c r="R4" s="14">
         <v>-19.832048</v>
       </c>
-      <c r="S4" s="26">
+      <c r="S4" s="21">
         <v>-44.154600000000002</v>
       </c>
-      <c r="T4" s="23"/>
-      <c r="U4" s="23" t="s">
+      <c r="T4" s="18"/>
+      <c r="U4" s="18" t="s">
         <v>43</v>
       </c>
     </row>
@@ -1899,7 +2051,7 @@
       <c r="G5" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="H5" s="21" t="s">
+      <c r="H5" s="16" t="s">
         <v>34</v>
       </c>
       <c r="I5" s="11">
@@ -1923,14 +2075,14 @@
         <v>28</v>
       </c>
       <c r="Q5" s="8"/>
-      <c r="R5" s="19">
+      <c r="R5" s="14">
         <v>-19.822685</v>
       </c>
-      <c r="S5" s="26">
+      <c r="S5" s="21">
         <v>-44.146169</v>
       </c>
-      <c r="T5" s="23"/>
-      <c r="U5" s="23" t="s">
+      <c r="T5" s="18"/>
+      <c r="U5" s="18" t="s">
         <v>48</v>
       </c>
     </row>
@@ -1956,7 +2108,7 @@
       <c r="G6" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="H6" s="21" t="s">
+      <c r="H6" s="16" t="s">
         <v>34</v>
       </c>
       <c r="I6" s="11">
@@ -1982,14 +2134,14 @@
         <v>28</v>
       </c>
       <c r="Q6" s="8"/>
-      <c r="R6" s="19">
+      <c r="R6" s="14">
         <v>-19.821555</v>
       </c>
-      <c r="S6" s="26">
+      <c r="S6" s="21">
         <v>-44.137194000000001</v>
       </c>
-      <c r="T6" s="23"/>
-      <c r="U6" s="23" t="s">
+      <c r="T6" s="18"/>
+      <c r="U6" s="18" t="s">
         <v>50</v>
       </c>
     </row>
@@ -2015,7 +2167,7 @@
       <c r="G7" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="H7" s="21" t="s">
+      <c r="H7" s="16" t="s">
         <v>34</v>
       </c>
       <c r="I7" s="11">
@@ -2039,14 +2191,14 @@
         <v>28</v>
       </c>
       <c r="Q7" s="8"/>
-      <c r="R7" s="19">
+      <c r="R7" s="14">
         <v>-19.828685</v>
       </c>
-      <c r="S7" s="26">
+      <c r="S7" s="21">
         <v>-44.148451999999999</v>
       </c>
-      <c r="T7" s="23"/>
-      <c r="U7" s="23" t="s">
+      <c r="T7" s="18"/>
+      <c r="U7" s="18" t="s">
         <v>54</v>
       </c>
     </row>
@@ -2072,7 +2224,7 @@
       <c r="G8" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="H8" s="21" t="s">
+      <c r="H8" s="16" t="s">
         <v>34</v>
       </c>
       <c r="I8" s="11">
@@ -2098,1392 +2250,1392 @@
         <v>28</v>
       </c>
       <c r="Q8" s="8"/>
-      <c r="R8" s="19">
+      <c r="R8" s="14">
         <v>-19.866872000000001</v>
       </c>
-      <c r="S8" s="26">
+      <c r="S8" s="21">
         <v>-44.044767</v>
       </c>
-      <c r="T8" s="23"/>
-      <c r="U8" s="23" t="s">
+      <c r="T8" s="18"/>
+      <c r="U8" s="18" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="9" spans="1:21">
-      <c r="A9" s="21"/>
-      <c r="B9" s="21"/>
-      <c r="C9" s="21"/>
-      <c r="D9" s="21"/>
-      <c r="E9" s="21"/>
-      <c r="F9" s="21"/>
-      <c r="G9" s="21"/>
-      <c r="H9" s="25"/>
-      <c r="I9" s="21"/>
-      <c r="J9" s="21"/>
-      <c r="K9" s="21"/>
-      <c r="L9" s="21"/>
-      <c r="M9" s="21"/>
-      <c r="N9" s="21"/>
-      <c r="O9" s="21"/>
-      <c r="P9" s="21"/>
-      <c r="Q9" s="21"/>
-      <c r="R9" s="21"/>
-      <c r="S9" s="21"/>
-      <c r="T9" s="21"/>
-      <c r="U9" s="21"/>
+      <c r="A9" s="16"/>
+      <c r="B9" s="16"/>
+      <c r="C9" s="16"/>
+      <c r="D9" s="16"/>
+      <c r="E9" s="16"/>
+      <c r="F9" s="16"/>
+      <c r="G9" s="16"/>
+      <c r="H9" s="20"/>
+      <c r="I9" s="16"/>
+      <c r="J9" s="16"/>
+      <c r="K9" s="16"/>
+      <c r="L9" s="16"/>
+      <c r="M9" s="16"/>
+      <c r="N9" s="16"/>
+      <c r="O9" s="16"/>
+      <c r="P9" s="16"/>
+      <c r="Q9" s="16"/>
+      <c r="R9" s="16"/>
+      <c r="S9" s="16"/>
+      <c r="T9" s="16"/>
+      <c r="U9" s="16"/>
     </row>
     <row r="10" spans="1:21" ht="63.75">
-      <c r="A10" s="24" t="s">
+      <c r="A10" s="19" t="s">
         <v>58</v>
       </c>
-      <c r="B10" s="24" t="s">
+      <c r="B10" s="19" t="s">
         <v>59</v>
       </c>
-      <c r="C10" s="24" t="s">
+      <c r="C10" s="19" t="s">
         <v>59</v>
       </c>
-      <c r="D10" s="24" t="s">
+      <c r="D10" s="19" t="s">
         <v>59</v>
       </c>
-      <c r="E10" s="24" t="s">
+      <c r="E10" s="19" t="s">
         <v>60</v>
       </c>
-      <c r="F10" s="24" t="s">
+      <c r="F10" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="G10" s="24" t="s">
+      <c r="G10" s="19" t="s">
         <v>62</v>
       </c>
-      <c r="H10" s="24" t="s">
+      <c r="H10" s="19" t="s">
         <v>63</v>
       </c>
-      <c r="I10" s="24" t="s">
+      <c r="I10" s="19" t="s">
         <v>64</v>
       </c>
-      <c r="J10" s="24" t="s">
+      <c r="J10" s="19" t="s">
         <v>59</v>
       </c>
-      <c r="K10" s="24" t="s">
+      <c r="K10" s="19" t="s">
         <v>65</v>
       </c>
-      <c r="L10" s="24" t="s">
+      <c r="L10" s="19" t="s">
         <v>59</v>
       </c>
-      <c r="M10" s="24" t="s">
+      <c r="M10" s="19" t="s">
         <v>59</v>
       </c>
-      <c r="N10" s="24" t="s">
+      <c r="N10" s="19" t="s">
         <v>59</v>
       </c>
-      <c r="O10" s="24" t="s">
+      <c r="O10" s="19" t="s">
         <v>66</v>
       </c>
-      <c r="P10" s="24" t="s">
+      <c r="P10" s="19" t="s">
         <v>66</v>
       </c>
-      <c r="Q10" s="24" t="s">
+      <c r="Q10" s="19" t="s">
         <v>64</v>
       </c>
-      <c r="R10" s="24" t="s">
+      <c r="R10" s="19" t="s">
         <v>67</v>
       </c>
-      <c r="S10" s="24" t="s">
+      <c r="S10" s="19" t="s">
         <v>67</v>
       </c>
-      <c r="T10" s="27" t="s">
+      <c r="T10" s="22" t="s">
         <v>68</v>
       </c>
-      <c r="U10" s="24" t="s">
+      <c r="U10" s="19" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="11" spans="1:21">
-      <c r="A11" s="21"/>
-      <c r="B11" s="21"/>
-      <c r="C11" s="21"/>
-      <c r="D11" s="21"/>
-      <c r="E11" s="21"/>
-      <c r="F11" s="21"/>
-      <c r="G11" s="21"/>
-      <c r="H11" s="25"/>
-      <c r="I11" s="21"/>
-      <c r="J11" s="21"/>
-      <c r="K11" s="21"/>
-      <c r="L11" s="21"/>
-      <c r="M11" s="21"/>
-      <c r="N11" s="21"/>
-      <c r="O11" s="21"/>
-      <c r="P11" s="21"/>
-      <c r="Q11" s="21"/>
-      <c r="R11" s="21"/>
-      <c r="S11" s="21"/>
-      <c r="T11" s="21"/>
-      <c r="U11" s="21"/>
+      <c r="A11" s="16"/>
+      <c r="B11" s="16"/>
+      <c r="C11" s="16"/>
+      <c r="D11" s="16"/>
+      <c r="E11" s="16"/>
+      <c r="F11" s="16"/>
+      <c r="G11" s="16"/>
+      <c r="H11" s="20"/>
+      <c r="I11" s="16"/>
+      <c r="J11" s="16"/>
+      <c r="K11" s="16"/>
+      <c r="L11" s="16"/>
+      <c r="M11" s="16"/>
+      <c r="N11" s="16"/>
+      <c r="O11" s="16"/>
+      <c r="P11" s="16"/>
+      <c r="Q11" s="16"/>
+      <c r="R11" s="16"/>
+      <c r="S11" s="16"/>
+      <c r="T11" s="16"/>
+      <c r="U11" s="16"/>
     </row>
     <row r="12" spans="1:21">
-      <c r="A12" s="21"/>
-      <c r="B12" s="21"/>
-      <c r="C12" s="21"/>
-      <c r="D12" s="21"/>
-      <c r="E12" s="21"/>
-      <c r="F12" s="21"/>
-      <c r="G12" s="21"/>
-      <c r="H12" s="25"/>
-      <c r="I12" s="21"/>
-      <c r="J12" s="21"/>
-      <c r="K12" s="21"/>
-      <c r="L12" s="21"/>
-      <c r="M12" s="21"/>
-      <c r="N12" s="21"/>
-      <c r="O12" s="21"/>
-      <c r="P12" s="21"/>
-      <c r="Q12" s="21"/>
-      <c r="R12" s="21"/>
-      <c r="S12" s="21"/>
-      <c r="T12" s="21"/>
-      <c r="U12" s="21"/>
+      <c r="A12" s="16"/>
+      <c r="B12" s="16"/>
+      <c r="C12" s="16"/>
+      <c r="D12" s="16"/>
+      <c r="E12" s="16"/>
+      <c r="F12" s="16"/>
+      <c r="G12" s="16"/>
+      <c r="H12" s="20"/>
+      <c r="I12" s="16"/>
+      <c r="J12" s="16"/>
+      <c r="K12" s="16"/>
+      <c r="L12" s="16"/>
+      <c r="M12" s="16"/>
+      <c r="N12" s="16"/>
+      <c r="O12" s="16"/>
+      <c r="P12" s="16"/>
+      <c r="Q12" s="16"/>
+      <c r="R12" s="16"/>
+      <c r="S12" s="16"/>
+      <c r="T12" s="16"/>
+      <c r="U12" s="16"/>
     </row>
     <row r="13" spans="1:21">
-      <c r="A13" s="21"/>
-      <c r="B13" s="21"/>
-      <c r="C13" s="21"/>
-      <c r="D13" s="21"/>
-      <c r="E13" s="21"/>
-      <c r="F13" s="21"/>
-      <c r="G13" s="21"/>
-      <c r="H13" s="25"/>
-      <c r="I13" s="21"/>
-      <c r="J13" s="21"/>
-      <c r="K13" s="21"/>
-      <c r="L13" s="21"/>
-      <c r="M13" s="21"/>
-      <c r="N13" s="21"/>
-      <c r="O13" s="21"/>
-      <c r="P13" s="21"/>
-      <c r="Q13" s="21"/>
-      <c r="R13" s="21"/>
-      <c r="S13" s="21"/>
-      <c r="T13" s="21"/>
-      <c r="U13" s="21"/>
+      <c r="A13" s="16"/>
+      <c r="B13" s="16"/>
+      <c r="C13" s="16"/>
+      <c r="D13" s="16"/>
+      <c r="E13" s="16"/>
+      <c r="F13" s="16"/>
+      <c r="G13" s="16"/>
+      <c r="H13" s="20"/>
+      <c r="I13" s="16"/>
+      <c r="J13" s="16"/>
+      <c r="K13" s="16"/>
+      <c r="L13" s="16"/>
+      <c r="M13" s="16"/>
+      <c r="N13" s="16"/>
+      <c r="O13" s="16"/>
+      <c r="P13" s="16"/>
+      <c r="Q13" s="16"/>
+      <c r="R13" s="16"/>
+      <c r="S13" s="16"/>
+      <c r="T13" s="16"/>
+      <c r="U13" s="16"/>
     </row>
     <row r="14" spans="1:21">
-      <c r="A14" s="21"/>
-      <c r="B14" s="21"/>
-      <c r="C14" s="21"/>
-      <c r="D14" s="21"/>
-      <c r="E14" s="21"/>
-      <c r="F14" s="21"/>
-      <c r="G14" s="21"/>
-      <c r="H14" s="25"/>
-      <c r="I14" s="21"/>
-      <c r="J14" s="21"/>
-      <c r="K14" s="21"/>
-      <c r="L14" s="21"/>
-      <c r="M14" s="21"/>
-      <c r="N14" s="21"/>
-      <c r="O14" s="21"/>
-      <c r="P14" s="21"/>
-      <c r="Q14" s="21"/>
-      <c r="R14" s="21"/>
-      <c r="S14" s="21"/>
-      <c r="T14" s="21"/>
-      <c r="U14" s="21"/>
+      <c r="A14" s="16"/>
+      <c r="B14" s="16"/>
+      <c r="C14" s="16"/>
+      <c r="D14" s="16"/>
+      <c r="E14" s="16"/>
+      <c r="F14" s="16"/>
+      <c r="G14" s="16"/>
+      <c r="H14" s="20"/>
+      <c r="I14" s="16"/>
+      <c r="J14" s="16"/>
+      <c r="K14" s="16"/>
+      <c r="L14" s="16"/>
+      <c r="M14" s="16"/>
+      <c r="N14" s="16"/>
+      <c r="O14" s="16"/>
+      <c r="P14" s="16"/>
+      <c r="Q14" s="16"/>
+      <c r="R14" s="16"/>
+      <c r="S14" s="16"/>
+      <c r="T14" s="16"/>
+      <c r="U14" s="16"/>
     </row>
     <row r="15" spans="1:21">
-      <c r="A15" s="21"/>
-      <c r="B15" s="21"/>
-      <c r="C15" s="21"/>
-      <c r="D15" s="21"/>
-      <c r="E15" s="21"/>
-      <c r="F15" s="21"/>
-      <c r="G15" s="21"/>
-      <c r="H15" s="25"/>
-      <c r="I15" s="21"/>
-      <c r="J15" s="21"/>
-      <c r="K15" s="21"/>
-      <c r="L15" s="21"/>
-      <c r="M15" s="21"/>
-      <c r="N15" s="21"/>
-      <c r="O15" s="21"/>
-      <c r="P15" s="21"/>
-      <c r="Q15" s="21"/>
-      <c r="R15" s="21"/>
-      <c r="S15" s="21"/>
-      <c r="T15" s="21"/>
-      <c r="U15" s="21"/>
+      <c r="A15" s="16"/>
+      <c r="B15" s="16"/>
+      <c r="C15" s="16"/>
+      <c r="D15" s="16"/>
+      <c r="E15" s="16"/>
+      <c r="F15" s="16"/>
+      <c r="G15" s="16"/>
+      <c r="H15" s="20"/>
+      <c r="I15" s="16"/>
+      <c r="J15" s="16"/>
+      <c r="K15" s="16"/>
+      <c r="L15" s="16"/>
+      <c r="M15" s="16"/>
+      <c r="N15" s="16"/>
+      <c r="O15" s="16"/>
+      <c r="P15" s="16"/>
+      <c r="Q15" s="16"/>
+      <c r="R15" s="16"/>
+      <c r="S15" s="16"/>
+      <c r="T15" s="16"/>
+      <c r="U15" s="16"/>
     </row>
     <row r="16" spans="1:21">
-      <c r="A16" s="21"/>
-      <c r="B16" s="21"/>
-      <c r="C16" s="21"/>
-      <c r="D16" s="21"/>
-      <c r="E16" s="21"/>
-      <c r="F16" s="21"/>
-      <c r="G16" s="21"/>
-      <c r="H16" s="25"/>
-      <c r="I16" s="21"/>
-      <c r="J16" s="21"/>
-      <c r="K16" s="21"/>
-      <c r="L16" s="21"/>
-      <c r="M16" s="21"/>
-      <c r="N16" s="21"/>
-      <c r="O16" s="21"/>
-      <c r="P16" s="21"/>
-      <c r="Q16" s="21"/>
-      <c r="R16" s="21"/>
-      <c r="S16" s="21"/>
-      <c r="T16" s="21"/>
-      <c r="U16" s="21"/>
+      <c r="A16" s="16"/>
+      <c r="B16" s="16"/>
+      <c r="C16" s="16"/>
+      <c r="D16" s="16"/>
+      <c r="E16" s="16"/>
+      <c r="F16" s="16"/>
+      <c r="G16" s="16"/>
+      <c r="H16" s="20"/>
+      <c r="I16" s="16"/>
+      <c r="J16" s="16"/>
+      <c r="K16" s="16"/>
+      <c r="L16" s="16"/>
+      <c r="M16" s="16"/>
+      <c r="N16" s="16"/>
+      <c r="O16" s="16"/>
+      <c r="P16" s="16"/>
+      <c r="Q16" s="16"/>
+      <c r="R16" s="16"/>
+      <c r="S16" s="16"/>
+      <c r="T16" s="16"/>
+      <c r="U16" s="16"/>
     </row>
     <row r="17" spans="1:21">
-      <c r="A17" s="21"/>
-      <c r="B17" s="21"/>
-      <c r="C17" s="21"/>
-      <c r="D17" s="21"/>
-      <c r="E17" s="21"/>
-      <c r="F17" s="21"/>
-      <c r="G17" s="21"/>
-      <c r="H17" s="25"/>
-      <c r="I17" s="21"/>
-      <c r="J17" s="21"/>
-      <c r="K17" s="21"/>
-      <c r="L17" s="21"/>
-      <c r="M17" s="21"/>
-      <c r="N17" s="21"/>
-      <c r="O17" s="21"/>
-      <c r="P17" s="21"/>
-      <c r="Q17" s="21"/>
-      <c r="R17" s="21"/>
-      <c r="S17" s="21"/>
-      <c r="T17" s="21"/>
-      <c r="U17" s="21"/>
+      <c r="A17" s="16"/>
+      <c r="B17" s="16"/>
+      <c r="C17" s="16"/>
+      <c r="D17" s="16"/>
+      <c r="E17" s="16"/>
+      <c r="F17" s="16"/>
+      <c r="G17" s="16"/>
+      <c r="H17" s="20"/>
+      <c r="I17" s="16"/>
+      <c r="J17" s="16"/>
+      <c r="K17" s="16"/>
+      <c r="L17" s="16"/>
+      <c r="M17" s="16"/>
+      <c r="N17" s="16"/>
+      <c r="O17" s="16"/>
+      <c r="P17" s="16"/>
+      <c r="Q17" s="16"/>
+      <c r="R17" s="16"/>
+      <c r="S17" s="16"/>
+      <c r="T17" s="16"/>
+      <c r="U17" s="16"/>
     </row>
     <row r="18" spans="1:21">
-      <c r="A18" s="21"/>
-      <c r="B18" s="21"/>
-      <c r="C18" s="21"/>
-      <c r="D18" s="21"/>
-      <c r="E18" s="21"/>
-      <c r="F18" s="21"/>
-      <c r="G18" s="21"/>
-      <c r="H18" s="25"/>
-      <c r="I18" s="21"/>
-      <c r="J18" s="21"/>
-      <c r="K18" s="21"/>
-      <c r="L18" s="21"/>
-      <c r="M18" s="21"/>
-      <c r="N18" s="21"/>
-      <c r="O18" s="21"/>
-      <c r="P18" s="21"/>
-      <c r="Q18" s="21"/>
-      <c r="R18" s="21"/>
-      <c r="S18" s="21"/>
-      <c r="T18" s="21"/>
-      <c r="U18" s="21"/>
+      <c r="A18" s="16"/>
+      <c r="B18" s="16"/>
+      <c r="C18" s="16"/>
+      <c r="D18" s="16"/>
+      <c r="E18" s="16"/>
+      <c r="F18" s="16"/>
+      <c r="G18" s="16"/>
+      <c r="H18" s="20"/>
+      <c r="I18" s="16"/>
+      <c r="J18" s="16"/>
+      <c r="K18" s="16"/>
+      <c r="L18" s="16"/>
+      <c r="M18" s="16"/>
+      <c r="N18" s="16"/>
+      <c r="O18" s="16"/>
+      <c r="P18" s="16"/>
+      <c r="Q18" s="16"/>
+      <c r="R18" s="16"/>
+      <c r="S18" s="16"/>
+      <c r="T18" s="16"/>
+      <c r="U18" s="16"/>
     </row>
     <row r="19" spans="1:21">
-      <c r="A19" s="21"/>
-      <c r="B19" s="21"/>
-      <c r="C19" s="21"/>
-      <c r="D19" s="21"/>
-      <c r="E19" s="21"/>
-      <c r="F19" s="21"/>
-      <c r="G19" s="21"/>
-      <c r="H19" s="25"/>
-      <c r="I19" s="21"/>
-      <c r="J19" s="21"/>
-      <c r="K19" s="21"/>
-      <c r="L19" s="21"/>
-      <c r="M19" s="21"/>
-      <c r="N19" s="21"/>
-      <c r="O19" s="21"/>
-      <c r="P19" s="21"/>
-      <c r="Q19" s="21"/>
-      <c r="R19" s="21"/>
-      <c r="S19" s="21"/>
-      <c r="T19" s="21"/>
-      <c r="U19" s="21"/>
+      <c r="A19" s="16"/>
+      <c r="B19" s="16"/>
+      <c r="C19" s="16"/>
+      <c r="D19" s="16"/>
+      <c r="E19" s="16"/>
+      <c r="F19" s="16"/>
+      <c r="G19" s="16"/>
+      <c r="H19" s="20"/>
+      <c r="I19" s="16"/>
+      <c r="J19" s="16"/>
+      <c r="K19" s="16"/>
+      <c r="L19" s="16"/>
+      <c r="M19" s="16"/>
+      <c r="N19" s="16"/>
+      <c r="O19" s="16"/>
+      <c r="P19" s="16"/>
+      <c r="Q19" s="16"/>
+      <c r="R19" s="16"/>
+      <c r="S19" s="16"/>
+      <c r="T19" s="16"/>
+      <c r="U19" s="16"/>
     </row>
     <row r="20" spans="1:21">
-      <c r="A20" s="21"/>
-      <c r="B20" s="21"/>
-      <c r="C20" s="21"/>
-      <c r="D20" s="21"/>
-      <c r="E20" s="21"/>
-      <c r="F20" s="21"/>
-      <c r="G20" s="21"/>
-      <c r="H20" s="25"/>
-      <c r="I20" s="21"/>
-      <c r="J20" s="21"/>
-      <c r="K20" s="21"/>
-      <c r="L20" s="21"/>
-      <c r="M20" s="21"/>
-      <c r="N20" s="21"/>
-      <c r="O20" s="21"/>
-      <c r="P20" s="21"/>
-      <c r="Q20" s="21"/>
-      <c r="R20" s="21"/>
-      <c r="S20" s="21"/>
-      <c r="T20" s="21"/>
-      <c r="U20" s="21"/>
+      <c r="A20" s="16"/>
+      <c r="B20" s="16"/>
+      <c r="C20" s="16"/>
+      <c r="D20" s="16"/>
+      <c r="E20" s="16"/>
+      <c r="F20" s="16"/>
+      <c r="G20" s="16"/>
+      <c r="H20" s="20"/>
+      <c r="I20" s="16"/>
+      <c r="J20" s="16"/>
+      <c r="K20" s="16"/>
+      <c r="L20" s="16"/>
+      <c r="M20" s="16"/>
+      <c r="N20" s="16"/>
+      <c r="O20" s="16"/>
+      <c r="P20" s="16"/>
+      <c r="Q20" s="16"/>
+      <c r="R20" s="16"/>
+      <c r="S20" s="16"/>
+      <c r="T20" s="16"/>
+      <c r="U20" s="16"/>
     </row>
     <row r="21" spans="1:21">
-      <c r="A21" s="21"/>
-      <c r="B21" s="21"/>
-      <c r="C21" s="21"/>
-      <c r="D21" s="21"/>
-      <c r="E21" s="21"/>
-      <c r="F21" s="21"/>
-      <c r="G21" s="21"/>
-      <c r="H21" s="25"/>
-      <c r="I21" s="21"/>
-      <c r="J21" s="21"/>
-      <c r="K21" s="21"/>
-      <c r="L21" s="21"/>
-      <c r="M21" s="21"/>
-      <c r="N21" s="21"/>
-      <c r="O21" s="21"/>
-      <c r="P21" s="21"/>
-      <c r="Q21" s="21"/>
-      <c r="R21" s="21"/>
-      <c r="S21" s="21"/>
-      <c r="T21" s="21"/>
-      <c r="U21" s="21"/>
+      <c r="A21" s="16"/>
+      <c r="B21" s="16"/>
+      <c r="C21" s="16"/>
+      <c r="D21" s="16"/>
+      <c r="E21" s="16"/>
+      <c r="F21" s="16"/>
+      <c r="G21" s="16"/>
+      <c r="H21" s="20"/>
+      <c r="I21" s="16"/>
+      <c r="J21" s="16"/>
+      <c r="K21" s="16"/>
+      <c r="L21" s="16"/>
+      <c r="M21" s="16"/>
+      <c r="N21" s="16"/>
+      <c r="O21" s="16"/>
+      <c r="P21" s="16"/>
+      <c r="Q21" s="16"/>
+      <c r="R21" s="16"/>
+      <c r="S21" s="16"/>
+      <c r="T21" s="16"/>
+      <c r="U21" s="16"/>
     </row>
     <row r="22" spans="1:21">
-      <c r="A22" s="21"/>
-      <c r="B22" s="21"/>
-      <c r="C22" s="21"/>
-      <c r="D22" s="21"/>
-      <c r="E22" s="21"/>
-      <c r="F22" s="21"/>
-      <c r="G22" s="21"/>
-      <c r="H22" s="25"/>
-      <c r="I22" s="21"/>
-      <c r="J22" s="21"/>
-      <c r="K22" s="21"/>
-      <c r="L22" s="21"/>
-      <c r="M22" s="21"/>
-      <c r="N22" s="21"/>
-      <c r="O22" s="21"/>
-      <c r="P22" s="21"/>
-      <c r="Q22" s="21"/>
-      <c r="R22" s="21"/>
-      <c r="S22" s="21"/>
-      <c r="T22" s="21"/>
-      <c r="U22" s="21"/>
+      <c r="A22" s="16"/>
+      <c r="B22" s="16"/>
+      <c r="C22" s="16"/>
+      <c r="D22" s="16"/>
+      <c r="E22" s="16"/>
+      <c r="F22" s="16"/>
+      <c r="G22" s="16"/>
+      <c r="H22" s="20"/>
+      <c r="I22" s="16"/>
+      <c r="J22" s="16"/>
+      <c r="K22" s="16"/>
+      <c r="L22" s="16"/>
+      <c r="M22" s="16"/>
+      <c r="N22" s="16"/>
+      <c r="O22" s="16"/>
+      <c r="P22" s="16"/>
+      <c r="Q22" s="16"/>
+      <c r="R22" s="16"/>
+      <c r="S22" s="16"/>
+      <c r="T22" s="16"/>
+      <c r="U22" s="16"/>
     </row>
     <row r="23" spans="1:21">
-      <c r="A23" s="21"/>
-      <c r="B23" s="21"/>
-      <c r="C23" s="21"/>
-      <c r="D23" s="21"/>
-      <c r="E23" s="21"/>
-      <c r="F23" s="21"/>
-      <c r="G23" s="21"/>
-      <c r="H23" s="25"/>
-      <c r="I23" s="21"/>
-      <c r="J23" s="21"/>
-      <c r="K23" s="21"/>
-      <c r="L23" s="21"/>
-      <c r="M23" s="21"/>
-      <c r="N23" s="21"/>
-      <c r="O23" s="21"/>
-      <c r="P23" s="21"/>
-      <c r="Q23" s="21"/>
-      <c r="R23" s="21"/>
-      <c r="S23" s="21"/>
-      <c r="T23" s="21"/>
-      <c r="U23" s="21"/>
+      <c r="A23" s="16"/>
+      <c r="B23" s="16"/>
+      <c r="C23" s="16"/>
+      <c r="D23" s="16"/>
+      <c r="E23" s="16"/>
+      <c r="F23" s="16"/>
+      <c r="G23" s="16"/>
+      <c r="H23" s="20"/>
+      <c r="I23" s="16"/>
+      <c r="J23" s="16"/>
+      <c r="K23" s="16"/>
+      <c r="L23" s="16"/>
+      <c r="M23" s="16"/>
+      <c r="N23" s="16"/>
+      <c r="O23" s="16"/>
+      <c r="P23" s="16"/>
+      <c r="Q23" s="16"/>
+      <c r="R23" s="16"/>
+      <c r="S23" s="16"/>
+      <c r="T23" s="16"/>
+      <c r="U23" s="16"/>
     </row>
     <row r="24" spans="1:21">
-      <c r="A24" s="21"/>
-      <c r="B24" s="21"/>
-      <c r="C24" s="21"/>
-      <c r="D24" s="21"/>
-      <c r="E24" s="21"/>
-      <c r="F24" s="21"/>
-      <c r="G24" s="21"/>
-      <c r="H24" s="25"/>
-      <c r="I24" s="21"/>
-      <c r="J24" s="21"/>
-      <c r="K24" s="21"/>
-      <c r="L24" s="21"/>
-      <c r="M24" s="21"/>
-      <c r="N24" s="21"/>
-      <c r="O24" s="21"/>
-      <c r="P24" s="21"/>
-      <c r="Q24" s="21"/>
-      <c r="R24" s="21"/>
-      <c r="S24" s="21"/>
-      <c r="T24" s="21"/>
-      <c r="U24" s="21"/>
+      <c r="A24" s="16"/>
+      <c r="B24" s="16"/>
+      <c r="C24" s="16"/>
+      <c r="D24" s="16"/>
+      <c r="E24" s="16"/>
+      <c r="F24" s="16"/>
+      <c r="G24" s="16"/>
+      <c r="H24" s="20"/>
+      <c r="I24" s="16"/>
+      <c r="J24" s="16"/>
+      <c r="K24" s="16"/>
+      <c r="L24" s="16"/>
+      <c r="M24" s="16"/>
+      <c r="N24" s="16"/>
+      <c r="O24" s="16"/>
+      <c r="P24" s="16"/>
+      <c r="Q24" s="16"/>
+      <c r="R24" s="16"/>
+      <c r="S24" s="16"/>
+      <c r="T24" s="16"/>
+      <c r="U24" s="16"/>
     </row>
     <row r="25" spans="1:21">
-      <c r="A25" s="21"/>
-      <c r="B25" s="21"/>
-      <c r="C25" s="21"/>
-      <c r="D25" s="21"/>
-      <c r="E25" s="21"/>
-      <c r="F25" s="21"/>
-      <c r="G25" s="21"/>
-      <c r="H25" s="25"/>
-      <c r="I25" s="21"/>
-      <c r="J25" s="21"/>
-      <c r="K25" s="21"/>
-      <c r="L25" s="21"/>
-      <c r="M25" s="21"/>
-      <c r="N25" s="21"/>
-      <c r="O25" s="21"/>
-      <c r="P25" s="21"/>
-      <c r="Q25" s="21"/>
-      <c r="R25" s="21"/>
-      <c r="S25" s="21"/>
-      <c r="T25" s="21"/>
-      <c r="U25" s="21"/>
+      <c r="A25" s="16"/>
+      <c r="B25" s="16"/>
+      <c r="C25" s="16"/>
+      <c r="D25" s="16"/>
+      <c r="E25" s="16"/>
+      <c r="F25" s="16"/>
+      <c r="G25" s="16"/>
+      <c r="H25" s="20"/>
+      <c r="I25" s="16"/>
+      <c r="J25" s="16"/>
+      <c r="K25" s="16"/>
+      <c r="L25" s="16"/>
+      <c r="M25" s="16"/>
+      <c r="N25" s="16"/>
+      <c r="O25" s="16"/>
+      <c r="P25" s="16"/>
+      <c r="Q25" s="16"/>
+      <c r="R25" s="16"/>
+      <c r="S25" s="16"/>
+      <c r="T25" s="16"/>
+      <c r="U25" s="16"/>
     </row>
     <row r="26" spans="1:21">
-      <c r="A26" s="21"/>
-      <c r="B26" s="21"/>
-      <c r="C26" s="21"/>
-      <c r="D26" s="21"/>
-      <c r="E26" s="21"/>
-      <c r="F26" s="21"/>
-      <c r="G26" s="21"/>
-      <c r="H26" s="25"/>
-      <c r="I26" s="21"/>
-      <c r="J26" s="21"/>
-      <c r="K26" s="21"/>
-      <c r="L26" s="21"/>
-      <c r="M26" s="21"/>
-      <c r="N26" s="21"/>
-      <c r="O26" s="21"/>
-      <c r="P26" s="21"/>
-      <c r="Q26" s="21"/>
-      <c r="R26" s="21"/>
-      <c r="S26" s="21"/>
-      <c r="T26" s="21"/>
-      <c r="U26" s="21"/>
+      <c r="A26" s="16"/>
+      <c r="B26" s="16"/>
+      <c r="C26" s="16"/>
+      <c r="D26" s="16"/>
+      <c r="E26" s="16"/>
+      <c r="F26" s="16"/>
+      <c r="G26" s="16"/>
+      <c r="H26" s="20"/>
+      <c r="I26" s="16"/>
+      <c r="J26" s="16"/>
+      <c r="K26" s="16"/>
+      <c r="L26" s="16"/>
+      <c r="M26" s="16"/>
+      <c r="N26" s="16"/>
+      <c r="O26" s="16"/>
+      <c r="P26" s="16"/>
+      <c r="Q26" s="16"/>
+      <c r="R26" s="16"/>
+      <c r="S26" s="16"/>
+      <c r="T26" s="16"/>
+      <c r="U26" s="16"/>
     </row>
     <row r="27" spans="1:21">
-      <c r="A27" s="21"/>
-      <c r="B27" s="21"/>
-      <c r="C27" s="21"/>
-      <c r="D27" s="21"/>
-      <c r="E27" s="21"/>
-      <c r="F27" s="21"/>
-      <c r="G27" s="21"/>
-      <c r="H27" s="25"/>
-      <c r="I27" s="21"/>
-      <c r="J27" s="21"/>
-      <c r="K27" s="21"/>
-      <c r="L27" s="21"/>
-      <c r="M27" s="21"/>
-      <c r="N27" s="21"/>
-      <c r="O27" s="21"/>
-      <c r="P27" s="21"/>
-      <c r="Q27" s="21"/>
-      <c r="R27" s="21"/>
-      <c r="S27" s="21"/>
-      <c r="T27" s="21"/>
-      <c r="U27" s="21"/>
+      <c r="A27" s="16"/>
+      <c r="B27" s="16"/>
+      <c r="C27" s="16"/>
+      <c r="D27" s="16"/>
+      <c r="E27" s="16"/>
+      <c r="F27" s="16"/>
+      <c r="G27" s="16"/>
+      <c r="H27" s="20"/>
+      <c r="I27" s="16"/>
+      <c r="J27" s="16"/>
+      <c r="K27" s="16"/>
+      <c r="L27" s="16"/>
+      <c r="M27" s="16"/>
+      <c r="N27" s="16"/>
+      <c r="O27" s="16"/>
+      <c r="P27" s="16"/>
+      <c r="Q27" s="16"/>
+      <c r="R27" s="16"/>
+      <c r="S27" s="16"/>
+      <c r="T27" s="16"/>
+      <c r="U27" s="16"/>
     </row>
     <row r="28" spans="1:21">
-      <c r="A28" s="21"/>
-      <c r="B28" s="21"/>
-      <c r="C28" s="21"/>
-      <c r="D28" s="21"/>
-      <c r="E28" s="21"/>
-      <c r="F28" s="21"/>
-      <c r="G28" s="21"/>
-      <c r="H28" s="25"/>
-      <c r="I28" s="21"/>
-      <c r="J28" s="21"/>
-      <c r="K28" s="21"/>
-      <c r="L28" s="21"/>
-      <c r="M28" s="21"/>
-      <c r="N28" s="21"/>
-      <c r="O28" s="21"/>
-      <c r="P28" s="21"/>
-      <c r="Q28" s="21"/>
-      <c r="R28" s="21"/>
-      <c r="S28" s="21"/>
-      <c r="T28" s="21"/>
-      <c r="U28" s="21"/>
+      <c r="A28" s="16"/>
+      <c r="B28" s="16"/>
+      <c r="C28" s="16"/>
+      <c r="D28" s="16"/>
+      <c r="E28" s="16"/>
+      <c r="F28" s="16"/>
+      <c r="G28" s="16"/>
+      <c r="H28" s="20"/>
+      <c r="I28" s="16"/>
+      <c r="J28" s="16"/>
+      <c r="K28" s="16"/>
+      <c r="L28" s="16"/>
+      <c r="M28" s="16"/>
+      <c r="N28" s="16"/>
+      <c r="O28" s="16"/>
+      <c r="P28" s="16"/>
+      <c r="Q28" s="16"/>
+      <c r="R28" s="16"/>
+      <c r="S28" s="16"/>
+      <c r="T28" s="16"/>
+      <c r="U28" s="16"/>
     </row>
     <row r="29" spans="1:21">
-      <c r="A29" s="21"/>
-      <c r="B29" s="21"/>
-      <c r="C29" s="21"/>
-      <c r="D29" s="21"/>
-      <c r="E29" s="21"/>
-      <c r="F29" s="21"/>
-      <c r="G29" s="21"/>
-      <c r="H29" s="25"/>
-      <c r="I29" s="21"/>
-      <c r="J29" s="21"/>
-      <c r="K29" s="21"/>
-      <c r="L29" s="21"/>
-      <c r="M29" s="21"/>
-      <c r="N29" s="21"/>
-      <c r="O29" s="21"/>
-      <c r="P29" s="21"/>
-      <c r="Q29" s="21"/>
-      <c r="R29" s="21"/>
-      <c r="S29" s="21"/>
-      <c r="T29" s="21"/>
-      <c r="U29" s="21"/>
+      <c r="A29" s="16"/>
+      <c r="B29" s="16"/>
+      <c r="C29" s="16"/>
+      <c r="D29" s="16"/>
+      <c r="E29" s="16"/>
+      <c r="F29" s="16"/>
+      <c r="G29" s="16"/>
+      <c r="H29" s="20"/>
+      <c r="I29" s="16"/>
+      <c r="J29" s="16"/>
+      <c r="K29" s="16"/>
+      <c r="L29" s="16"/>
+      <c r="M29" s="16"/>
+      <c r="N29" s="16"/>
+      <c r="O29" s="16"/>
+      <c r="P29" s="16"/>
+      <c r="Q29" s="16"/>
+      <c r="R29" s="16"/>
+      <c r="S29" s="16"/>
+      <c r="T29" s="16"/>
+      <c r="U29" s="16"/>
     </row>
     <row r="30" spans="1:21">
-      <c r="A30" s="21"/>
-      <c r="B30" s="21"/>
-      <c r="C30" s="21"/>
-      <c r="D30" s="21"/>
-      <c r="E30" s="21"/>
-      <c r="F30" s="21"/>
-      <c r="G30" s="21"/>
-      <c r="H30" s="25"/>
-      <c r="I30" s="21"/>
-      <c r="J30" s="21"/>
-      <c r="K30" s="21"/>
-      <c r="L30" s="21"/>
-      <c r="M30" s="21"/>
-      <c r="N30" s="21"/>
-      <c r="O30" s="21"/>
-      <c r="P30" s="21"/>
-      <c r="Q30" s="21"/>
-      <c r="R30" s="21"/>
-      <c r="S30" s="21"/>
-      <c r="T30" s="21"/>
-      <c r="U30" s="21"/>
+      <c r="A30" s="16"/>
+      <c r="B30" s="16"/>
+      <c r="C30" s="16"/>
+      <c r="D30" s="16"/>
+      <c r="E30" s="16"/>
+      <c r="F30" s="16"/>
+      <c r="G30" s="16"/>
+      <c r="H30" s="20"/>
+      <c r="I30" s="16"/>
+      <c r="J30" s="16"/>
+      <c r="K30" s="16"/>
+      <c r="L30" s="16"/>
+      <c r="M30" s="16"/>
+      <c r="N30" s="16"/>
+      <c r="O30" s="16"/>
+      <c r="P30" s="16"/>
+      <c r="Q30" s="16"/>
+      <c r="R30" s="16"/>
+      <c r="S30" s="16"/>
+      <c r="T30" s="16"/>
+      <c r="U30" s="16"/>
     </row>
     <row r="31" spans="1:21">
-      <c r="A31" s="21"/>
-      <c r="B31" s="21"/>
-      <c r="C31" s="21"/>
-      <c r="D31" s="21"/>
-      <c r="E31" s="21"/>
-      <c r="F31" s="21"/>
-      <c r="G31" s="21"/>
-      <c r="H31" s="25"/>
-      <c r="I31" s="21"/>
-      <c r="J31" s="21"/>
-      <c r="K31" s="21"/>
-      <c r="L31" s="21"/>
-      <c r="M31" s="21"/>
-      <c r="N31" s="21"/>
-      <c r="O31" s="21"/>
-      <c r="P31" s="21"/>
-      <c r="Q31" s="21"/>
-      <c r="R31" s="21"/>
-      <c r="S31" s="21"/>
-      <c r="T31" s="21"/>
-      <c r="U31" s="21"/>
+      <c r="A31" s="16"/>
+      <c r="B31" s="16"/>
+      <c r="C31" s="16"/>
+      <c r="D31" s="16"/>
+      <c r="E31" s="16"/>
+      <c r="F31" s="16"/>
+      <c r="G31" s="16"/>
+      <c r="H31" s="20"/>
+      <c r="I31" s="16"/>
+      <c r="J31" s="16"/>
+      <c r="K31" s="16"/>
+      <c r="L31" s="16"/>
+      <c r="M31" s="16"/>
+      <c r="N31" s="16"/>
+      <c r="O31" s="16"/>
+      <c r="P31" s="16"/>
+      <c r="Q31" s="16"/>
+      <c r="R31" s="16"/>
+      <c r="S31" s="16"/>
+      <c r="T31" s="16"/>
+      <c r="U31" s="16"/>
     </row>
     <row r="32" spans="1:21">
-      <c r="A32" s="21"/>
-      <c r="B32" s="21"/>
-      <c r="C32" s="21"/>
-      <c r="D32" s="21"/>
-      <c r="E32" s="21"/>
-      <c r="F32" s="21"/>
-      <c r="G32" s="21"/>
-      <c r="H32" s="25"/>
-      <c r="I32" s="21"/>
-      <c r="J32" s="21"/>
-      <c r="K32" s="21"/>
-      <c r="L32" s="21"/>
-      <c r="M32" s="21"/>
-      <c r="N32" s="21"/>
-      <c r="O32" s="21"/>
-      <c r="P32" s="21"/>
-      <c r="Q32" s="21"/>
-      <c r="R32" s="21"/>
-      <c r="S32" s="21"/>
-      <c r="T32" s="21"/>
-      <c r="U32" s="21"/>
+      <c r="A32" s="16"/>
+      <c r="B32" s="16"/>
+      <c r="C32" s="16"/>
+      <c r="D32" s="16"/>
+      <c r="E32" s="16"/>
+      <c r="F32" s="16"/>
+      <c r="G32" s="16"/>
+      <c r="H32" s="20"/>
+      <c r="I32" s="16"/>
+      <c r="J32" s="16"/>
+      <c r="K32" s="16"/>
+      <c r="L32" s="16"/>
+      <c r="M32" s="16"/>
+      <c r="N32" s="16"/>
+      <c r="O32" s="16"/>
+      <c r="P32" s="16"/>
+      <c r="Q32" s="16"/>
+      <c r="R32" s="16"/>
+      <c r="S32" s="16"/>
+      <c r="T32" s="16"/>
+      <c r="U32" s="16"/>
     </row>
     <row r="33" spans="1:21">
-      <c r="A33" s="21"/>
-      <c r="B33" s="21"/>
-      <c r="C33" s="21"/>
-      <c r="D33" s="21"/>
-      <c r="E33" s="21"/>
-      <c r="F33" s="21"/>
-      <c r="G33" s="21"/>
-      <c r="H33" s="25"/>
-      <c r="I33" s="21"/>
-      <c r="J33" s="21"/>
-      <c r="K33" s="21"/>
-      <c r="L33" s="21"/>
-      <c r="M33" s="21"/>
-      <c r="N33" s="21"/>
-      <c r="O33" s="21"/>
-      <c r="P33" s="21"/>
-      <c r="Q33" s="21"/>
-      <c r="R33" s="21"/>
-      <c r="S33" s="21"/>
-      <c r="T33" s="21"/>
-      <c r="U33" s="21"/>
+      <c r="A33" s="16"/>
+      <c r="B33" s="16"/>
+      <c r="C33" s="16"/>
+      <c r="D33" s="16"/>
+      <c r="E33" s="16"/>
+      <c r="F33" s="16"/>
+      <c r="G33" s="16"/>
+      <c r="H33" s="20"/>
+      <c r="I33" s="16"/>
+      <c r="J33" s="16"/>
+      <c r="K33" s="16"/>
+      <c r="L33" s="16"/>
+      <c r="M33" s="16"/>
+      <c r="N33" s="16"/>
+      <c r="O33" s="16"/>
+      <c r="P33" s="16"/>
+      <c r="Q33" s="16"/>
+      <c r="R33" s="16"/>
+      <c r="S33" s="16"/>
+      <c r="T33" s="16"/>
+      <c r="U33" s="16"/>
     </row>
     <row r="34" spans="1:21">
-      <c r="A34" s="21"/>
-      <c r="B34" s="21"/>
-      <c r="C34" s="21"/>
-      <c r="D34" s="21"/>
-      <c r="E34" s="21"/>
-      <c r="F34" s="21"/>
-      <c r="G34" s="21"/>
-      <c r="H34" s="25"/>
-      <c r="I34" s="21"/>
-      <c r="J34" s="21"/>
-      <c r="K34" s="21"/>
-      <c r="L34" s="21"/>
-      <c r="M34" s="21"/>
-      <c r="N34" s="21"/>
-      <c r="O34" s="21"/>
-      <c r="P34" s="21"/>
-      <c r="Q34" s="21"/>
-      <c r="R34" s="21"/>
-      <c r="S34" s="21"/>
-      <c r="T34" s="21"/>
-      <c r="U34" s="21"/>
+      <c r="A34" s="16"/>
+      <c r="B34" s="16"/>
+      <c r="C34" s="16"/>
+      <c r="D34" s="16"/>
+      <c r="E34" s="16"/>
+      <c r="F34" s="16"/>
+      <c r="G34" s="16"/>
+      <c r="H34" s="20"/>
+      <c r="I34" s="16"/>
+      <c r="J34" s="16"/>
+      <c r="K34" s="16"/>
+      <c r="L34" s="16"/>
+      <c r="M34" s="16"/>
+      <c r="N34" s="16"/>
+      <c r="O34" s="16"/>
+      <c r="P34" s="16"/>
+      <c r="Q34" s="16"/>
+      <c r="R34" s="16"/>
+      <c r="S34" s="16"/>
+      <c r="T34" s="16"/>
+      <c r="U34" s="16"/>
     </row>
     <row r="35" spans="1:21">
-      <c r="A35" s="21"/>
-      <c r="B35" s="21"/>
-      <c r="C35" s="21"/>
-      <c r="D35" s="21"/>
-      <c r="E35" s="21"/>
-      <c r="F35" s="21"/>
-      <c r="G35" s="21"/>
-      <c r="H35" s="25"/>
-      <c r="I35" s="21"/>
-      <c r="J35" s="21"/>
-      <c r="K35" s="21"/>
-      <c r="L35" s="21"/>
-      <c r="M35" s="21"/>
-      <c r="N35" s="21"/>
-      <c r="O35" s="21"/>
-      <c r="P35" s="21"/>
-      <c r="Q35" s="21"/>
-      <c r="R35" s="21"/>
-      <c r="S35" s="21"/>
-      <c r="T35" s="21"/>
-      <c r="U35" s="21"/>
+      <c r="A35" s="16"/>
+      <c r="B35" s="16"/>
+      <c r="C35" s="16"/>
+      <c r="D35" s="16"/>
+      <c r="E35" s="16"/>
+      <c r="F35" s="16"/>
+      <c r="G35" s="16"/>
+      <c r="H35" s="20"/>
+      <c r="I35" s="16"/>
+      <c r="J35" s="16"/>
+      <c r="K35" s="16"/>
+      <c r="L35" s="16"/>
+      <c r="M35" s="16"/>
+      <c r="N35" s="16"/>
+      <c r="O35" s="16"/>
+      <c r="P35" s="16"/>
+      <c r="Q35" s="16"/>
+      <c r="R35" s="16"/>
+      <c r="S35" s="16"/>
+      <c r="T35" s="16"/>
+      <c r="U35" s="16"/>
     </row>
     <row r="36" spans="1:21">
-      <c r="A36" s="21"/>
-      <c r="B36" s="21"/>
-      <c r="C36" s="21"/>
-      <c r="D36" s="21"/>
-      <c r="E36" s="21"/>
-      <c r="F36" s="21"/>
-      <c r="G36" s="21"/>
-      <c r="H36" s="25"/>
-      <c r="I36" s="21"/>
-      <c r="J36" s="21"/>
-      <c r="K36" s="21"/>
-      <c r="L36" s="21"/>
-      <c r="M36" s="21"/>
-      <c r="N36" s="21"/>
-      <c r="O36" s="21"/>
-      <c r="P36" s="21"/>
-      <c r="Q36" s="21"/>
-      <c r="R36" s="21"/>
-      <c r="S36" s="21"/>
-      <c r="T36" s="21"/>
-      <c r="U36" s="21"/>
+      <c r="A36" s="16"/>
+      <c r="B36" s="16"/>
+      <c r="C36" s="16"/>
+      <c r="D36" s="16"/>
+      <c r="E36" s="16"/>
+      <c r="F36" s="16"/>
+      <c r="G36" s="16"/>
+      <c r="H36" s="20"/>
+      <c r="I36" s="16"/>
+      <c r="J36" s="16"/>
+      <c r="K36" s="16"/>
+      <c r="L36" s="16"/>
+      <c r="M36" s="16"/>
+      <c r="N36" s="16"/>
+      <c r="O36" s="16"/>
+      <c r="P36" s="16"/>
+      <c r="Q36" s="16"/>
+      <c r="R36" s="16"/>
+      <c r="S36" s="16"/>
+      <c r="T36" s="16"/>
+      <c r="U36" s="16"/>
     </row>
     <row r="37" spans="1:21">
-      <c r="A37" s="21"/>
-      <c r="B37" s="21"/>
-      <c r="C37" s="21"/>
-      <c r="D37" s="21"/>
-      <c r="E37" s="21"/>
-      <c r="F37" s="21"/>
-      <c r="G37" s="21"/>
-      <c r="H37" s="25"/>
-      <c r="I37" s="21"/>
-      <c r="J37" s="21"/>
-      <c r="K37" s="21"/>
-      <c r="L37" s="21"/>
-      <c r="M37" s="21"/>
-      <c r="N37" s="21"/>
-      <c r="O37" s="21"/>
-      <c r="P37" s="21"/>
-      <c r="Q37" s="21"/>
-      <c r="R37" s="21"/>
-      <c r="S37" s="21"/>
-      <c r="T37" s="21"/>
-      <c r="U37" s="21"/>
+      <c r="A37" s="16"/>
+      <c r="B37" s="16"/>
+      <c r="C37" s="16"/>
+      <c r="D37" s="16"/>
+      <c r="E37" s="16"/>
+      <c r="F37" s="16"/>
+      <c r="G37" s="16"/>
+      <c r="H37" s="20"/>
+      <c r="I37" s="16"/>
+      <c r="J37" s="16"/>
+      <c r="K37" s="16"/>
+      <c r="L37" s="16"/>
+      <c r="M37" s="16"/>
+      <c r="N37" s="16"/>
+      <c r="O37" s="16"/>
+      <c r="P37" s="16"/>
+      <c r="Q37" s="16"/>
+      <c r="R37" s="16"/>
+      <c r="S37" s="16"/>
+      <c r="T37" s="16"/>
+      <c r="U37" s="16"/>
     </row>
     <row r="38" spans="1:21">
-      <c r="A38" s="21"/>
-      <c r="B38" s="21"/>
-      <c r="C38" s="21"/>
-      <c r="D38" s="21"/>
-      <c r="E38" s="21"/>
-      <c r="F38" s="21"/>
-      <c r="G38" s="21"/>
-      <c r="H38" s="25"/>
-      <c r="I38" s="21"/>
-      <c r="J38" s="21"/>
-      <c r="K38" s="21"/>
-      <c r="L38" s="21"/>
-      <c r="M38" s="21"/>
-      <c r="N38" s="21"/>
-      <c r="O38" s="21"/>
-      <c r="P38" s="21"/>
-      <c r="Q38" s="21"/>
-      <c r="R38" s="21"/>
-      <c r="S38" s="21"/>
-      <c r="T38" s="21"/>
-      <c r="U38" s="21"/>
+      <c r="A38" s="16"/>
+      <c r="B38" s="16"/>
+      <c r="C38" s="16"/>
+      <c r="D38" s="16"/>
+      <c r="E38" s="16"/>
+      <c r="F38" s="16"/>
+      <c r="G38" s="16"/>
+      <c r="H38" s="20"/>
+      <c r="I38" s="16"/>
+      <c r="J38" s="16"/>
+      <c r="K38" s="16"/>
+      <c r="L38" s="16"/>
+      <c r="M38" s="16"/>
+      <c r="N38" s="16"/>
+      <c r="O38" s="16"/>
+      <c r="P38" s="16"/>
+      <c r="Q38" s="16"/>
+      <c r="R38" s="16"/>
+      <c r="S38" s="16"/>
+      <c r="T38" s="16"/>
+      <c r="U38" s="16"/>
     </row>
     <row r="39" spans="1:21">
-      <c r="A39" s="21"/>
-      <c r="B39" s="21"/>
-      <c r="C39" s="21"/>
-      <c r="D39" s="21"/>
-      <c r="E39" s="21"/>
-      <c r="F39" s="21"/>
-      <c r="G39" s="21"/>
-      <c r="H39" s="25"/>
-      <c r="I39" s="21"/>
-      <c r="J39" s="21"/>
-      <c r="K39" s="21"/>
-      <c r="L39" s="21"/>
-      <c r="M39" s="21"/>
-      <c r="N39" s="21"/>
-      <c r="O39" s="21"/>
-      <c r="P39" s="21"/>
-      <c r="Q39" s="21"/>
-      <c r="R39" s="21"/>
-      <c r="S39" s="21"/>
-      <c r="T39" s="21"/>
-      <c r="U39" s="21"/>
+      <c r="A39" s="16"/>
+      <c r="B39" s="16"/>
+      <c r="C39" s="16"/>
+      <c r="D39" s="16"/>
+      <c r="E39" s="16"/>
+      <c r="F39" s="16"/>
+      <c r="G39" s="16"/>
+      <c r="H39" s="20"/>
+      <c r="I39" s="16"/>
+      <c r="J39" s="16"/>
+      <c r="K39" s="16"/>
+      <c r="L39" s="16"/>
+      <c r="M39" s="16"/>
+      <c r="N39" s="16"/>
+      <c r="O39" s="16"/>
+      <c r="P39" s="16"/>
+      <c r="Q39" s="16"/>
+      <c r="R39" s="16"/>
+      <c r="S39" s="16"/>
+      <c r="T39" s="16"/>
+      <c r="U39" s="16"/>
     </row>
     <row r="40" spans="1:21">
-      <c r="A40" s="21"/>
-      <c r="B40" s="21"/>
-      <c r="C40" s="21"/>
-      <c r="D40" s="21"/>
-      <c r="E40" s="21"/>
-      <c r="F40" s="21"/>
-      <c r="G40" s="21"/>
-      <c r="H40" s="25"/>
-      <c r="I40" s="21"/>
-      <c r="J40" s="21"/>
-      <c r="K40" s="21"/>
-      <c r="L40" s="21"/>
-      <c r="M40" s="21"/>
-      <c r="N40" s="21"/>
-      <c r="O40" s="21"/>
-      <c r="P40" s="21"/>
-      <c r="Q40" s="21"/>
-      <c r="R40" s="21"/>
-      <c r="S40" s="21"/>
-      <c r="T40" s="21"/>
-      <c r="U40" s="21"/>
+      <c r="A40" s="16"/>
+      <c r="B40" s="16"/>
+      <c r="C40" s="16"/>
+      <c r="D40" s="16"/>
+      <c r="E40" s="16"/>
+      <c r="F40" s="16"/>
+      <c r="G40" s="16"/>
+      <c r="H40" s="20"/>
+      <c r="I40" s="16"/>
+      <c r="J40" s="16"/>
+      <c r="K40" s="16"/>
+      <c r="L40" s="16"/>
+      <c r="M40" s="16"/>
+      <c r="N40" s="16"/>
+      <c r="O40" s="16"/>
+      <c r="P40" s="16"/>
+      <c r="Q40" s="16"/>
+      <c r="R40" s="16"/>
+      <c r="S40" s="16"/>
+      <c r="T40" s="16"/>
+      <c r="U40" s="16"/>
     </row>
     <row r="41" spans="1:21">
-      <c r="A41" s="21"/>
-      <c r="B41" s="21"/>
-      <c r="C41" s="21"/>
-      <c r="D41" s="21"/>
-      <c r="E41" s="21"/>
-      <c r="F41" s="21"/>
-      <c r="G41" s="21"/>
-      <c r="H41" s="25"/>
-      <c r="I41" s="21"/>
-      <c r="J41" s="21"/>
-      <c r="K41" s="21"/>
-      <c r="L41" s="21"/>
-      <c r="M41" s="21"/>
-      <c r="N41" s="21"/>
-      <c r="O41" s="21"/>
-      <c r="P41" s="21"/>
-      <c r="Q41" s="21"/>
-      <c r="R41" s="21"/>
-      <c r="S41" s="21"/>
-      <c r="T41" s="21"/>
-      <c r="U41" s="21"/>
+      <c r="A41" s="16"/>
+      <c r="B41" s="16"/>
+      <c r="C41" s="16"/>
+      <c r="D41" s="16"/>
+      <c r="E41" s="16"/>
+      <c r="F41" s="16"/>
+      <c r="G41" s="16"/>
+      <c r="H41" s="20"/>
+      <c r="I41" s="16"/>
+      <c r="J41" s="16"/>
+      <c r="K41" s="16"/>
+      <c r="L41" s="16"/>
+      <c r="M41" s="16"/>
+      <c r="N41" s="16"/>
+      <c r="O41" s="16"/>
+      <c r="P41" s="16"/>
+      <c r="Q41" s="16"/>
+      <c r="R41" s="16"/>
+      <c r="S41" s="16"/>
+      <c r="T41" s="16"/>
+      <c r="U41" s="16"/>
     </row>
     <row r="42" spans="1:21">
-      <c r="A42" s="21"/>
-      <c r="B42" s="21"/>
-      <c r="C42" s="21"/>
-      <c r="D42" s="21"/>
-      <c r="E42" s="21"/>
-      <c r="F42" s="21"/>
-      <c r="G42" s="21"/>
-      <c r="H42" s="25"/>
-      <c r="I42" s="21"/>
-      <c r="J42" s="21"/>
-      <c r="K42" s="21"/>
-      <c r="L42" s="21"/>
-      <c r="M42" s="21"/>
-      <c r="N42" s="21"/>
-      <c r="O42" s="21"/>
-      <c r="P42" s="21"/>
-      <c r="Q42" s="21"/>
-      <c r="R42" s="21"/>
-      <c r="S42" s="21"/>
-      <c r="T42" s="21"/>
-      <c r="U42" s="21"/>
+      <c r="A42" s="16"/>
+      <c r="B42" s="16"/>
+      <c r="C42" s="16"/>
+      <c r="D42" s="16"/>
+      <c r="E42" s="16"/>
+      <c r="F42" s="16"/>
+      <c r="G42" s="16"/>
+      <c r="H42" s="20"/>
+      <c r="I42" s="16"/>
+      <c r="J42" s="16"/>
+      <c r="K42" s="16"/>
+      <c r="L42" s="16"/>
+      <c r="M42" s="16"/>
+      <c r="N42" s="16"/>
+      <c r="O42" s="16"/>
+      <c r="P42" s="16"/>
+      <c r="Q42" s="16"/>
+      <c r="R42" s="16"/>
+      <c r="S42" s="16"/>
+      <c r="T42" s="16"/>
+      <c r="U42" s="16"/>
     </row>
     <row r="43" spans="1:21">
-      <c r="A43" s="21"/>
-      <c r="B43" s="21"/>
-      <c r="C43" s="21"/>
-      <c r="D43" s="21"/>
-      <c r="E43" s="21"/>
-      <c r="F43" s="21"/>
-      <c r="G43" s="21"/>
-      <c r="H43" s="25"/>
-      <c r="I43" s="21"/>
-      <c r="J43" s="21"/>
-      <c r="K43" s="21"/>
-      <c r="L43" s="21"/>
-      <c r="M43" s="21"/>
-      <c r="N43" s="21"/>
-      <c r="O43" s="21"/>
-      <c r="P43" s="21"/>
-      <c r="Q43" s="21"/>
-      <c r="R43" s="21"/>
-      <c r="S43" s="21"/>
-      <c r="T43" s="21"/>
-      <c r="U43" s="21"/>
+      <c r="A43" s="16"/>
+      <c r="B43" s="16"/>
+      <c r="C43" s="16"/>
+      <c r="D43" s="16"/>
+      <c r="E43" s="16"/>
+      <c r="F43" s="16"/>
+      <c r="G43" s="16"/>
+      <c r="H43" s="20"/>
+      <c r="I43" s="16"/>
+      <c r="J43" s="16"/>
+      <c r="K43" s="16"/>
+      <c r="L43" s="16"/>
+      <c r="M43" s="16"/>
+      <c r="N43" s="16"/>
+      <c r="O43" s="16"/>
+      <c r="P43" s="16"/>
+      <c r="Q43" s="16"/>
+      <c r="R43" s="16"/>
+      <c r="S43" s="16"/>
+      <c r="T43" s="16"/>
+      <c r="U43" s="16"/>
     </row>
     <row r="44" spans="1:21">
-      <c r="A44" s="21"/>
-      <c r="B44" s="21"/>
-      <c r="C44" s="21"/>
-      <c r="D44" s="21"/>
-      <c r="E44" s="21"/>
-      <c r="F44" s="21"/>
-      <c r="G44" s="21"/>
-      <c r="H44" s="25"/>
-      <c r="I44" s="21"/>
-      <c r="J44" s="21"/>
-      <c r="K44" s="21"/>
-      <c r="L44" s="21"/>
-      <c r="M44" s="21"/>
-      <c r="N44" s="21"/>
-      <c r="O44" s="21"/>
-      <c r="P44" s="21"/>
-      <c r="Q44" s="21"/>
-      <c r="R44" s="21"/>
-      <c r="S44" s="21"/>
-      <c r="T44" s="21"/>
-      <c r="U44" s="21"/>
+      <c r="A44" s="16"/>
+      <c r="B44" s="16"/>
+      <c r="C44" s="16"/>
+      <c r="D44" s="16"/>
+      <c r="E44" s="16"/>
+      <c r="F44" s="16"/>
+      <c r="G44" s="16"/>
+      <c r="H44" s="20"/>
+      <c r="I44" s="16"/>
+      <c r="J44" s="16"/>
+      <c r="K44" s="16"/>
+      <c r="L44" s="16"/>
+      <c r="M44" s="16"/>
+      <c r="N44" s="16"/>
+      <c r="O44" s="16"/>
+      <c r="P44" s="16"/>
+      <c r="Q44" s="16"/>
+      <c r="R44" s="16"/>
+      <c r="S44" s="16"/>
+      <c r="T44" s="16"/>
+      <c r="U44" s="16"/>
     </row>
     <row r="45" spans="1:21">
-      <c r="A45" s="21"/>
-      <c r="B45" s="21"/>
-      <c r="C45" s="21"/>
-      <c r="D45" s="21"/>
-      <c r="E45" s="21"/>
-      <c r="F45" s="21"/>
-      <c r="G45" s="21"/>
-      <c r="H45" s="25"/>
-      <c r="I45" s="21"/>
-      <c r="J45" s="21"/>
-      <c r="K45" s="21"/>
-      <c r="L45" s="21"/>
-      <c r="M45" s="21"/>
-      <c r="N45" s="21"/>
-      <c r="O45" s="21"/>
-      <c r="P45" s="21"/>
-      <c r="Q45" s="21"/>
-      <c r="R45" s="21"/>
-      <c r="S45" s="21"/>
-      <c r="T45" s="21"/>
-      <c r="U45" s="21"/>
+      <c r="A45" s="16"/>
+      <c r="B45" s="16"/>
+      <c r="C45" s="16"/>
+      <c r="D45" s="16"/>
+      <c r="E45" s="16"/>
+      <c r="F45" s="16"/>
+      <c r="G45" s="16"/>
+      <c r="H45" s="20"/>
+      <c r="I45" s="16"/>
+      <c r="J45" s="16"/>
+      <c r="K45" s="16"/>
+      <c r="L45" s="16"/>
+      <c r="M45" s="16"/>
+      <c r="N45" s="16"/>
+      <c r="O45" s="16"/>
+      <c r="P45" s="16"/>
+      <c r="Q45" s="16"/>
+      <c r="R45" s="16"/>
+      <c r="S45" s="16"/>
+      <c r="T45" s="16"/>
+      <c r="U45" s="16"/>
     </row>
     <row r="46" spans="1:21">
-      <c r="A46" s="21"/>
-      <c r="B46" s="21"/>
-      <c r="C46" s="21"/>
-      <c r="D46" s="21"/>
-      <c r="E46" s="21"/>
-      <c r="F46" s="21"/>
-      <c r="G46" s="21"/>
-      <c r="H46" s="25"/>
-      <c r="I46" s="21"/>
-      <c r="J46" s="21"/>
-      <c r="K46" s="21"/>
-      <c r="L46" s="21"/>
-      <c r="M46" s="21"/>
-      <c r="N46" s="21"/>
-      <c r="O46" s="21"/>
-      <c r="P46" s="21"/>
-      <c r="Q46" s="21"/>
-      <c r="R46" s="21"/>
-      <c r="S46" s="21"/>
-      <c r="T46" s="21"/>
-      <c r="U46" s="21"/>
+      <c r="A46" s="16"/>
+      <c r="B46" s="16"/>
+      <c r="C46" s="16"/>
+      <c r="D46" s="16"/>
+      <c r="E46" s="16"/>
+      <c r="F46" s="16"/>
+      <c r="G46" s="16"/>
+      <c r="H46" s="20"/>
+      <c r="I46" s="16"/>
+      <c r="J46" s="16"/>
+      <c r="K46" s="16"/>
+      <c r="L46" s="16"/>
+      <c r="M46" s="16"/>
+      <c r="N46" s="16"/>
+      <c r="O46" s="16"/>
+      <c r="P46" s="16"/>
+      <c r="Q46" s="16"/>
+      <c r="R46" s="16"/>
+      <c r="S46" s="16"/>
+      <c r="T46" s="16"/>
+      <c r="U46" s="16"/>
     </row>
     <row r="47" spans="1:21">
-      <c r="A47" s="21"/>
-      <c r="B47" s="21"/>
-      <c r="C47" s="21"/>
-      <c r="D47" s="21"/>
-      <c r="E47" s="21"/>
-      <c r="F47" s="21"/>
-      <c r="G47" s="21"/>
-      <c r="H47" s="25"/>
-      <c r="I47" s="21"/>
-      <c r="J47" s="21"/>
-      <c r="K47" s="21"/>
-      <c r="L47" s="21"/>
-      <c r="M47" s="21"/>
-      <c r="N47" s="21"/>
-      <c r="O47" s="21"/>
-      <c r="P47" s="21"/>
-      <c r="Q47" s="21"/>
-      <c r="R47" s="21"/>
-      <c r="S47" s="21"/>
-      <c r="T47" s="21"/>
-      <c r="U47" s="21"/>
+      <c r="A47" s="16"/>
+      <c r="B47" s="16"/>
+      <c r="C47" s="16"/>
+      <c r="D47" s="16"/>
+      <c r="E47" s="16"/>
+      <c r="F47" s="16"/>
+      <c r="G47" s="16"/>
+      <c r="H47" s="20"/>
+      <c r="I47" s="16"/>
+      <c r="J47" s="16"/>
+      <c r="K47" s="16"/>
+      <c r="L47" s="16"/>
+      <c r="M47" s="16"/>
+      <c r="N47" s="16"/>
+      <c r="O47" s="16"/>
+      <c r="P47" s="16"/>
+      <c r="Q47" s="16"/>
+      <c r="R47" s="16"/>
+      <c r="S47" s="16"/>
+      <c r="T47" s="16"/>
+      <c r="U47" s="16"/>
     </row>
     <row r="48" spans="1:21">
-      <c r="A48" s="21"/>
-      <c r="B48" s="21"/>
-      <c r="C48" s="21"/>
-      <c r="D48" s="21"/>
-      <c r="E48" s="21"/>
-      <c r="F48" s="21"/>
-      <c r="G48" s="21"/>
-      <c r="H48" s="25"/>
-      <c r="I48" s="21"/>
-      <c r="J48" s="21"/>
-      <c r="K48" s="21"/>
-      <c r="L48" s="21"/>
-      <c r="M48" s="21"/>
-      <c r="N48" s="21"/>
-      <c r="O48" s="21"/>
-      <c r="P48" s="21"/>
-      <c r="Q48" s="21"/>
-      <c r="R48" s="21"/>
-      <c r="S48" s="21"/>
-      <c r="T48" s="21"/>
-      <c r="U48" s="21"/>
+      <c r="A48" s="16"/>
+      <c r="B48" s="16"/>
+      <c r="C48" s="16"/>
+      <c r="D48" s="16"/>
+      <c r="E48" s="16"/>
+      <c r="F48" s="16"/>
+      <c r="G48" s="16"/>
+      <c r="H48" s="20"/>
+      <c r="I48" s="16"/>
+      <c r="J48" s="16"/>
+      <c r="K48" s="16"/>
+      <c r="L48" s="16"/>
+      <c r="M48" s="16"/>
+      <c r="N48" s="16"/>
+      <c r="O48" s="16"/>
+      <c r="P48" s="16"/>
+      <c r="Q48" s="16"/>
+      <c r="R48" s="16"/>
+      <c r="S48" s="16"/>
+      <c r="T48" s="16"/>
+      <c r="U48" s="16"/>
     </row>
     <row r="49" spans="1:21">
-      <c r="A49" s="21"/>
-      <c r="B49" s="21"/>
-      <c r="C49" s="21"/>
-      <c r="D49" s="21"/>
-      <c r="E49" s="21"/>
-      <c r="F49" s="21"/>
-      <c r="G49" s="21"/>
-      <c r="H49" s="25"/>
-      <c r="I49" s="21"/>
-      <c r="J49" s="21"/>
-      <c r="K49" s="21"/>
-      <c r="L49" s="21"/>
-      <c r="M49" s="21"/>
-      <c r="N49" s="21"/>
-      <c r="O49" s="21"/>
-      <c r="P49" s="21"/>
-      <c r="Q49" s="21"/>
-      <c r="R49" s="21"/>
-      <c r="S49" s="21"/>
-      <c r="T49" s="21"/>
-      <c r="U49" s="21"/>
+      <c r="A49" s="16"/>
+      <c r="B49" s="16"/>
+      <c r="C49" s="16"/>
+      <c r="D49" s="16"/>
+      <c r="E49" s="16"/>
+      <c r="F49" s="16"/>
+      <c r="G49" s="16"/>
+      <c r="H49" s="20"/>
+      <c r="I49" s="16"/>
+      <c r="J49" s="16"/>
+      <c r="K49" s="16"/>
+      <c r="L49" s="16"/>
+      <c r="M49" s="16"/>
+      <c r="N49" s="16"/>
+      <c r="O49" s="16"/>
+      <c r="P49" s="16"/>
+      <c r="Q49" s="16"/>
+      <c r="R49" s="16"/>
+      <c r="S49" s="16"/>
+      <c r="T49" s="16"/>
+      <c r="U49" s="16"/>
     </row>
     <row r="50" spans="1:21">
-      <c r="A50" s="21"/>
-      <c r="B50" s="21"/>
-      <c r="C50" s="21"/>
-      <c r="D50" s="21"/>
-      <c r="E50" s="21"/>
-      <c r="F50" s="21"/>
-      <c r="G50" s="21"/>
-      <c r="H50" s="25"/>
-      <c r="I50" s="21"/>
-      <c r="J50" s="21"/>
-      <c r="K50" s="21"/>
-      <c r="L50" s="21"/>
-      <c r="M50" s="21"/>
-      <c r="N50" s="21"/>
-      <c r="O50" s="21"/>
-      <c r="P50" s="21"/>
-      <c r="Q50" s="21"/>
-      <c r="R50" s="21"/>
-      <c r="S50" s="21"/>
-      <c r="T50" s="21"/>
-      <c r="U50" s="21"/>
+      <c r="A50" s="16"/>
+      <c r="B50" s="16"/>
+      <c r="C50" s="16"/>
+      <c r="D50" s="16"/>
+      <c r="E50" s="16"/>
+      <c r="F50" s="16"/>
+      <c r="G50" s="16"/>
+      <c r="H50" s="20"/>
+      <c r="I50" s="16"/>
+      <c r="J50" s="16"/>
+      <c r="K50" s="16"/>
+      <c r="L50" s="16"/>
+      <c r="M50" s="16"/>
+      <c r="N50" s="16"/>
+      <c r="O50" s="16"/>
+      <c r="P50" s="16"/>
+      <c r="Q50" s="16"/>
+      <c r="R50" s="16"/>
+      <c r="S50" s="16"/>
+      <c r="T50" s="16"/>
+      <c r="U50" s="16"/>
     </row>
     <row r="51" spans="1:21">
-      <c r="A51" s="21"/>
-      <c r="B51" s="21"/>
-      <c r="C51" s="21"/>
-      <c r="D51" s="21"/>
-      <c r="E51" s="21"/>
-      <c r="F51" s="21"/>
-      <c r="G51" s="21"/>
-      <c r="H51" s="25"/>
-      <c r="I51" s="21"/>
-      <c r="J51" s="21"/>
-      <c r="K51" s="21"/>
-      <c r="L51" s="21"/>
-      <c r="M51" s="21"/>
-      <c r="N51" s="21"/>
-      <c r="O51" s="21"/>
-      <c r="P51" s="21"/>
-      <c r="Q51" s="21"/>
-      <c r="R51" s="21"/>
-      <c r="S51" s="21"/>
-      <c r="T51" s="21"/>
-      <c r="U51" s="21"/>
+      <c r="A51" s="16"/>
+      <c r="B51" s="16"/>
+      <c r="C51" s="16"/>
+      <c r="D51" s="16"/>
+      <c r="E51" s="16"/>
+      <c r="F51" s="16"/>
+      <c r="G51" s="16"/>
+      <c r="H51" s="20"/>
+      <c r="I51" s="16"/>
+      <c r="J51" s="16"/>
+      <c r="K51" s="16"/>
+      <c r="L51" s="16"/>
+      <c r="M51" s="16"/>
+      <c r="N51" s="16"/>
+      <c r="O51" s="16"/>
+      <c r="P51" s="16"/>
+      <c r="Q51" s="16"/>
+      <c r="R51" s="16"/>
+      <c r="S51" s="16"/>
+      <c r="T51" s="16"/>
+      <c r="U51" s="16"/>
     </row>
     <row r="52" spans="1:21">
-      <c r="A52" s="21"/>
-      <c r="B52" s="21"/>
-      <c r="C52" s="21"/>
-      <c r="D52" s="21"/>
-      <c r="E52" s="21"/>
-      <c r="F52" s="21"/>
-      <c r="G52" s="21"/>
-      <c r="H52" s="25"/>
-      <c r="I52" s="21"/>
-      <c r="J52" s="21"/>
-      <c r="K52" s="21"/>
-      <c r="L52" s="21"/>
-      <c r="M52" s="21"/>
-      <c r="N52" s="21"/>
-      <c r="O52" s="21"/>
-      <c r="P52" s="21"/>
-      <c r="Q52" s="21"/>
-      <c r="R52" s="21"/>
-      <c r="S52" s="21"/>
-      <c r="T52" s="21"/>
-      <c r="U52" s="21"/>
+      <c r="A52" s="16"/>
+      <c r="B52" s="16"/>
+      <c r="C52" s="16"/>
+      <c r="D52" s="16"/>
+      <c r="E52" s="16"/>
+      <c r="F52" s="16"/>
+      <c r="G52" s="16"/>
+      <c r="H52" s="20"/>
+      <c r="I52" s="16"/>
+      <c r="J52" s="16"/>
+      <c r="K52" s="16"/>
+      <c r="L52" s="16"/>
+      <c r="M52" s="16"/>
+      <c r="N52" s="16"/>
+      <c r="O52" s="16"/>
+      <c r="P52" s="16"/>
+      <c r="Q52" s="16"/>
+      <c r="R52" s="16"/>
+      <c r="S52" s="16"/>
+      <c r="T52" s="16"/>
+      <c r="U52" s="16"/>
     </row>
     <row r="53" spans="1:21">
-      <c r="A53" s="21"/>
-      <c r="B53" s="21"/>
-      <c r="C53" s="21"/>
-      <c r="D53" s="21"/>
-      <c r="E53" s="21"/>
-      <c r="F53" s="21"/>
-      <c r="G53" s="21"/>
-      <c r="H53" s="25"/>
-      <c r="I53" s="21"/>
-      <c r="J53" s="21"/>
-      <c r="K53" s="21"/>
-      <c r="L53" s="21"/>
-      <c r="M53" s="21"/>
-      <c r="N53" s="21"/>
-      <c r="O53" s="21"/>
-      <c r="P53" s="21"/>
-      <c r="Q53" s="21"/>
-      <c r="R53" s="21"/>
-      <c r="S53" s="21"/>
-      <c r="T53" s="21"/>
-      <c r="U53" s="21"/>
+      <c r="A53" s="16"/>
+      <c r="B53" s="16"/>
+      <c r="C53" s="16"/>
+      <c r="D53" s="16"/>
+      <c r="E53" s="16"/>
+      <c r="F53" s="16"/>
+      <c r="G53" s="16"/>
+      <c r="H53" s="20"/>
+      <c r="I53" s="16"/>
+      <c r="J53" s="16"/>
+      <c r="K53" s="16"/>
+      <c r="L53" s="16"/>
+      <c r="M53" s="16"/>
+      <c r="N53" s="16"/>
+      <c r="O53" s="16"/>
+      <c r="P53" s="16"/>
+      <c r="Q53" s="16"/>
+      <c r="R53" s="16"/>
+      <c r="S53" s="16"/>
+      <c r="T53" s="16"/>
+      <c r="U53" s="16"/>
     </row>
     <row r="54" spans="1:21">
-      <c r="A54" s="21"/>
-      <c r="B54" s="21"/>
-      <c r="C54" s="21"/>
-      <c r="D54" s="21"/>
-      <c r="E54" s="21"/>
-      <c r="F54" s="21"/>
-      <c r="G54" s="21"/>
-      <c r="H54" s="25"/>
-      <c r="I54" s="21"/>
-      <c r="J54" s="21"/>
-      <c r="K54" s="21"/>
-      <c r="L54" s="21"/>
-      <c r="M54" s="21"/>
-      <c r="N54" s="21"/>
-      <c r="O54" s="21"/>
-      <c r="P54" s="21"/>
-      <c r="Q54" s="21"/>
-      <c r="R54" s="21"/>
-      <c r="S54" s="21"/>
-      <c r="T54" s="21"/>
-      <c r="U54" s="21"/>
+      <c r="A54" s="16"/>
+      <c r="B54" s="16"/>
+      <c r="C54" s="16"/>
+      <c r="D54" s="16"/>
+      <c r="E54" s="16"/>
+      <c r="F54" s="16"/>
+      <c r="G54" s="16"/>
+      <c r="H54" s="20"/>
+      <c r="I54" s="16"/>
+      <c r="J54" s="16"/>
+      <c r="K54" s="16"/>
+      <c r="L54" s="16"/>
+      <c r="M54" s="16"/>
+      <c r="N54" s="16"/>
+      <c r="O54" s="16"/>
+      <c r="P54" s="16"/>
+      <c r="Q54" s="16"/>
+      <c r="R54" s="16"/>
+      <c r="S54" s="16"/>
+      <c r="T54" s="16"/>
+      <c r="U54" s="16"/>
     </row>
     <row r="55" spans="1:21">
-      <c r="A55" s="21"/>
-      <c r="B55" s="21"/>
-      <c r="C55" s="21"/>
-      <c r="D55" s="21"/>
-      <c r="E55" s="21"/>
-      <c r="F55" s="21"/>
-      <c r="G55" s="21"/>
-      <c r="H55" s="25"/>
-      <c r="I55" s="21"/>
-      <c r="J55" s="21"/>
-      <c r="K55" s="21"/>
-      <c r="L55" s="21"/>
-      <c r="M55" s="21"/>
-      <c r="N55" s="21"/>
-      <c r="O55" s="21"/>
-      <c r="P55" s="21"/>
-      <c r="Q55" s="21"/>
-      <c r="R55" s="21"/>
-      <c r="S55" s="21"/>
-      <c r="T55" s="21"/>
-      <c r="U55" s="21"/>
+      <c r="A55" s="16"/>
+      <c r="B55" s="16"/>
+      <c r="C55" s="16"/>
+      <c r="D55" s="16"/>
+      <c r="E55" s="16"/>
+      <c r="F55" s="16"/>
+      <c r="G55" s="16"/>
+      <c r="H55" s="20"/>
+      <c r="I55" s="16"/>
+      <c r="J55" s="16"/>
+      <c r="K55" s="16"/>
+      <c r="L55" s="16"/>
+      <c r="M55" s="16"/>
+      <c r="N55" s="16"/>
+      <c r="O55" s="16"/>
+      <c r="P55" s="16"/>
+      <c r="Q55" s="16"/>
+      <c r="R55" s="16"/>
+      <c r="S55" s="16"/>
+      <c r="T55" s="16"/>
+      <c r="U55" s="16"/>
     </row>
     <row r="56" spans="1:21">
-      <c r="A56" s="21"/>
-      <c r="B56" s="21"/>
-      <c r="C56" s="21"/>
-      <c r="D56" s="21"/>
-      <c r="E56" s="21"/>
-      <c r="F56" s="21"/>
-      <c r="G56" s="21"/>
-      <c r="H56" s="25"/>
-      <c r="I56" s="21"/>
-      <c r="J56" s="21"/>
-      <c r="K56" s="21"/>
-      <c r="L56" s="21"/>
-      <c r="M56" s="21"/>
-      <c r="N56" s="21"/>
-      <c r="O56" s="21"/>
-      <c r="P56" s="21"/>
-      <c r="Q56" s="21"/>
-      <c r="R56" s="21"/>
-      <c r="S56" s="21"/>
-      <c r="T56" s="21"/>
-      <c r="U56" s="21"/>
+      <c r="A56" s="16"/>
+      <c r="B56" s="16"/>
+      <c r="C56" s="16"/>
+      <c r="D56" s="16"/>
+      <c r="E56" s="16"/>
+      <c r="F56" s="16"/>
+      <c r="G56" s="16"/>
+      <c r="H56" s="20"/>
+      <c r="I56" s="16"/>
+      <c r="J56" s="16"/>
+      <c r="K56" s="16"/>
+      <c r="L56" s="16"/>
+      <c r="M56" s="16"/>
+      <c r="N56" s="16"/>
+      <c r="O56" s="16"/>
+      <c r="P56" s="16"/>
+      <c r="Q56" s="16"/>
+      <c r="R56" s="16"/>
+      <c r="S56" s="16"/>
+      <c r="T56" s="16"/>
+      <c r="U56" s="16"/>
     </row>
     <row r="57" spans="1:21">
-      <c r="A57" s="21"/>
-      <c r="B57" s="21"/>
-      <c r="C57" s="21"/>
-      <c r="D57" s="21"/>
-      <c r="E57" s="21"/>
-      <c r="F57" s="21"/>
-      <c r="G57" s="21"/>
-      <c r="H57" s="25"/>
-      <c r="I57" s="21"/>
-      <c r="J57" s="21"/>
-      <c r="K57" s="21"/>
-      <c r="L57" s="21"/>
-      <c r="M57" s="21"/>
-      <c r="N57" s="21"/>
-      <c r="O57" s="21"/>
-      <c r="P57" s="21"/>
-      <c r="Q57" s="21"/>
-      <c r="R57" s="21"/>
-      <c r="S57" s="21"/>
-      <c r="T57" s="21"/>
-      <c r="U57" s="21"/>
+      <c r="A57" s="16"/>
+      <c r="B57" s="16"/>
+      <c r="C57" s="16"/>
+      <c r="D57" s="16"/>
+      <c r="E57" s="16"/>
+      <c r="F57" s="16"/>
+      <c r="G57" s="16"/>
+      <c r="H57" s="20"/>
+      <c r="I57" s="16"/>
+      <c r="J57" s="16"/>
+      <c r="K57" s="16"/>
+      <c r="L57" s="16"/>
+      <c r="M57" s="16"/>
+      <c r="N57" s="16"/>
+      <c r="O57" s="16"/>
+      <c r="P57" s="16"/>
+      <c r="Q57" s="16"/>
+      <c r="R57" s="16"/>
+      <c r="S57" s="16"/>
+      <c r="T57" s="16"/>
+      <c r="U57" s="16"/>
     </row>
     <row r="58" spans="1:21">
-      <c r="A58" s="21"/>
-      <c r="B58" s="21"/>
-      <c r="C58" s="21"/>
-      <c r="D58" s="21"/>
-      <c r="E58" s="21"/>
-      <c r="F58" s="21"/>
-      <c r="G58" s="21"/>
-      <c r="H58" s="25"/>
-      <c r="I58" s="21"/>
-      <c r="J58" s="21"/>
-      <c r="K58" s="21"/>
-      <c r="L58" s="21"/>
-      <c r="M58" s="21"/>
-      <c r="N58" s="21"/>
-      <c r="O58" s="21"/>
-      <c r="P58" s="21"/>
-      <c r="Q58" s="21"/>
-      <c r="R58" s="21"/>
-      <c r="S58" s="21"/>
-      <c r="T58" s="21"/>
-      <c r="U58" s="21"/>
+      <c r="A58" s="16"/>
+      <c r="B58" s="16"/>
+      <c r="C58" s="16"/>
+      <c r="D58" s="16"/>
+      <c r="E58" s="16"/>
+      <c r="F58" s="16"/>
+      <c r="G58" s="16"/>
+      <c r="H58" s="20"/>
+      <c r="I58" s="16"/>
+      <c r="J58" s="16"/>
+      <c r="K58" s="16"/>
+      <c r="L58" s="16"/>
+      <c r="M58" s="16"/>
+      <c r="N58" s="16"/>
+      <c r="O58" s="16"/>
+      <c r="P58" s="16"/>
+      <c r="Q58" s="16"/>
+      <c r="R58" s="16"/>
+      <c r="S58" s="16"/>
+      <c r="T58" s="16"/>
+      <c r="U58" s="16"/>
     </row>
     <row r="59" spans="1:21">
-      <c r="A59" s="21"/>
-      <c r="B59" s="21"/>
-      <c r="C59" s="21"/>
-      <c r="D59" s="21"/>
-      <c r="E59" s="21"/>
-      <c r="F59" s="21"/>
-      <c r="G59" s="21"/>
-      <c r="H59" s="25"/>
-      <c r="I59" s="21"/>
-      <c r="J59" s="21"/>
-      <c r="K59" s="21"/>
-      <c r="L59" s="21"/>
-      <c r="M59" s="21"/>
-      <c r="N59" s="21"/>
-      <c r="O59" s="21"/>
-      <c r="P59" s="21"/>
-      <c r="Q59" s="21"/>
-      <c r="R59" s="21"/>
-      <c r="S59" s="21"/>
-      <c r="T59" s="21"/>
-      <c r="U59" s="21"/>
+      <c r="A59" s="16"/>
+      <c r="B59" s="16"/>
+      <c r="C59" s="16"/>
+      <c r="D59" s="16"/>
+      <c r="E59" s="16"/>
+      <c r="F59" s="16"/>
+      <c r="G59" s="16"/>
+      <c r="H59" s="20"/>
+      <c r="I59" s="16"/>
+      <c r="J59" s="16"/>
+      <c r="K59" s="16"/>
+      <c r="L59" s="16"/>
+      <c r="M59" s="16"/>
+      <c r="N59" s="16"/>
+      <c r="O59" s="16"/>
+      <c r="P59" s="16"/>
+      <c r="Q59" s="16"/>
+      <c r="R59" s="16"/>
+      <c r="S59" s="16"/>
+      <c r="T59" s="16"/>
+      <c r="U59" s="16"/>
     </row>
     <row r="60" spans="1:21">
-      <c r="A60" s="21"/>
-      <c r="B60" s="21"/>
-      <c r="C60" s="21"/>
-      <c r="D60" s="21"/>
-      <c r="E60" s="21"/>
-      <c r="F60" s="21"/>
-      <c r="G60" s="21"/>
-      <c r="H60" s="25"/>
-      <c r="I60" s="21"/>
-      <c r="J60" s="21"/>
-      <c r="K60" s="21"/>
-      <c r="L60" s="21"/>
-      <c r="M60" s="21"/>
-      <c r="N60" s="21"/>
-      <c r="O60" s="21"/>
-      <c r="P60" s="21"/>
-      <c r="Q60" s="21"/>
-      <c r="R60" s="21"/>
-      <c r="S60" s="21"/>
-      <c r="T60" s="21"/>
-      <c r="U60" s="21"/>
+      <c r="A60" s="16"/>
+      <c r="B60" s="16"/>
+      <c r="C60" s="16"/>
+      <c r="D60" s="16"/>
+      <c r="E60" s="16"/>
+      <c r="F60" s="16"/>
+      <c r="G60" s="16"/>
+      <c r="H60" s="20"/>
+      <c r="I60" s="16"/>
+      <c r="J60" s="16"/>
+      <c r="K60" s="16"/>
+      <c r="L60" s="16"/>
+      <c r="M60" s="16"/>
+      <c r="N60" s="16"/>
+      <c r="O60" s="16"/>
+      <c r="P60" s="16"/>
+      <c r="Q60" s="16"/>
+      <c r="R60" s="16"/>
+      <c r="S60" s="16"/>
+      <c r="T60" s="16"/>
+      <c r="U60" s="16"/>
     </row>
     <row r="61" spans="1:21">
-      <c r="A61" s="21"/>
-      <c r="B61" s="21"/>
-      <c r="C61" s="21"/>
-      <c r="D61" s="21"/>
-      <c r="E61" s="21"/>
-      <c r="F61" s="21"/>
-      <c r="G61" s="21"/>
-      <c r="H61" s="25"/>
-      <c r="I61" s="21"/>
-      <c r="J61" s="21"/>
-      <c r="K61" s="21"/>
-      <c r="L61" s="21"/>
-      <c r="M61" s="21"/>
-      <c r="N61" s="21"/>
-      <c r="O61" s="21"/>
-      <c r="P61" s="21"/>
-      <c r="Q61" s="21"/>
-      <c r="R61" s="21"/>
-      <c r="S61" s="21"/>
-      <c r="T61" s="21"/>
-      <c r="U61" s="21"/>
+      <c r="A61" s="16"/>
+      <c r="B61" s="16"/>
+      <c r="C61" s="16"/>
+      <c r="D61" s="16"/>
+      <c r="E61" s="16"/>
+      <c r="F61" s="16"/>
+      <c r="G61" s="16"/>
+      <c r="H61" s="20"/>
+      <c r="I61" s="16"/>
+      <c r="J61" s="16"/>
+      <c r="K61" s="16"/>
+      <c r="L61" s="16"/>
+      <c r="M61" s="16"/>
+      <c r="N61" s="16"/>
+      <c r="O61" s="16"/>
+      <c r="P61" s="16"/>
+      <c r="Q61" s="16"/>
+      <c r="R61" s="16"/>
+      <c r="S61" s="16"/>
+      <c r="T61" s="16"/>
+      <c r="U61" s="16"/>
     </row>
     <row r="62" spans="1:21">
-      <c r="A62" s="21"/>
-      <c r="B62" s="21"/>
-      <c r="C62" s="21"/>
-      <c r="D62" s="21"/>
-      <c r="E62" s="21"/>
-      <c r="F62" s="21"/>
-      <c r="G62" s="21"/>
-      <c r="H62" s="25"/>
-      <c r="I62" s="21"/>
-      <c r="J62" s="21"/>
-      <c r="K62" s="21"/>
-      <c r="L62" s="21"/>
-      <c r="M62" s="21"/>
-      <c r="N62" s="21"/>
-      <c r="O62" s="21"/>
-      <c r="P62" s="21"/>
-      <c r="Q62" s="21"/>
-      <c r="R62" s="21"/>
-      <c r="S62" s="21"/>
-      <c r="T62" s="21"/>
-      <c r="U62" s="21"/>
+      <c r="A62" s="16"/>
+      <c r="B62" s="16"/>
+      <c r="C62" s="16"/>
+      <c r="D62" s="16"/>
+      <c r="E62" s="16"/>
+      <c r="F62" s="16"/>
+      <c r="G62" s="16"/>
+      <c r="H62" s="20"/>
+      <c r="I62" s="16"/>
+      <c r="J62" s="16"/>
+      <c r="K62" s="16"/>
+      <c r="L62" s="16"/>
+      <c r="M62" s="16"/>
+      <c r="N62" s="16"/>
+      <c r="O62" s="16"/>
+      <c r="P62" s="16"/>
+      <c r="Q62" s="16"/>
+      <c r="R62" s="16"/>
+      <c r="S62" s="16"/>
+      <c r="T62" s="16"/>
+      <c r="U62" s="16"/>
     </row>
     <row r="63" spans="1:21">
-      <c r="A63" s="21"/>
-      <c r="B63" s="21"/>
-      <c r="C63" s="21"/>
-      <c r="D63" s="21"/>
-      <c r="E63" s="21"/>
-      <c r="F63" s="21"/>
-      <c r="G63" s="21"/>
-      <c r="H63" s="25"/>
-      <c r="I63" s="21"/>
-      <c r="J63" s="21"/>
-      <c r="K63" s="21"/>
-      <c r="L63" s="21"/>
-      <c r="M63" s="21"/>
-      <c r="N63" s="21"/>
-      <c r="O63" s="21"/>
-      <c r="P63" s="21"/>
-      <c r="Q63" s="21"/>
-      <c r="R63" s="21"/>
-      <c r="S63" s="21"/>
-      <c r="T63" s="21"/>
-      <c r="U63" s="21"/>
+      <c r="A63" s="16"/>
+      <c r="B63" s="16"/>
+      <c r="C63" s="16"/>
+      <c r="D63" s="16"/>
+      <c r="E63" s="16"/>
+      <c r="F63" s="16"/>
+      <c r="G63" s="16"/>
+      <c r="H63" s="20"/>
+      <c r="I63" s="16"/>
+      <c r="J63" s="16"/>
+      <c r="K63" s="16"/>
+      <c r="L63" s="16"/>
+      <c r="M63" s="16"/>
+      <c r="N63" s="16"/>
+      <c r="O63" s="16"/>
+      <c r="P63" s="16"/>
+      <c r="Q63" s="16"/>
+      <c r="R63" s="16"/>
+      <c r="S63" s="16"/>
+      <c r="T63" s="16"/>
+      <c r="U63" s="16"/>
     </row>
     <row r="64" spans="1:21">
-      <c r="A64" s="21"/>
-      <c r="B64" s="21"/>
-      <c r="C64" s="21"/>
-      <c r="D64" s="21"/>
-      <c r="E64" s="21"/>
-      <c r="F64" s="21"/>
-      <c r="G64" s="21"/>
-      <c r="H64" s="25"/>
-      <c r="I64" s="21"/>
-      <c r="J64" s="21"/>
-      <c r="K64" s="21"/>
-      <c r="L64" s="21"/>
-      <c r="M64" s="21"/>
-      <c r="N64" s="21"/>
-      <c r="O64" s="21"/>
-      <c r="P64" s="21"/>
-      <c r="Q64" s="21"/>
-      <c r="R64" s="21"/>
-      <c r="S64" s="21"/>
-      <c r="T64" s="21"/>
-      <c r="U64" s="21"/>
+      <c r="A64" s="16"/>
+      <c r="B64" s="16"/>
+      <c r="C64" s="16"/>
+      <c r="D64" s="16"/>
+      <c r="E64" s="16"/>
+      <c r="F64" s="16"/>
+      <c r="G64" s="16"/>
+      <c r="H64" s="20"/>
+      <c r="I64" s="16"/>
+      <c r="J64" s="16"/>
+      <c r="K64" s="16"/>
+      <c r="L64" s="16"/>
+      <c r="M64" s="16"/>
+      <c r="N64" s="16"/>
+      <c r="O64" s="16"/>
+      <c r="P64" s="16"/>
+      <c r="Q64" s="16"/>
+      <c r="R64" s="16"/>
+      <c r="S64" s="16"/>
+      <c r="T64" s="16"/>
+      <c r="U64" s="16"/>
     </row>
     <row r="65" spans="1:21">
-      <c r="A65" s="21"/>
-      <c r="B65" s="21"/>
-      <c r="C65" s="21"/>
-      <c r="D65" s="21"/>
-      <c r="E65" s="21"/>
-      <c r="F65" s="21"/>
-      <c r="G65" s="21"/>
-      <c r="H65" s="25"/>
-      <c r="I65" s="21"/>
-      <c r="J65" s="21"/>
-      <c r="K65" s="21"/>
-      <c r="L65" s="21"/>
-      <c r="M65" s="21"/>
-      <c r="N65" s="21"/>
-      <c r="O65" s="21"/>
-      <c r="P65" s="21"/>
-      <c r="Q65" s="21"/>
-      <c r="R65" s="21"/>
-      <c r="S65" s="21"/>
-      <c r="T65" s="21"/>
-      <c r="U65" s="21"/>
+      <c r="A65" s="16"/>
+      <c r="B65" s="16"/>
+      <c r="C65" s="16"/>
+      <c r="D65" s="16"/>
+      <c r="E65" s="16"/>
+      <c r="F65" s="16"/>
+      <c r="G65" s="16"/>
+      <c r="H65" s="20"/>
+      <c r="I65" s="16"/>
+      <c r="J65" s="16"/>
+      <c r="K65" s="16"/>
+      <c r="L65" s="16"/>
+      <c r="M65" s="16"/>
+      <c r="N65" s="16"/>
+      <c r="O65" s="16"/>
+      <c r="P65" s="16"/>
+      <c r="Q65" s="16"/>
+      <c r="R65" s="16"/>
+      <c r="S65" s="16"/>
+      <c r="T65" s="16"/>
+      <c r="U65" s="16"/>
     </row>
     <row r="66" spans="1:21">
-      <c r="A66" s="21"/>
-      <c r="B66" s="21"/>
-      <c r="C66" s="21"/>
-      <c r="D66" s="21"/>
-      <c r="E66" s="21"/>
-      <c r="F66" s="21"/>
-      <c r="G66" s="21"/>
-      <c r="H66" s="25"/>
-      <c r="I66" s="21"/>
-      <c r="J66" s="21"/>
-      <c r="K66" s="21"/>
-      <c r="L66" s="21"/>
-      <c r="M66" s="21"/>
-      <c r="N66" s="21"/>
-      <c r="O66" s="21"/>
-      <c r="P66" s="21"/>
-      <c r="Q66" s="21"/>
-      <c r="R66" s="21"/>
-      <c r="S66" s="21"/>
-      <c r="T66" s="21"/>
-      <c r="U66" s="21"/>
+      <c r="A66" s="16"/>
+      <c r="B66" s="16"/>
+      <c r="C66" s="16"/>
+      <c r="D66" s="16"/>
+      <c r="E66" s="16"/>
+      <c r="F66" s="16"/>
+      <c r="G66" s="16"/>
+      <c r="H66" s="20"/>
+      <c r="I66" s="16"/>
+      <c r="J66" s="16"/>
+      <c r="K66" s="16"/>
+      <c r="L66" s="16"/>
+      <c r="M66" s="16"/>
+      <c r="N66" s="16"/>
+      <c r="O66" s="16"/>
+      <c r="P66" s="16"/>
+      <c r="Q66" s="16"/>
+      <c r="R66" s="16"/>
+      <c r="S66" s="16"/>
+      <c r="T66" s="16"/>
+      <c r="U66" s="16"/>
     </row>
     <row r="67" spans="1:21">
       <c r="H67" s="7"/>
@@ -6306,6 +6458,7 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -6323,12 +6476,12 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:8" ht="13.5">
-      <c r="A2" s="14" t="s">
+      <c r="A2" s="26" t="s">
         <v>69</v>
       </c>
-      <c r="B2" s="15"/>
-      <c r="C2" s="15"/>
-      <c r="D2" s="16"/>
+      <c r="B2" s="27"/>
+      <c r="C2" s="27"/>
+      <c r="D2" s="24"/>
       <c r="F2" s="1" t="s">
         <v>70</v>
       </c>
@@ -6336,14 +6489,14 @@
       <c r="H2" s="1"/>
     </row>
     <row r="3" spans="1:8" ht="15">
-      <c r="A3" s="17" t="s">
+      <c r="A3" s="23" t="s">
         <v>71</v>
       </c>
-      <c r="B3" s="16"/>
-      <c r="C3" s="17" t="s">
+      <c r="B3" s="24"/>
+      <c r="C3" s="23" t="s">
         <v>72</v>
       </c>
-      <c r="D3" s="16"/>
+      <c r="D3" s="24"/>
       <c r="F3" s="2" t="s">
         <v>73</v>
       </c>
@@ -6351,983 +6504,1162 @@
       <c r="H3" s="1"/>
     </row>
     <row r="4" spans="1:8">
-      <c r="A4" s="17" t="s">
+      <c r="A4" s="23" t="s">
         <v>74</v>
       </c>
-      <c r="B4" s="16"/>
-      <c r="C4" s="17" t="s">
+      <c r="B4" s="24"/>
+      <c r="C4" s="23" t="s">
         <v>75</v>
       </c>
-      <c r="D4" s="16"/>
+      <c r="D4" s="24"/>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
     </row>
     <row r="5" spans="1:8">
-      <c r="A5" s="17" t="s">
+      <c r="A5" s="23" t="s">
         <v>76</v>
       </c>
-      <c r="B5" s="16"/>
-      <c r="C5" s="17" t="s">
+      <c r="B5" s="24"/>
+      <c r="C5" s="23" t="s">
         <v>77</v>
       </c>
-      <c r="D5" s="16"/>
+      <c r="D5" s="24"/>
       <c r="F5" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="6" spans="1:8">
-      <c r="A6" s="17" t="s">
+      <c r="A6" s="23" t="s">
         <v>79</v>
       </c>
-      <c r="B6" s="16"/>
-      <c r="C6" s="17" t="s">
+      <c r="B6" s="24"/>
+      <c r="C6" s="23" t="s">
         <v>80</v>
       </c>
-      <c r="D6" s="16"/>
+      <c r="D6" s="24"/>
     </row>
     <row r="7" spans="1:8">
-      <c r="A7" s="17" t="s">
+      <c r="A7" s="23" t="s">
         <v>81</v>
       </c>
-      <c r="B7" s="16"/>
-      <c r="C7" s="17" t="s">
+      <c r="B7" s="24"/>
+      <c r="C7" s="23" t="s">
         <v>82</v>
       </c>
-      <c r="D7" s="16"/>
+      <c r="D7" s="24"/>
     </row>
     <row r="8" spans="1:8">
-      <c r="A8" s="17" t="s">
+      <c r="A8" s="23" t="s">
         <v>83</v>
       </c>
-      <c r="B8" s="16"/>
-      <c r="C8" s="17" t="s">
+      <c r="B8" s="24"/>
+      <c r="C8" s="23" t="s">
         <v>84</v>
       </c>
-      <c r="D8" s="16"/>
+      <c r="D8" s="24"/>
     </row>
     <row r="9" spans="1:8">
-      <c r="A9" s="17" t="s">
+      <c r="A9" s="23" t="s">
         <v>85</v>
       </c>
-      <c r="B9" s="16"/>
-      <c r="C9" s="17" t="s">
+      <c r="B9" s="24"/>
+      <c r="C9" s="23" t="s">
         <v>86</v>
       </c>
-      <c r="D9" s="16"/>
+      <c r="D9" s="24"/>
     </row>
     <row r="10" spans="1:8">
-      <c r="A10" s="17" t="s">
+      <c r="A10" s="23" t="s">
         <v>87</v>
       </c>
-      <c r="B10" s="16"/>
-      <c r="C10" s="17" t="s">
+      <c r="B10" s="24"/>
+      <c r="C10" s="23" t="s">
         <v>88</v>
       </c>
-      <c r="D10" s="16"/>
+      <c r="D10" s="24"/>
     </row>
     <row r="11" spans="1:8">
-      <c r="A11" s="17" t="s">
+      <c r="A11" s="23" t="s">
         <v>89</v>
       </c>
-      <c r="B11" s="16"/>
-      <c r="C11" s="17" t="s">
+      <c r="B11" s="24"/>
+      <c r="C11" s="23" t="s">
         <v>90</v>
       </c>
-      <c r="D11" s="16"/>
+      <c r="D11" s="24"/>
     </row>
     <row r="12" spans="1:8">
-      <c r="A12" s="17" t="s">
+      <c r="A12" s="23" t="s">
         <v>91</v>
       </c>
-      <c r="B12" s="16"/>
-      <c r="C12" s="17" t="s">
+      <c r="B12" s="24"/>
+      <c r="C12" s="23" t="s">
         <v>92</v>
       </c>
-      <c r="D12" s="16"/>
+      <c r="D12" s="24"/>
     </row>
     <row r="13" spans="1:8">
-      <c r="A13" s="17" t="s">
+      <c r="A13" s="23" t="s">
         <v>93</v>
       </c>
-      <c r="B13" s="16"/>
-      <c r="C13" s="17" t="s">
+      <c r="B13" s="24"/>
+      <c r="C13" s="23" t="s">
         <v>94</v>
       </c>
-      <c r="D13" s="16"/>
+      <c r="D13" s="24"/>
     </row>
     <row r="14" spans="1:8">
-      <c r="A14" s="17" t="s">
+      <c r="A14" s="23" t="s">
         <v>95</v>
       </c>
-      <c r="B14" s="16"/>
-      <c r="C14" s="17" t="s">
+      <c r="B14" s="24"/>
+      <c r="C14" s="23" t="s">
         <v>96</v>
       </c>
-      <c r="D14" s="16"/>
+      <c r="D14" s="24"/>
     </row>
     <row r="15" spans="1:8">
-      <c r="A15" s="17" t="s">
+      <c r="A15" s="23" t="s">
         <v>97</v>
       </c>
-      <c r="B15" s="16"/>
-      <c r="C15" s="17" t="s">
+      <c r="B15" s="24"/>
+      <c r="C15" s="23" t="s">
         <v>98</v>
       </c>
-      <c r="D15" s="16"/>
+      <c r="D15" s="24"/>
     </row>
     <row r="16" spans="1:8">
-      <c r="A16" s="17" t="s">
+      <c r="A16" s="23" t="s">
         <v>99</v>
       </c>
-      <c r="B16" s="16"/>
-      <c r="C16" s="17" t="s">
+      <c r="B16" s="24"/>
+      <c r="C16" s="23" t="s">
         <v>100</v>
       </c>
-      <c r="D16" s="16"/>
+      <c r="D16" s="24"/>
     </row>
     <row r="17" spans="1:4">
-      <c r="A17" s="17" t="s">
+      <c r="A17" s="23" t="s">
         <v>101</v>
       </c>
-      <c r="B17" s="16"/>
-      <c r="C17" s="17" t="s">
+      <c r="B17" s="24"/>
+      <c r="C17" s="23" t="s">
         <v>102</v>
       </c>
-      <c r="D17" s="16"/>
+      <c r="D17" s="24"/>
     </row>
     <row r="18" spans="1:4">
-      <c r="A18" s="17" t="s">
+      <c r="A18" s="23" t="s">
         <v>103</v>
       </c>
-      <c r="B18" s="16"/>
-      <c r="C18" s="17" t="s">
+      <c r="B18" s="24"/>
+      <c r="C18" s="23" t="s">
         <v>104</v>
       </c>
-      <c r="D18" s="16"/>
+      <c r="D18" s="24"/>
     </row>
     <row r="19" spans="1:4">
-      <c r="A19" s="17" t="s">
+      <c r="A19" s="23" t="s">
         <v>105</v>
       </c>
-      <c r="B19" s="16"/>
-      <c r="C19" s="17" t="s">
+      <c r="B19" s="24"/>
+      <c r="C19" s="23" t="s">
         <v>106</v>
       </c>
-      <c r="D19" s="16"/>
+      <c r="D19" s="24"/>
     </row>
     <row r="20" spans="1:4">
-      <c r="A20" s="17" t="s">
+      <c r="A20" s="23" t="s">
         <v>107</v>
       </c>
-      <c r="B20" s="16"/>
-      <c r="C20" s="17" t="s">
+      <c r="B20" s="24"/>
+      <c r="C20" s="23" t="s">
         <v>108</v>
       </c>
-      <c r="D20" s="16"/>
+      <c r="D20" s="24"/>
     </row>
     <row r="21" spans="1:4">
-      <c r="A21" s="17" t="s">
+      <c r="A21" s="23" t="s">
         <v>109</v>
       </c>
-      <c r="B21" s="16"/>
-      <c r="C21" s="17" t="s">
+      <c r="B21" s="24"/>
+      <c r="C21" s="23" t="s">
         <v>110</v>
       </c>
-      <c r="D21" s="16"/>
+      <c r="D21" s="24"/>
     </row>
     <row r="22" spans="1:4">
-      <c r="A22" s="17" t="s">
+      <c r="A22" s="23" t="s">
         <v>111</v>
       </c>
-      <c r="B22" s="16"/>
-      <c r="C22" s="17" t="s">
+      <c r="B22" s="24"/>
+      <c r="C22" s="23" t="s">
         <v>112</v>
       </c>
-      <c r="D22" s="16"/>
+      <c r="D22" s="24"/>
     </row>
     <row r="23" spans="1:4">
-      <c r="A23" s="17" t="s">
+      <c r="A23" s="23" t="s">
         <v>113</v>
       </c>
-      <c r="B23" s="16"/>
-      <c r="C23" s="17" t="s">
+      <c r="B23" s="24"/>
+      <c r="C23" s="23" t="s">
         <v>114</v>
       </c>
-      <c r="D23" s="16"/>
+      <c r="D23" s="24"/>
     </row>
     <row r="24" spans="1:4">
-      <c r="A24" s="17" t="s">
+      <c r="A24" s="23" t="s">
         <v>115</v>
       </c>
-      <c r="B24" s="16"/>
-      <c r="C24" s="17" t="s">
+      <c r="B24" s="24"/>
+      <c r="C24" s="23" t="s">
         <v>116</v>
       </c>
-      <c r="D24" s="16"/>
+      <c r="D24" s="24"/>
     </row>
     <row r="25" spans="1:4">
-      <c r="A25" s="17" t="s">
+      <c r="A25" s="23" t="s">
         <v>117</v>
       </c>
-      <c r="B25" s="16"/>
-      <c r="C25" s="17" t="s">
+      <c r="B25" s="24"/>
+      <c r="C25" s="23" t="s">
         <v>118</v>
       </c>
-      <c r="D25" s="16"/>
+      <c r="D25" s="24"/>
     </row>
     <row r="26" spans="1:4">
-      <c r="A26" s="17" t="s">
+      <c r="A26" s="23" t="s">
         <v>119</v>
       </c>
-      <c r="B26" s="16"/>
-      <c r="C26" s="17" t="s">
+      <c r="B26" s="24"/>
+      <c r="C26" s="23" t="s">
         <v>120</v>
       </c>
-      <c r="D26" s="16"/>
+      <c r="D26" s="24"/>
     </row>
     <row r="27" spans="1:4">
-      <c r="A27" s="17" t="s">
+      <c r="A27" s="23" t="s">
         <v>121</v>
       </c>
-      <c r="B27" s="16"/>
-      <c r="C27" s="17" t="s">
+      <c r="B27" s="24"/>
+      <c r="C27" s="23" t="s">
         <v>122</v>
       </c>
-      <c r="D27" s="16"/>
+      <c r="D27" s="24"/>
     </row>
     <row r="28" spans="1:4">
-      <c r="A28" s="17" t="s">
+      <c r="A28" s="23" t="s">
         <v>123</v>
       </c>
-      <c r="B28" s="16"/>
-      <c r="C28" s="17" t="s">
+      <c r="B28" s="24"/>
+      <c r="C28" s="23" t="s">
         <v>124</v>
       </c>
-      <c r="D28" s="16"/>
+      <c r="D28" s="24"/>
     </row>
     <row r="29" spans="1:4">
-      <c r="A29" s="17" t="s">
+      <c r="A29" s="23" t="s">
         <v>125</v>
       </c>
-      <c r="B29" s="16"/>
-      <c r="C29" s="17" t="s">
+      <c r="B29" s="24"/>
+      <c r="C29" s="23" t="s">
         <v>126</v>
       </c>
-      <c r="D29" s="16"/>
+      <c r="D29" s="24"/>
     </row>
     <row r="30" spans="1:4">
-      <c r="A30" s="17" t="s">
+      <c r="A30" s="23" t="s">
         <v>127</v>
       </c>
-      <c r="B30" s="16"/>
-      <c r="C30" s="17" t="s">
+      <c r="B30" s="24"/>
+      <c r="C30" s="23" t="s">
         <v>128</v>
       </c>
-      <c r="D30" s="16"/>
+      <c r="D30" s="24"/>
     </row>
     <row r="31" spans="1:4">
-      <c r="A31" s="17" t="s">
+      <c r="A31" s="23" t="s">
         <v>129</v>
       </c>
-      <c r="B31" s="16"/>
-      <c r="C31" s="17" t="s">
+      <c r="B31" s="24"/>
+      <c r="C31" s="23" t="s">
         <v>130</v>
       </c>
-      <c r="D31" s="16"/>
+      <c r="D31" s="24"/>
     </row>
     <row r="32" spans="1:4">
-      <c r="A32" s="17" t="s">
+      <c r="A32" s="23" t="s">
         <v>131</v>
       </c>
-      <c r="B32" s="16"/>
-      <c r="C32" s="17" t="s">
+      <c r="B32" s="24"/>
+      <c r="C32" s="23" t="s">
         <v>132</v>
       </c>
-      <c r="D32" s="16"/>
+      <c r="D32" s="24"/>
     </row>
     <row r="33" spans="1:4">
-      <c r="A33" s="17" t="s">
+      <c r="A33" s="23" t="s">
         <v>133</v>
       </c>
-      <c r="B33" s="16"/>
-      <c r="C33" s="17" t="s">
+      <c r="B33" s="24"/>
+      <c r="C33" s="23" t="s">
         <v>134</v>
       </c>
-      <c r="D33" s="16"/>
+      <c r="D33" s="24"/>
     </row>
     <row r="34" spans="1:4">
-      <c r="A34" s="17" t="s">
+      <c r="A34" s="23" t="s">
         <v>135</v>
       </c>
-      <c r="B34" s="16"/>
-      <c r="C34" s="17" t="s">
+      <c r="B34" s="24"/>
+      <c r="C34" s="23" t="s">
         <v>136</v>
       </c>
-      <c r="D34" s="16"/>
+      <c r="D34" s="24"/>
     </row>
     <row r="35" spans="1:4">
-      <c r="A35" s="17" t="s">
+      <c r="A35" s="23" t="s">
         <v>137</v>
       </c>
-      <c r="B35" s="16"/>
-      <c r="C35" s="17" t="s">
+      <c r="B35" s="24"/>
+      <c r="C35" s="23" t="s">
         <v>138</v>
       </c>
-      <c r="D35" s="16"/>
+      <c r="D35" s="24"/>
     </row>
     <row r="36" spans="1:4">
-      <c r="A36" s="17" t="s">
+      <c r="A36" s="23" t="s">
         <v>139</v>
       </c>
-      <c r="B36" s="16"/>
-      <c r="C36" s="17" t="s">
+      <c r="B36" s="24"/>
+      <c r="C36" s="23" t="s">
         <v>140</v>
       </c>
-      <c r="D36" s="16"/>
+      <c r="D36" s="24"/>
     </row>
     <row r="37" spans="1:4">
-      <c r="A37" s="17" t="s">
+      <c r="A37" s="23" t="s">
         <v>141</v>
       </c>
-      <c r="B37" s="16"/>
-      <c r="C37" s="17" t="s">
+      <c r="B37" s="24"/>
+      <c r="C37" s="23" t="s">
         <v>142</v>
       </c>
-      <c r="D37" s="16"/>
+      <c r="D37" s="24"/>
     </row>
     <row r="38" spans="1:4">
-      <c r="A38" s="17" t="s">
+      <c r="A38" s="23" t="s">
         <v>143</v>
       </c>
-      <c r="B38" s="16"/>
-      <c r="C38" s="17" t="s">
+      <c r="B38" s="24"/>
+      <c r="C38" s="23" t="s">
         <v>144</v>
       </c>
-      <c r="D38" s="16"/>
+      <c r="D38" s="24"/>
     </row>
     <row r="39" spans="1:4">
-      <c r="A39" s="17" t="s">
+      <c r="A39" s="23" t="s">
         <v>145</v>
       </c>
-      <c r="B39" s="16"/>
-      <c r="C39" s="17" t="s">
+      <c r="B39" s="24"/>
+      <c r="C39" s="23" t="s">
         <v>146</v>
       </c>
-      <c r="D39" s="16"/>
+      <c r="D39" s="24"/>
     </row>
     <row r="40" spans="1:4">
-      <c r="A40" s="17" t="s">
+      <c r="A40" s="23" t="s">
         <v>147</v>
       </c>
-      <c r="B40" s="16"/>
-      <c r="C40" s="17" t="s">
+      <c r="B40" s="24"/>
+      <c r="C40" s="23" t="s">
         <v>148</v>
       </c>
-      <c r="D40" s="16"/>
+      <c r="D40" s="24"/>
     </row>
     <row r="41" spans="1:4">
-      <c r="A41" s="17" t="s">
+      <c r="A41" s="23" t="s">
         <v>149</v>
       </c>
-      <c r="B41" s="16"/>
-      <c r="C41" s="17" t="s">
+      <c r="B41" s="24"/>
+      <c r="C41" s="23" t="s">
         <v>150</v>
       </c>
-      <c r="D41" s="16"/>
+      <c r="D41" s="24"/>
     </row>
     <row r="42" spans="1:4">
-      <c r="A42" s="17" t="s">
+      <c r="A42" s="23" t="s">
         <v>151</v>
       </c>
-      <c r="B42" s="16"/>
-      <c r="C42" s="17" t="s">
+      <c r="B42" s="24"/>
+      <c r="C42" s="23" t="s">
         <v>152</v>
       </c>
-      <c r="D42" s="16"/>
+      <c r="D42" s="24"/>
     </row>
     <row r="43" spans="1:4">
-      <c r="A43" s="17" t="s">
+      <c r="A43" s="23" t="s">
         <v>153</v>
       </c>
-      <c r="B43" s="16"/>
-      <c r="C43" s="17" t="s">
+      <c r="B43" s="24"/>
+      <c r="C43" s="23" t="s">
         <v>154</v>
       </c>
-      <c r="D43" s="16"/>
+      <c r="D43" s="24"/>
     </row>
     <row r="44" spans="1:4">
-      <c r="A44" s="17" t="s">
+      <c r="A44" s="23" t="s">
         <v>155</v>
       </c>
-      <c r="B44" s="16"/>
-      <c r="C44" s="17" t="s">
+      <c r="B44" s="24"/>
+      <c r="C44" s="23" t="s">
         <v>156</v>
       </c>
-      <c r="D44" s="16"/>
+      <c r="D44" s="24"/>
     </row>
     <row r="45" spans="1:4">
-      <c r="A45" s="17" t="s">
+      <c r="A45" s="23" t="s">
         <v>157</v>
       </c>
-      <c r="B45" s="16"/>
-      <c r="C45" s="17" t="s">
+      <c r="B45" s="24"/>
+      <c r="C45" s="23" t="s">
         <v>158</v>
       </c>
-      <c r="D45" s="16"/>
+      <c r="D45" s="24"/>
     </row>
     <row r="46" spans="1:4">
-      <c r="A46" s="17" t="s">
+      <c r="A46" s="23" t="s">
         <v>159</v>
       </c>
-      <c r="B46" s="16"/>
-      <c r="C46" s="17" t="s">
+      <c r="B46" s="24"/>
+      <c r="C46" s="23" t="s">
         <v>160</v>
       </c>
-      <c r="D46" s="16"/>
+      <c r="D46" s="24"/>
     </row>
     <row r="47" spans="1:4">
-      <c r="A47" s="17" t="s">
+      <c r="A47" s="23" t="s">
         <v>161</v>
       </c>
-      <c r="B47" s="16"/>
-      <c r="C47" s="17" t="s">
+      <c r="B47" s="24"/>
+      <c r="C47" s="23" t="s">
         <v>162</v>
       </c>
-      <c r="D47" s="16"/>
+      <c r="D47" s="24"/>
     </row>
     <row r="48" spans="1:4">
-      <c r="A48" s="17" t="s">
+      <c r="A48" s="23" t="s">
         <v>163</v>
       </c>
-      <c r="B48" s="16"/>
-      <c r="C48" s="17" t="s">
+      <c r="B48" s="24"/>
+      <c r="C48" s="23" t="s">
         <v>164</v>
       </c>
-      <c r="D48" s="16"/>
+      <c r="D48" s="24"/>
     </row>
     <row r="49" spans="1:4">
-      <c r="A49" s="17" t="s">
+      <c r="A49" s="23" t="s">
         <v>165</v>
       </c>
-      <c r="B49" s="16"/>
-      <c r="C49" s="17" t="s">
+      <c r="B49" s="24"/>
+      <c r="C49" s="23" t="s">
         <v>166</v>
       </c>
-      <c r="D49" s="16"/>
+      <c r="D49" s="24"/>
     </row>
     <row r="50" spans="1:4">
-      <c r="A50" s="17" t="s">
+      <c r="A50" s="23" t="s">
         <v>167</v>
       </c>
-      <c r="B50" s="16"/>
-      <c r="C50" s="17" t="s">
+      <c r="B50" s="24"/>
+      <c r="C50" s="23" t="s">
         <v>168</v>
       </c>
-      <c r="D50" s="16"/>
+      <c r="D50" s="24"/>
     </row>
     <row r="51" spans="1:4">
-      <c r="A51" s="17" t="s">
+      <c r="A51" s="23" t="s">
         <v>169</v>
       </c>
-      <c r="B51" s="16"/>
-      <c r="C51" s="17" t="s">
+      <c r="B51" s="24"/>
+      <c r="C51" s="23" t="s">
         <v>170</v>
       </c>
-      <c r="D51" s="16"/>
+      <c r="D51" s="24"/>
     </row>
     <row r="52" spans="1:4">
-      <c r="A52" s="17" t="s">
+      <c r="A52" s="23" t="s">
         <v>171</v>
       </c>
-      <c r="B52" s="16"/>
-      <c r="C52" s="17" t="s">
+      <c r="B52" s="24"/>
+      <c r="C52" s="23" t="s">
         <v>172</v>
       </c>
-      <c r="D52" s="16"/>
+      <c r="D52" s="24"/>
     </row>
     <row r="53" spans="1:4">
-      <c r="A53" s="17" t="s">
+      <c r="A53" s="23" t="s">
         <v>173</v>
       </c>
-      <c r="B53" s="16"/>
-      <c r="C53" s="17" t="s">
+      <c r="B53" s="24"/>
+      <c r="C53" s="23" t="s">
         <v>174</v>
       </c>
-      <c r="D53" s="16"/>
+      <c r="D53" s="24"/>
     </row>
     <row r="54" spans="1:4">
-      <c r="A54" s="17" t="s">
+      <c r="A54" s="23" t="s">
         <v>175</v>
       </c>
-      <c r="B54" s="16"/>
-      <c r="C54" s="17" t="s">
+      <c r="B54" s="24"/>
+      <c r="C54" s="23" t="s">
         <v>176</v>
       </c>
-      <c r="D54" s="16"/>
+      <c r="D54" s="24"/>
     </row>
     <row r="55" spans="1:4">
-      <c r="A55" s="17" t="s">
+      <c r="A55" s="23" t="s">
         <v>177</v>
       </c>
-      <c r="B55" s="16"/>
-      <c r="C55" s="17" t="s">
+      <c r="B55" s="24"/>
+      <c r="C55" s="23" t="s">
         <v>178</v>
       </c>
-      <c r="D55" s="16"/>
+      <c r="D55" s="24"/>
     </row>
     <row r="56" spans="1:4">
-      <c r="A56" s="17" t="s">
+      <c r="A56" s="23" t="s">
         <v>179</v>
       </c>
-      <c r="B56" s="16"/>
-      <c r="C56" s="17" t="s">
+      <c r="B56" s="24"/>
+      <c r="C56" s="23" t="s">
         <v>180</v>
       </c>
-      <c r="D56" s="16"/>
+      <c r="D56" s="24"/>
     </row>
     <row r="57" spans="1:4">
-      <c r="A57" s="17" t="s">
+      <c r="A57" s="23" t="s">
         <v>181</v>
       </c>
-      <c r="B57" s="16"/>
-      <c r="C57" s="17" t="s">
+      <c r="B57" s="24"/>
+      <c r="C57" s="23" t="s">
         <v>182</v>
       </c>
-      <c r="D57" s="16"/>
+      <c r="D57" s="24"/>
     </row>
     <row r="58" spans="1:4">
-      <c r="A58" s="17" t="s">
+      <c r="A58" s="23" t="s">
         <v>183</v>
       </c>
-      <c r="B58" s="16"/>
-      <c r="C58" s="17" t="s">
+      <c r="B58" s="24"/>
+      <c r="C58" s="23" t="s">
         <v>184</v>
       </c>
-      <c r="D58" s="16"/>
+      <c r="D58" s="24"/>
     </row>
     <row r="59" spans="1:4">
-      <c r="A59" s="17" t="s">
+      <c r="A59" s="23" t="s">
         <v>185</v>
       </c>
-      <c r="B59" s="16"/>
-      <c r="C59" s="17" t="s">
+      <c r="B59" s="24"/>
+      <c r="C59" s="23" t="s">
         <v>150</v>
       </c>
-      <c r="D59" s="16"/>
+      <c r="D59" s="24"/>
     </row>
     <row r="60" spans="1:4">
-      <c r="A60" s="17" t="s">
+      <c r="A60" s="23" t="s">
         <v>186</v>
       </c>
-      <c r="B60" s="16"/>
-      <c r="C60" s="17" t="s">
+      <c r="B60" s="24"/>
+      <c r="C60" s="23" t="s">
         <v>187</v>
       </c>
-      <c r="D60" s="16"/>
+      <c r="D60" s="24"/>
     </row>
     <row r="61" spans="1:4">
-      <c r="A61" s="17" t="s">
+      <c r="A61" s="23" t="s">
         <v>188</v>
       </c>
-      <c r="B61" s="16"/>
-      <c r="C61" s="17" t="s">
+      <c r="B61" s="24"/>
+      <c r="C61" s="23" t="s">
         <v>189</v>
       </c>
-      <c r="D61" s="16"/>
+      <c r="D61" s="24"/>
     </row>
     <row r="62" spans="1:4">
-      <c r="A62" s="17" t="s">
+      <c r="A62" s="23" t="s">
         <v>190</v>
       </c>
-      <c r="B62" s="16"/>
-      <c r="C62" s="17" t="s">
+      <c r="B62" s="24"/>
+      <c r="C62" s="23" t="s">
         <v>191</v>
       </c>
-      <c r="D62" s="16"/>
+      <c r="D62" s="24"/>
     </row>
     <row r="63" spans="1:4">
-      <c r="A63" s="17" t="s">
+      <c r="A63" s="23" t="s">
         <v>192</v>
       </c>
-      <c r="B63" s="16"/>
-      <c r="C63" s="17" t="s">
+      <c r="B63" s="24"/>
+      <c r="C63" s="23" t="s">
         <v>193</v>
       </c>
-      <c r="D63" s="16"/>
+      <c r="D63" s="24"/>
     </row>
     <row r="64" spans="1:4">
-      <c r="A64" s="17" t="s">
+      <c r="A64" s="23" t="s">
         <v>194</v>
       </c>
-      <c r="B64" s="16"/>
-      <c r="C64" s="17" t="s">
+      <c r="B64" s="24"/>
+      <c r="C64" s="23" t="s">
         <v>195</v>
       </c>
-      <c r="D64" s="16"/>
+      <c r="D64" s="24"/>
     </row>
     <row r="65" spans="1:4">
-      <c r="A65" s="17" t="s">
+      <c r="A65" s="23" t="s">
         <v>196</v>
       </c>
-      <c r="B65" s="16"/>
-      <c r="C65" s="17" t="s">
+      <c r="B65" s="24"/>
+      <c r="C65" s="23" t="s">
         <v>197</v>
       </c>
-      <c r="D65" s="16"/>
+      <c r="D65" s="24"/>
     </row>
     <row r="66" spans="1:4">
-      <c r="A66" s="17" t="s">
+      <c r="A66" s="23" t="s">
         <v>198</v>
       </c>
-      <c r="B66" s="16"/>
-      <c r="C66" s="17" t="s">
+      <c r="B66" s="24"/>
+      <c r="C66" s="23" t="s">
         <v>199</v>
       </c>
-      <c r="D66" s="16"/>
+      <c r="D66" s="24"/>
     </row>
     <row r="67" spans="1:4">
-      <c r="A67" s="17" t="s">
+      <c r="A67" s="23" t="s">
         <v>200</v>
       </c>
-      <c r="B67" s="16"/>
-      <c r="C67" s="17" t="s">
+      <c r="B67" s="24"/>
+      <c r="C67" s="23" t="s">
         <v>201</v>
       </c>
-      <c r="D67" s="16"/>
+      <c r="D67" s="24"/>
     </row>
     <row r="68" spans="1:4">
-      <c r="A68" s="17" t="s">
+      <c r="A68" s="23" t="s">
         <v>202</v>
       </c>
-      <c r="B68" s="16"/>
-      <c r="C68" s="17" t="s">
+      <c r="B68" s="24"/>
+      <c r="C68" s="23" t="s">
         <v>203</v>
       </c>
-      <c r="D68" s="16"/>
+      <c r="D68" s="24"/>
     </row>
     <row r="69" spans="1:4">
-      <c r="A69" s="17" t="s">
+      <c r="A69" s="23" t="s">
         <v>204</v>
       </c>
-      <c r="B69" s="16"/>
-      <c r="C69" s="17" t="s">
+      <c r="B69" s="24"/>
+      <c r="C69" s="23" t="s">
         <v>205</v>
       </c>
-      <c r="D69" s="16"/>
+      <c r="D69" s="24"/>
     </row>
     <row r="70" spans="1:4">
-      <c r="A70" s="17" t="s">
+      <c r="A70" s="23" t="s">
         <v>206</v>
       </c>
-      <c r="B70" s="16"/>
-      <c r="C70" s="17" t="s">
+      <c r="B70" s="24"/>
+      <c r="C70" s="23" t="s">
         <v>207</v>
       </c>
-      <c r="D70" s="16"/>
+      <c r="D70" s="24"/>
     </row>
     <row r="71" spans="1:4">
-      <c r="A71" s="18" t="s">
+      <c r="A71" s="25" t="s">
         <v>208</v>
       </c>
-      <c r="B71" s="16"/>
-      <c r="C71" s="17" t="s">
+      <c r="B71" s="24"/>
+      <c r="C71" s="23" t="s">
         <v>209</v>
       </c>
-      <c r="D71" s="16"/>
+      <c r="D71" s="24"/>
     </row>
     <row r="72" spans="1:4">
-      <c r="A72" s="17" t="s">
+      <c r="A72" s="23" t="s">
         <v>210</v>
       </c>
-      <c r="B72" s="16"/>
-      <c r="C72" s="17" t="s">
+      <c r="B72" s="24"/>
+      <c r="C72" s="23" t="s">
         <v>211</v>
       </c>
-      <c r="D72" s="16"/>
+      <c r="D72" s="24"/>
     </row>
     <row r="73" spans="1:4">
-      <c r="A73" s="17" t="s">
+      <c r="A73" s="23" t="s">
         <v>212</v>
       </c>
-      <c r="B73" s="16"/>
-      <c r="C73" s="17" t="s">
+      <c r="B73" s="24"/>
+      <c r="C73" s="23" t="s">
         <v>213</v>
       </c>
-      <c r="D73" s="16"/>
+      <c r="D73" s="24"/>
     </row>
     <row r="74" spans="1:4">
-      <c r="A74" s="17" t="s">
+      <c r="A74" s="23" t="s">
         <v>214</v>
       </c>
-      <c r="B74" s="16"/>
-      <c r="C74" s="17" t="s">
+      <c r="B74" s="24"/>
+      <c r="C74" s="23" t="s">
         <v>215</v>
       </c>
-      <c r="D74" s="16"/>
+      <c r="D74" s="24"/>
     </row>
     <row r="75" spans="1:4">
-      <c r="A75" s="17" t="s">
+      <c r="A75" s="23" t="s">
         <v>216</v>
       </c>
-      <c r="B75" s="16"/>
-      <c r="C75" s="17" t="s">
+      <c r="B75" s="24"/>
+      <c r="C75" s="23" t="s">
         <v>217</v>
       </c>
-      <c r="D75" s="16"/>
+      <c r="D75" s="24"/>
     </row>
     <row r="76" spans="1:4">
-      <c r="A76" s="17" t="s">
+      <c r="A76" s="23" t="s">
         <v>218</v>
       </c>
-      <c r="B76" s="16"/>
-      <c r="C76" s="17" t="s">
+      <c r="B76" s="24"/>
+      <c r="C76" s="23" t="s">
         <v>219</v>
       </c>
-      <c r="D76" s="16"/>
+      <c r="D76" s="24"/>
     </row>
     <row r="77" spans="1:4">
-      <c r="A77" s="17" t="s">
+      <c r="A77" s="23" t="s">
         <v>220</v>
       </c>
-      <c r="B77" s="16"/>
-      <c r="C77" s="17" t="s">
+      <c r="B77" s="24"/>
+      <c r="C77" s="23" t="s">
         <v>221</v>
       </c>
-      <c r="D77" s="16"/>
+      <c r="D77" s="24"/>
     </row>
     <row r="78" spans="1:4">
-      <c r="A78" s="17" t="s">
+      <c r="A78" s="23" t="s">
         <v>222</v>
       </c>
-      <c r="B78" s="16"/>
-      <c r="C78" s="17" t="s">
+      <c r="B78" s="24"/>
+      <c r="C78" s="23" t="s">
         <v>223</v>
       </c>
-      <c r="D78" s="16"/>
+      <c r="D78" s="24"/>
     </row>
     <row r="79" spans="1:4">
-      <c r="A79" s="17" t="s">
+      <c r="A79" s="23" t="s">
         <v>224</v>
       </c>
-      <c r="B79" s="16"/>
-      <c r="C79" s="17" t="s">
+      <c r="B79" s="24"/>
+      <c r="C79" s="23" t="s">
         <v>225</v>
       </c>
-      <c r="D79" s="16"/>
+      <c r="D79" s="24"/>
     </row>
     <row r="80" spans="1:4">
-      <c r="A80" s="17" t="s">
+      <c r="A80" s="23" t="s">
         <v>226</v>
       </c>
-      <c r="B80" s="16"/>
-      <c r="C80" s="17" t="s">
+      <c r="B80" s="24"/>
+      <c r="C80" s="23" t="s">
         <v>227</v>
       </c>
-      <c r="D80" s="16"/>
+      <c r="D80" s="24"/>
     </row>
     <row r="81" spans="1:4">
-      <c r="A81" s="17" t="s">
+      <c r="A81" s="23" t="s">
         <v>228</v>
       </c>
-      <c r="B81" s="16"/>
-      <c r="C81" s="17" t="s">
+      <c r="B81" s="24"/>
+      <c r="C81" s="23" t="s">
         <v>229</v>
       </c>
-      <c r="D81" s="16"/>
+      <c r="D81" s="24"/>
     </row>
     <row r="82" spans="1:4">
-      <c r="A82" s="17" t="s">
+      <c r="A82" s="23" t="s">
         <v>230</v>
       </c>
-      <c r="B82" s="16"/>
-      <c r="C82" s="17" t="s">
+      <c r="B82" s="24"/>
+      <c r="C82" s="23" t="s">
         <v>231</v>
       </c>
-      <c r="D82" s="16"/>
+      <c r="D82" s="24"/>
     </row>
     <row r="83" spans="1:4">
-      <c r="A83" s="17" t="s">
+      <c r="A83" s="23" t="s">
         <v>232</v>
       </c>
-      <c r="B83" s="16"/>
-      <c r="C83" s="17" t="s">
+      <c r="B83" s="24"/>
+      <c r="C83" s="23" t="s">
         <v>233</v>
       </c>
-      <c r="D83" s="16"/>
+      <c r="D83" s="24"/>
     </row>
     <row r="84" spans="1:4">
-      <c r="A84" s="17" t="s">
+      <c r="A84" s="23" t="s">
         <v>234</v>
       </c>
-      <c r="B84" s="16"/>
-      <c r="C84" s="17" t="s">
+      <c r="B84" s="24"/>
+      <c r="C84" s="23" t="s">
         <v>235</v>
       </c>
-      <c r="D84" s="16"/>
+      <c r="D84" s="24"/>
     </row>
     <row r="85" spans="1:4">
-      <c r="A85" s="17" t="s">
+      <c r="A85" s="23" t="s">
         <v>236</v>
       </c>
-      <c r="B85" s="16"/>
-      <c r="C85" s="17" t="s">
+      <c r="B85" s="24"/>
+      <c r="C85" s="23" t="s">
         <v>237</v>
       </c>
-      <c r="D85" s="16"/>
+      <c r="D85" s="24"/>
     </row>
     <row r="86" spans="1:4">
-      <c r="A86" s="17" t="s">
+      <c r="A86" s="23" t="s">
         <v>238</v>
       </c>
-      <c r="B86" s="16"/>
-      <c r="C86" s="17" t="s">
+      <c r="B86" s="24"/>
+      <c r="C86" s="23" t="s">
         <v>239</v>
       </c>
-      <c r="D86" s="16"/>
+      <c r="D86" s="24"/>
     </row>
     <row r="87" spans="1:4">
-      <c r="A87" s="17" t="s">
+      <c r="A87" s="23" t="s">
         <v>240</v>
       </c>
-      <c r="B87" s="16"/>
-      <c r="C87" s="17" t="s">
+      <c r="B87" s="24"/>
+      <c r="C87" s="23" t="s">
         <v>241</v>
       </c>
-      <c r="D87" s="16"/>
+      <c r="D87" s="24"/>
     </row>
     <row r="88" spans="1:4">
-      <c r="A88" s="17" t="s">
+      <c r="A88" s="23" t="s">
         <v>242</v>
       </c>
-      <c r="B88" s="16"/>
-      <c r="C88" s="17" t="s">
+      <c r="B88" s="24"/>
+      <c r="C88" s="23" t="s">
         <v>243</v>
       </c>
-      <c r="D88" s="16"/>
+      <c r="D88" s="24"/>
     </row>
     <row r="89" spans="1:4">
-      <c r="A89" s="17" t="s">
+      <c r="A89" s="23" t="s">
         <v>244</v>
       </c>
-      <c r="B89" s="16"/>
-      <c r="C89" s="17" t="s">
+      <c r="B89" s="24"/>
+      <c r="C89" s="23" t="s">
         <v>245</v>
       </c>
-      <c r="D89" s="16"/>
+      <c r="D89" s="24"/>
     </row>
     <row r="90" spans="1:4">
-      <c r="A90" s="17" t="s">
+      <c r="A90" s="23" t="s">
         <v>246</v>
       </c>
-      <c r="B90" s="16"/>
-      <c r="C90" s="17" t="s">
+      <c r="B90" s="24"/>
+      <c r="C90" s="23" t="s">
         <v>247</v>
       </c>
-      <c r="D90" s="16"/>
+      <c r="D90" s="24"/>
     </row>
     <row r="91" spans="1:4">
-      <c r="A91" s="17" t="s">
+      <c r="A91" s="23" t="s">
         <v>248</v>
       </c>
-      <c r="B91" s="16"/>
-      <c r="C91" s="17" t="s">
+      <c r="B91" s="24"/>
+      <c r="C91" s="23" t="s">
         <v>249</v>
       </c>
-      <c r="D91" s="16"/>
+      <c r="D91" s="24"/>
     </row>
     <row r="92" spans="1:4">
-      <c r="A92" s="17" t="s">
+      <c r="A92" s="23" t="s">
         <v>250</v>
       </c>
-      <c r="B92" s="16"/>
-      <c r="C92" s="17" t="s">
+      <c r="B92" s="24"/>
+      <c r="C92" s="23" t="s">
         <v>251</v>
       </c>
-      <c r="D92" s="16"/>
+      <c r="D92" s="24"/>
     </row>
     <row r="93" spans="1:4">
-      <c r="A93" s="17" t="s">
+      <c r="A93" s="23" t="s">
         <v>252</v>
       </c>
-      <c r="B93" s="16"/>
-      <c r="C93" s="17" t="s">
+      <c r="B93" s="24"/>
+      <c r="C93" s="23" t="s">
         <v>253</v>
       </c>
-      <c r="D93" s="16"/>
+      <c r="D93" s="24"/>
     </row>
     <row r="94" spans="1:4">
-      <c r="A94" s="17" t="s">
+      <c r="A94" s="23" t="s">
         <v>254</v>
       </c>
-      <c r="B94" s="16"/>
-      <c r="C94" s="17" t="s">
+      <c r="B94" s="24"/>
+      <c r="C94" s="23" t="s">
         <v>255</v>
       </c>
-      <c r="D94" s="16"/>
+      <c r="D94" s="24"/>
     </row>
     <row r="95" spans="1:4">
-      <c r="A95" s="17" t="s">
+      <c r="A95" s="23" t="s">
         <v>256</v>
       </c>
-      <c r="B95" s="16"/>
-      <c r="C95" s="17" t="s">
+      <c r="B95" s="24"/>
+      <c r="C95" s="23" t="s">
         <v>257</v>
       </c>
-      <c r="D95" s="16"/>
+      <c r="D95" s="24"/>
     </row>
     <row r="96" spans="1:4">
-      <c r="A96" s="17" t="s">
+      <c r="A96" s="23" t="s">
         <v>258</v>
       </c>
-      <c r="B96" s="16"/>
-      <c r="C96" s="17" t="s">
+      <c r="B96" s="24"/>
+      <c r="C96" s="23" t="s">
         <v>259</v>
       </c>
-      <c r="D96" s="16"/>
+      <c r="D96" s="24"/>
     </row>
     <row r="97" spans="1:4">
-      <c r="A97" s="17" t="s">
+      <c r="A97" s="23" t="s">
         <v>260</v>
       </c>
-      <c r="B97" s="16"/>
-      <c r="C97" s="17" t="s">
+      <c r="B97" s="24"/>
+      <c r="C97" s="23" t="s">
         <v>261</v>
       </c>
-      <c r="D97" s="16"/>
+      <c r="D97" s="24"/>
     </row>
     <row r="98" spans="1:4">
-      <c r="A98" s="17" t="s">
+      <c r="A98" s="23" t="s">
         <v>262</v>
       </c>
-      <c r="B98" s="16"/>
-      <c r="C98" s="17" t="s">
+      <c r="B98" s="24"/>
+      <c r="C98" s="23" t="s">
         <v>263</v>
       </c>
-      <c r="D98" s="16"/>
+      <c r="D98" s="24"/>
     </row>
     <row r="99" spans="1:4">
-      <c r="A99" s="17" t="s">
+      <c r="A99" s="23" t="s">
         <v>264</v>
       </c>
-      <c r="B99" s="16"/>
-      <c r="C99" s="17" t="s">
+      <c r="B99" s="24"/>
+      <c r="C99" s="23" t="s">
         <v>265</v>
       </c>
-      <c r="D99" s="16"/>
+      <c r="D99" s="24"/>
     </row>
     <row r="100" spans="1:4">
-      <c r="A100" s="17" t="s">
+      <c r="A100" s="23" t="s">
         <v>266</v>
       </c>
-      <c r="B100" s="16"/>
-      <c r="C100" s="17" t="s">
+      <c r="B100" s="24"/>
+      <c r="C100" s="23" t="s">
         <v>267</v>
       </c>
-      <c r="D100" s="16"/>
+      <c r="D100" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="197">
+    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="A29:B29"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="C30:D30"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="C31:D31"/>
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="C32:D32"/>
+    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="C33:D33"/>
+    <mergeCell ref="A34:B34"/>
+    <mergeCell ref="C34:D34"/>
+    <mergeCell ref="A35:B35"/>
+    <mergeCell ref="C35:D35"/>
+    <mergeCell ref="A36:B36"/>
+    <mergeCell ref="C36:D36"/>
+    <mergeCell ref="A37:B37"/>
+    <mergeCell ref="C37:D37"/>
+    <mergeCell ref="A38:B38"/>
+    <mergeCell ref="C38:D38"/>
+    <mergeCell ref="A39:B39"/>
+    <mergeCell ref="C39:D39"/>
+    <mergeCell ref="A40:B40"/>
+    <mergeCell ref="C40:D40"/>
+    <mergeCell ref="A41:B41"/>
+    <mergeCell ref="C41:D41"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="C42:D42"/>
+    <mergeCell ref="A43:B43"/>
+    <mergeCell ref="C43:D43"/>
+    <mergeCell ref="A44:B44"/>
+    <mergeCell ref="C44:D44"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="C45:D45"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="C46:D46"/>
+    <mergeCell ref="A47:B47"/>
+    <mergeCell ref="C47:D47"/>
+    <mergeCell ref="A48:B48"/>
+    <mergeCell ref="C48:D48"/>
+    <mergeCell ref="A49:B49"/>
+    <mergeCell ref="C49:D49"/>
+    <mergeCell ref="A50:B50"/>
+    <mergeCell ref="C50:D50"/>
+    <mergeCell ref="A51:B51"/>
+    <mergeCell ref="C51:D51"/>
+    <mergeCell ref="A52:B52"/>
+    <mergeCell ref="C52:D52"/>
+    <mergeCell ref="A53:B53"/>
+    <mergeCell ref="C53:D53"/>
+    <mergeCell ref="A54:B54"/>
+    <mergeCell ref="C54:D54"/>
+    <mergeCell ref="A55:B55"/>
+    <mergeCell ref="C55:D55"/>
+    <mergeCell ref="A56:B56"/>
+    <mergeCell ref="C56:D56"/>
+    <mergeCell ref="A57:B57"/>
+    <mergeCell ref="C57:D57"/>
+    <mergeCell ref="A58:B58"/>
+    <mergeCell ref="C58:D58"/>
+    <mergeCell ref="A59:B59"/>
+    <mergeCell ref="C59:D59"/>
+    <mergeCell ref="A60:B60"/>
+    <mergeCell ref="C60:D60"/>
+    <mergeCell ref="A61:B61"/>
+    <mergeCell ref="C61:D61"/>
+    <mergeCell ref="A62:B62"/>
+    <mergeCell ref="C62:D62"/>
+    <mergeCell ref="A63:B63"/>
+    <mergeCell ref="C63:D63"/>
+    <mergeCell ref="A64:B64"/>
+    <mergeCell ref="C64:D64"/>
+    <mergeCell ref="A65:B65"/>
+    <mergeCell ref="C65:D65"/>
+    <mergeCell ref="A66:B66"/>
+    <mergeCell ref="C66:D66"/>
+    <mergeCell ref="A67:B67"/>
+    <mergeCell ref="C67:D67"/>
+    <mergeCell ref="A68:B68"/>
+    <mergeCell ref="C68:D68"/>
+    <mergeCell ref="A69:B69"/>
+    <mergeCell ref="C69:D69"/>
+    <mergeCell ref="A70:B70"/>
+    <mergeCell ref="C70:D70"/>
+    <mergeCell ref="A71:B71"/>
+    <mergeCell ref="C71:D71"/>
+    <mergeCell ref="A72:B72"/>
+    <mergeCell ref="C72:D72"/>
+    <mergeCell ref="A73:B73"/>
+    <mergeCell ref="C73:D73"/>
+    <mergeCell ref="A74:B74"/>
+    <mergeCell ref="C74:D74"/>
+    <mergeCell ref="A75:B75"/>
+    <mergeCell ref="C75:D75"/>
+    <mergeCell ref="A76:B76"/>
+    <mergeCell ref="C76:D76"/>
+    <mergeCell ref="A77:B77"/>
+    <mergeCell ref="C77:D77"/>
+    <mergeCell ref="A78:B78"/>
+    <mergeCell ref="C78:D78"/>
+    <mergeCell ref="A79:B79"/>
+    <mergeCell ref="C79:D79"/>
+    <mergeCell ref="A80:B80"/>
+    <mergeCell ref="C80:D80"/>
+    <mergeCell ref="A81:B81"/>
+    <mergeCell ref="C81:D81"/>
+    <mergeCell ref="A82:B82"/>
+    <mergeCell ref="C82:D82"/>
+    <mergeCell ref="A83:B83"/>
+    <mergeCell ref="C83:D83"/>
+    <mergeCell ref="A84:B84"/>
+    <mergeCell ref="C84:D84"/>
+    <mergeCell ref="A85:B85"/>
+    <mergeCell ref="C85:D85"/>
+    <mergeCell ref="A86:B86"/>
+    <mergeCell ref="C86:D86"/>
+    <mergeCell ref="A87:B87"/>
+    <mergeCell ref="C87:D87"/>
+    <mergeCell ref="A88:B88"/>
+    <mergeCell ref="C88:D88"/>
+    <mergeCell ref="A89:B89"/>
+    <mergeCell ref="C89:D89"/>
+    <mergeCell ref="A90:B90"/>
+    <mergeCell ref="C90:D90"/>
+    <mergeCell ref="A91:B91"/>
+    <mergeCell ref="C91:D91"/>
     <mergeCell ref="A97:B97"/>
     <mergeCell ref="C97:D97"/>
     <mergeCell ref="A98:B98"/>
@@ -7346,185 +7678,6 @@
     <mergeCell ref="C95:D95"/>
     <mergeCell ref="A96:B96"/>
     <mergeCell ref="C96:D96"/>
-    <mergeCell ref="A87:B87"/>
-    <mergeCell ref="C87:D87"/>
-    <mergeCell ref="A88:B88"/>
-    <mergeCell ref="C88:D88"/>
-    <mergeCell ref="A89:B89"/>
-    <mergeCell ref="C89:D89"/>
-    <mergeCell ref="A90:B90"/>
-    <mergeCell ref="C90:D90"/>
-    <mergeCell ref="A91:B91"/>
-    <mergeCell ref="C91:D91"/>
-    <mergeCell ref="A82:B82"/>
-    <mergeCell ref="C82:D82"/>
-    <mergeCell ref="A83:B83"/>
-    <mergeCell ref="C83:D83"/>
-    <mergeCell ref="A84:B84"/>
-    <mergeCell ref="C84:D84"/>
-    <mergeCell ref="A85:B85"/>
-    <mergeCell ref="C85:D85"/>
-    <mergeCell ref="A86:B86"/>
-    <mergeCell ref="C86:D86"/>
-    <mergeCell ref="A77:B77"/>
-    <mergeCell ref="C77:D77"/>
-    <mergeCell ref="A78:B78"/>
-    <mergeCell ref="C78:D78"/>
-    <mergeCell ref="A79:B79"/>
-    <mergeCell ref="C79:D79"/>
-    <mergeCell ref="A80:B80"/>
-    <mergeCell ref="C80:D80"/>
-    <mergeCell ref="A81:B81"/>
-    <mergeCell ref="C81:D81"/>
-    <mergeCell ref="A72:B72"/>
-    <mergeCell ref="C72:D72"/>
-    <mergeCell ref="A73:B73"/>
-    <mergeCell ref="C73:D73"/>
-    <mergeCell ref="A74:B74"/>
-    <mergeCell ref="C74:D74"/>
-    <mergeCell ref="A75:B75"/>
-    <mergeCell ref="C75:D75"/>
-    <mergeCell ref="A76:B76"/>
-    <mergeCell ref="C76:D76"/>
-    <mergeCell ref="A67:B67"/>
-    <mergeCell ref="C67:D67"/>
-    <mergeCell ref="A68:B68"/>
-    <mergeCell ref="C68:D68"/>
-    <mergeCell ref="A69:B69"/>
-    <mergeCell ref="C69:D69"/>
-    <mergeCell ref="A70:B70"/>
-    <mergeCell ref="C70:D70"/>
-    <mergeCell ref="A71:B71"/>
-    <mergeCell ref="C71:D71"/>
-    <mergeCell ref="A62:B62"/>
-    <mergeCell ref="C62:D62"/>
-    <mergeCell ref="A63:B63"/>
-    <mergeCell ref="C63:D63"/>
-    <mergeCell ref="A64:B64"/>
-    <mergeCell ref="C64:D64"/>
-    <mergeCell ref="A65:B65"/>
-    <mergeCell ref="C65:D65"/>
-    <mergeCell ref="A66:B66"/>
-    <mergeCell ref="C66:D66"/>
-    <mergeCell ref="A57:B57"/>
-    <mergeCell ref="C57:D57"/>
-    <mergeCell ref="A58:B58"/>
-    <mergeCell ref="C58:D58"/>
-    <mergeCell ref="A59:B59"/>
-    <mergeCell ref="C59:D59"/>
-    <mergeCell ref="A60:B60"/>
-    <mergeCell ref="C60:D60"/>
-    <mergeCell ref="A61:B61"/>
-    <mergeCell ref="C61:D61"/>
-    <mergeCell ref="A52:B52"/>
-    <mergeCell ref="C52:D52"/>
-    <mergeCell ref="A53:B53"/>
-    <mergeCell ref="C53:D53"/>
-    <mergeCell ref="A54:B54"/>
-    <mergeCell ref="C54:D54"/>
-    <mergeCell ref="A55:B55"/>
-    <mergeCell ref="C55:D55"/>
-    <mergeCell ref="A56:B56"/>
-    <mergeCell ref="C56:D56"/>
-    <mergeCell ref="A47:B47"/>
-    <mergeCell ref="C47:D47"/>
-    <mergeCell ref="A48:B48"/>
-    <mergeCell ref="C48:D48"/>
-    <mergeCell ref="A49:B49"/>
-    <mergeCell ref="C49:D49"/>
-    <mergeCell ref="A50:B50"/>
-    <mergeCell ref="C50:D50"/>
-    <mergeCell ref="A51:B51"/>
-    <mergeCell ref="C51:D51"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="C42:D42"/>
-    <mergeCell ref="A43:B43"/>
-    <mergeCell ref="C43:D43"/>
-    <mergeCell ref="A44:B44"/>
-    <mergeCell ref="C44:D44"/>
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="C45:D45"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="C46:D46"/>
-    <mergeCell ref="A37:B37"/>
-    <mergeCell ref="C37:D37"/>
-    <mergeCell ref="A38:B38"/>
-    <mergeCell ref="C38:D38"/>
-    <mergeCell ref="A39:B39"/>
-    <mergeCell ref="C39:D39"/>
-    <mergeCell ref="A40:B40"/>
-    <mergeCell ref="C40:D40"/>
-    <mergeCell ref="A41:B41"/>
-    <mergeCell ref="C41:D41"/>
-    <mergeCell ref="A32:B32"/>
-    <mergeCell ref="C32:D32"/>
-    <mergeCell ref="A33:B33"/>
-    <mergeCell ref="C33:D33"/>
-    <mergeCell ref="A34:B34"/>
-    <mergeCell ref="C34:D34"/>
-    <mergeCell ref="A35:B35"/>
-    <mergeCell ref="C35:D35"/>
-    <mergeCell ref="A36:B36"/>
-    <mergeCell ref="C36:D36"/>
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="A28:B28"/>
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="A29:B29"/>
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="A30:B30"/>
-    <mergeCell ref="C30:D30"/>
-    <mergeCell ref="A31:B31"/>
-    <mergeCell ref="C31:D31"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="A24:B24"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="C25:D25"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="C8:D8"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="C9:D9"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="C10:D10"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="A2:D2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="C6:D6"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="F3" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>

</xml_diff>

<commit_message>
alterações durante a aula
</commit_message>
<xml_diff>
--- a/Planilha de Monitoramento_Revisada_Luciene_Manhumirim.xlsx
+++ b/Planilha de Monitoramento_Revisada_Luciene_Manhumirim.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26924"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="45" documentId="11_2BF06DF04E5DE4C71D5F5451B3019729361D1167" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{714BD54E-7AAD-4F62-9565-7CF4CF0CBD34}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" tabRatio="475" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="OCORRÊNCIAS" sheetId="8" r:id="rId1"/>
@@ -1093,17 +1093,17 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hiperlink" xfId="1" builtinId="8"/>
@@ -1758,8 +1758,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:U1003"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="O14" sqref="O14"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75"/>
@@ -2202,7 +2202,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="8" spans="1:21">
+    <row r="8" spans="1:21" ht="25.5">
       <c r="A8" s="8" t="s">
         <v>55</v>
       </c>
@@ -6476,12 +6476,12 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:8" ht="13.5">
-      <c r="A2" s="26" t="s">
+      <c r="A2" s="23" t="s">
         <v>69</v>
       </c>
-      <c r="B2" s="27"/>
-      <c r="C2" s="27"/>
-      <c r="D2" s="24"/>
+      <c r="B2" s="24"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="25"/>
       <c r="F2" s="1" t="s">
         <v>70</v>
       </c>
@@ -6489,14 +6489,14 @@
       <c r="H2" s="1"/>
     </row>
     <row r="3" spans="1:8" ht="15">
-      <c r="A3" s="23" t="s">
+      <c r="A3" s="26" t="s">
         <v>71</v>
       </c>
-      <c r="B3" s="24"/>
-      <c r="C3" s="23" t="s">
+      <c r="B3" s="25"/>
+      <c r="C3" s="26" t="s">
         <v>72</v>
       </c>
-      <c r="D3" s="24"/>
+      <c r="D3" s="25"/>
       <c r="F3" s="2" t="s">
         <v>73</v>
       </c>
@@ -6504,1162 +6504,983 @@
       <c r="H3" s="1"/>
     </row>
     <row r="4" spans="1:8">
-      <c r="A4" s="23" t="s">
+      <c r="A4" s="26" t="s">
         <v>74</v>
       </c>
-      <c r="B4" s="24"/>
-      <c r="C4" s="23" t="s">
+      <c r="B4" s="25"/>
+      <c r="C4" s="26" t="s">
         <v>75</v>
       </c>
-      <c r="D4" s="24"/>
+      <c r="D4" s="25"/>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
     </row>
     <row r="5" spans="1:8">
-      <c r="A5" s="23" t="s">
+      <c r="A5" s="26" t="s">
         <v>76</v>
       </c>
-      <c r="B5" s="24"/>
-      <c r="C5" s="23" t="s">
+      <c r="B5" s="25"/>
+      <c r="C5" s="26" t="s">
         <v>77</v>
       </c>
-      <c r="D5" s="24"/>
+      <c r="D5" s="25"/>
       <c r="F5" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="6" spans="1:8">
-      <c r="A6" s="23" t="s">
+      <c r="A6" s="26" t="s">
         <v>79</v>
       </c>
-      <c r="B6" s="24"/>
-      <c r="C6" s="23" t="s">
+      <c r="B6" s="25"/>
+      <c r="C6" s="26" t="s">
         <v>80</v>
       </c>
-      <c r="D6" s="24"/>
+      <c r="D6" s="25"/>
     </row>
     <row r="7" spans="1:8">
-      <c r="A7" s="23" t="s">
+      <c r="A7" s="26" t="s">
         <v>81</v>
       </c>
-      <c r="B7" s="24"/>
-      <c r="C7" s="23" t="s">
+      <c r="B7" s="25"/>
+      <c r="C7" s="26" t="s">
         <v>82</v>
       </c>
-      <c r="D7" s="24"/>
+      <c r="D7" s="25"/>
     </row>
     <row r="8" spans="1:8">
-      <c r="A8" s="23" t="s">
+      <c r="A8" s="26" t="s">
         <v>83</v>
       </c>
-      <c r="B8" s="24"/>
-      <c r="C8" s="23" t="s">
+      <c r="B8" s="25"/>
+      <c r="C8" s="26" t="s">
         <v>84</v>
       </c>
-      <c r="D8" s="24"/>
+      <c r="D8" s="25"/>
     </row>
     <row r="9" spans="1:8">
-      <c r="A9" s="23" t="s">
+      <c r="A9" s="26" t="s">
         <v>85</v>
       </c>
-      <c r="B9" s="24"/>
-      <c r="C9" s="23" t="s">
+      <c r="B9" s="25"/>
+      <c r="C9" s="26" t="s">
         <v>86</v>
       </c>
-      <c r="D9" s="24"/>
+      <c r="D9" s="25"/>
     </row>
     <row r="10" spans="1:8">
-      <c r="A10" s="23" t="s">
+      <c r="A10" s="26" t="s">
         <v>87</v>
       </c>
-      <c r="B10" s="24"/>
-      <c r="C10" s="23" t="s">
+      <c r="B10" s="25"/>
+      <c r="C10" s="26" t="s">
         <v>88</v>
       </c>
-      <c r="D10" s="24"/>
+      <c r="D10" s="25"/>
     </row>
     <row r="11" spans="1:8">
-      <c r="A11" s="23" t="s">
+      <c r="A11" s="26" t="s">
         <v>89</v>
       </c>
-      <c r="B11" s="24"/>
-      <c r="C11" s="23" t="s">
+      <c r="B11" s="25"/>
+      <c r="C11" s="26" t="s">
         <v>90</v>
       </c>
-      <c r="D11" s="24"/>
+      <c r="D11" s="25"/>
     </row>
     <row r="12" spans="1:8">
-      <c r="A12" s="23" t="s">
+      <c r="A12" s="26" t="s">
         <v>91</v>
       </c>
-      <c r="B12" s="24"/>
-      <c r="C12" s="23" t="s">
+      <c r="B12" s="25"/>
+      <c r="C12" s="26" t="s">
         <v>92</v>
       </c>
-      <c r="D12" s="24"/>
+      <c r="D12" s="25"/>
     </row>
     <row r="13" spans="1:8">
-      <c r="A13" s="23" t="s">
+      <c r="A13" s="26" t="s">
         <v>93</v>
       </c>
-      <c r="B13" s="24"/>
-      <c r="C13" s="23" t="s">
+      <c r="B13" s="25"/>
+      <c r="C13" s="26" t="s">
         <v>94</v>
       </c>
-      <c r="D13" s="24"/>
+      <c r="D13" s="25"/>
     </row>
     <row r="14" spans="1:8">
-      <c r="A14" s="23" t="s">
+      <c r="A14" s="26" t="s">
         <v>95</v>
       </c>
-      <c r="B14" s="24"/>
-      <c r="C14" s="23" t="s">
+      <c r="B14" s="25"/>
+      <c r="C14" s="26" t="s">
         <v>96</v>
       </c>
-      <c r="D14" s="24"/>
+      <c r="D14" s="25"/>
     </row>
     <row r="15" spans="1:8">
-      <c r="A15" s="23" t="s">
+      <c r="A15" s="26" t="s">
         <v>97</v>
       </c>
-      <c r="B15" s="24"/>
-      <c r="C15" s="23" t="s">
+      <c r="B15" s="25"/>
+      <c r="C15" s="26" t="s">
         <v>98</v>
       </c>
-      <c r="D15" s="24"/>
+      <c r="D15" s="25"/>
     </row>
     <row r="16" spans="1:8">
-      <c r="A16" s="23" t="s">
+      <c r="A16" s="26" t="s">
         <v>99</v>
       </c>
-      <c r="B16" s="24"/>
-      <c r="C16" s="23" t="s">
+      <c r="B16" s="25"/>
+      <c r="C16" s="26" t="s">
         <v>100</v>
       </c>
-      <c r="D16" s="24"/>
+      <c r="D16" s="25"/>
     </row>
     <row r="17" spans="1:4">
-      <c r="A17" s="23" t="s">
+      <c r="A17" s="26" t="s">
         <v>101</v>
       </c>
-      <c r="B17" s="24"/>
-      <c r="C17" s="23" t="s">
+      <c r="B17" s="25"/>
+      <c r="C17" s="26" t="s">
         <v>102</v>
       </c>
-      <c r="D17" s="24"/>
+      <c r="D17" s="25"/>
     </row>
     <row r="18" spans="1:4">
-      <c r="A18" s="23" t="s">
+      <c r="A18" s="26" t="s">
         <v>103</v>
       </c>
-      <c r="B18" s="24"/>
-      <c r="C18" s="23" t="s">
+      <c r="B18" s="25"/>
+      <c r="C18" s="26" t="s">
         <v>104</v>
       </c>
-      <c r="D18" s="24"/>
+      <c r="D18" s="25"/>
     </row>
     <row r="19" spans="1:4">
-      <c r="A19" s="23" t="s">
+      <c r="A19" s="26" t="s">
         <v>105</v>
       </c>
-      <c r="B19" s="24"/>
-      <c r="C19" s="23" t="s">
+      <c r="B19" s="25"/>
+      <c r="C19" s="26" t="s">
         <v>106</v>
       </c>
-      <c r="D19" s="24"/>
+      <c r="D19" s="25"/>
     </row>
     <row r="20" spans="1:4">
-      <c r="A20" s="23" t="s">
+      <c r="A20" s="26" t="s">
         <v>107</v>
       </c>
-      <c r="B20" s="24"/>
-      <c r="C20" s="23" t="s">
+      <c r="B20" s="25"/>
+      <c r="C20" s="26" t="s">
         <v>108</v>
       </c>
-      <c r="D20" s="24"/>
+      <c r="D20" s="25"/>
     </row>
     <row r="21" spans="1:4">
-      <c r="A21" s="23" t="s">
+      <c r="A21" s="26" t="s">
         <v>109</v>
       </c>
-      <c r="B21" s="24"/>
-      <c r="C21" s="23" t="s">
+      <c r="B21" s="25"/>
+      <c r="C21" s="26" t="s">
         <v>110</v>
       </c>
-      <c r="D21" s="24"/>
+      <c r="D21" s="25"/>
     </row>
     <row r="22" spans="1:4">
-      <c r="A22" s="23" t="s">
+      <c r="A22" s="26" t="s">
         <v>111</v>
       </c>
-      <c r="B22" s="24"/>
-      <c r="C22" s="23" t="s">
+      <c r="B22" s="25"/>
+      <c r="C22" s="26" t="s">
         <v>112</v>
       </c>
-      <c r="D22" s="24"/>
+      <c r="D22" s="25"/>
     </row>
     <row r="23" spans="1:4">
-      <c r="A23" s="23" t="s">
+      <c r="A23" s="26" t="s">
         <v>113</v>
       </c>
-      <c r="B23" s="24"/>
-      <c r="C23" s="23" t="s">
+      <c r="B23" s="25"/>
+      <c r="C23" s="26" t="s">
         <v>114</v>
       </c>
-      <c r="D23" s="24"/>
+      <c r="D23" s="25"/>
     </row>
     <row r="24" spans="1:4">
-      <c r="A24" s="23" t="s">
+      <c r="A24" s="26" t="s">
         <v>115</v>
       </c>
-      <c r="B24" s="24"/>
-      <c r="C24" s="23" t="s">
+      <c r="B24" s="25"/>
+      <c r="C24" s="26" t="s">
         <v>116</v>
       </c>
-      <c r="D24" s="24"/>
+      <c r="D24" s="25"/>
     </row>
     <row r="25" spans="1:4">
-      <c r="A25" s="23" t="s">
+      <c r="A25" s="26" t="s">
         <v>117</v>
       </c>
-      <c r="B25" s="24"/>
-      <c r="C25" s="23" t="s">
+      <c r="B25" s="25"/>
+      <c r="C25" s="26" t="s">
         <v>118</v>
       </c>
-      <c r="D25" s="24"/>
+      <c r="D25" s="25"/>
     </row>
     <row r="26" spans="1:4">
-      <c r="A26" s="23" t="s">
+      <c r="A26" s="26" t="s">
         <v>119</v>
       </c>
-      <c r="B26" s="24"/>
-      <c r="C26" s="23" t="s">
+      <c r="B26" s="25"/>
+      <c r="C26" s="26" t="s">
         <v>120</v>
       </c>
-      <c r="D26" s="24"/>
+      <c r="D26" s="25"/>
     </row>
     <row r="27" spans="1:4">
-      <c r="A27" s="23" t="s">
+      <c r="A27" s="26" t="s">
         <v>121</v>
       </c>
-      <c r="B27" s="24"/>
-      <c r="C27" s="23" t="s">
+      <c r="B27" s="25"/>
+      <c r="C27" s="26" t="s">
         <v>122</v>
       </c>
-      <c r="D27" s="24"/>
+      <c r="D27" s="25"/>
     </row>
     <row r="28" spans="1:4">
-      <c r="A28" s="23" t="s">
+      <c r="A28" s="26" t="s">
         <v>123</v>
       </c>
-      <c r="B28" s="24"/>
-      <c r="C28" s="23" t="s">
+      <c r="B28" s="25"/>
+      <c r="C28" s="26" t="s">
         <v>124</v>
       </c>
-      <c r="D28" s="24"/>
+      <c r="D28" s="25"/>
     </row>
     <row r="29" spans="1:4">
-      <c r="A29" s="23" t="s">
+      <c r="A29" s="26" t="s">
         <v>125</v>
       </c>
-      <c r="B29" s="24"/>
-      <c r="C29" s="23" t="s">
+      <c r="B29" s="25"/>
+      <c r="C29" s="26" t="s">
         <v>126</v>
       </c>
-      <c r="D29" s="24"/>
+      <c r="D29" s="25"/>
     </row>
     <row r="30" spans="1:4">
-      <c r="A30" s="23" t="s">
+      <c r="A30" s="26" t="s">
         <v>127</v>
       </c>
-      <c r="B30" s="24"/>
-      <c r="C30" s="23" t="s">
+      <c r="B30" s="25"/>
+      <c r="C30" s="26" t="s">
         <v>128</v>
       </c>
-      <c r="D30" s="24"/>
+      <c r="D30" s="25"/>
     </row>
     <row r="31" spans="1:4">
-      <c r="A31" s="23" t="s">
+      <c r="A31" s="26" t="s">
         <v>129</v>
       </c>
-      <c r="B31" s="24"/>
-      <c r="C31" s="23" t="s">
+      <c r="B31" s="25"/>
+      <c r="C31" s="26" t="s">
         <v>130</v>
       </c>
-      <c r="D31" s="24"/>
+      <c r="D31" s="25"/>
     </row>
     <row r="32" spans="1:4">
-      <c r="A32" s="23" t="s">
+      <c r="A32" s="26" t="s">
         <v>131</v>
       </c>
-      <c r="B32" s="24"/>
-      <c r="C32" s="23" t="s">
+      <c r="B32" s="25"/>
+      <c r="C32" s="26" t="s">
         <v>132</v>
       </c>
-      <c r="D32" s="24"/>
+      <c r="D32" s="25"/>
     </row>
     <row r="33" spans="1:4">
-      <c r="A33" s="23" t="s">
+      <c r="A33" s="26" t="s">
         <v>133</v>
       </c>
-      <c r="B33" s="24"/>
-      <c r="C33" s="23" t="s">
+      <c r="B33" s="25"/>
+      <c r="C33" s="26" t="s">
         <v>134</v>
       </c>
-      <c r="D33" s="24"/>
+      <c r="D33" s="25"/>
     </row>
     <row r="34" spans="1:4">
-      <c r="A34" s="23" t="s">
+      <c r="A34" s="26" t="s">
         <v>135</v>
       </c>
-      <c r="B34" s="24"/>
-      <c r="C34" s="23" t="s">
+      <c r="B34" s="25"/>
+      <c r="C34" s="26" t="s">
         <v>136</v>
       </c>
-      <c r="D34" s="24"/>
+      <c r="D34" s="25"/>
     </row>
     <row r="35" spans="1:4">
-      <c r="A35" s="23" t="s">
+      <c r="A35" s="26" t="s">
         <v>137</v>
       </c>
-      <c r="B35" s="24"/>
-      <c r="C35" s="23" t="s">
+      <c r="B35" s="25"/>
+      <c r="C35" s="26" t="s">
         <v>138</v>
       </c>
-      <c r="D35" s="24"/>
+      <c r="D35" s="25"/>
     </row>
     <row r="36" spans="1:4">
-      <c r="A36" s="23" t="s">
+      <c r="A36" s="26" t="s">
         <v>139</v>
       </c>
-      <c r="B36" s="24"/>
-      <c r="C36" s="23" t="s">
+      <c r="B36" s="25"/>
+      <c r="C36" s="26" t="s">
         <v>140</v>
       </c>
-      <c r="D36" s="24"/>
+      <c r="D36" s="25"/>
     </row>
     <row r="37" spans="1:4">
-      <c r="A37" s="23" t="s">
+      <c r="A37" s="26" t="s">
         <v>141</v>
       </c>
-      <c r="B37" s="24"/>
-      <c r="C37" s="23" t="s">
+      <c r="B37" s="25"/>
+      <c r="C37" s="26" t="s">
         <v>142</v>
       </c>
-      <c r="D37" s="24"/>
+      <c r="D37" s="25"/>
     </row>
     <row r="38" spans="1:4">
-      <c r="A38" s="23" t="s">
+      <c r="A38" s="26" t="s">
         <v>143</v>
       </c>
-      <c r="B38" s="24"/>
-      <c r="C38" s="23" t="s">
+      <c r="B38" s="25"/>
+      <c r="C38" s="26" t="s">
         <v>144</v>
       </c>
-      <c r="D38" s="24"/>
+      <c r="D38" s="25"/>
     </row>
     <row r="39" spans="1:4">
-      <c r="A39" s="23" t="s">
+      <c r="A39" s="26" t="s">
         <v>145</v>
       </c>
-      <c r="B39" s="24"/>
-      <c r="C39" s="23" t="s">
+      <c r="B39" s="25"/>
+      <c r="C39" s="26" t="s">
         <v>146</v>
       </c>
-      <c r="D39" s="24"/>
+      <c r="D39" s="25"/>
     </row>
     <row r="40" spans="1:4">
-      <c r="A40" s="23" t="s">
+      <c r="A40" s="26" t="s">
         <v>147</v>
       </c>
-      <c r="B40" s="24"/>
-      <c r="C40" s="23" t="s">
+      <c r="B40" s="25"/>
+      <c r="C40" s="26" t="s">
         <v>148</v>
       </c>
-      <c r="D40" s="24"/>
+      <c r="D40" s="25"/>
     </row>
     <row r="41" spans="1:4">
-      <c r="A41" s="23" t="s">
+      <c r="A41" s="26" t="s">
         <v>149</v>
       </c>
-      <c r="B41" s="24"/>
-      <c r="C41" s="23" t="s">
+      <c r="B41" s="25"/>
+      <c r="C41" s="26" t="s">
         <v>150</v>
       </c>
-      <c r="D41" s="24"/>
+      <c r="D41" s="25"/>
     </row>
     <row r="42" spans="1:4">
-      <c r="A42" s="23" t="s">
+      <c r="A42" s="26" t="s">
         <v>151</v>
       </c>
-      <c r="B42" s="24"/>
-      <c r="C42" s="23" t="s">
+      <c r="B42" s="25"/>
+      <c r="C42" s="26" t="s">
         <v>152</v>
       </c>
-      <c r="D42" s="24"/>
+      <c r="D42" s="25"/>
     </row>
     <row r="43" spans="1:4">
-      <c r="A43" s="23" t="s">
+      <c r="A43" s="26" t="s">
         <v>153</v>
       </c>
-      <c r="B43" s="24"/>
-      <c r="C43" s="23" t="s">
+      <c r="B43" s="25"/>
+      <c r="C43" s="26" t="s">
         <v>154</v>
       </c>
-      <c r="D43" s="24"/>
+      <c r="D43" s="25"/>
     </row>
     <row r="44" spans="1:4">
-      <c r="A44" s="23" t="s">
+      <c r="A44" s="26" t="s">
         <v>155</v>
       </c>
-      <c r="B44" s="24"/>
-      <c r="C44" s="23" t="s">
+      <c r="B44" s="25"/>
+      <c r="C44" s="26" t="s">
         <v>156</v>
       </c>
-      <c r="D44" s="24"/>
+      <c r="D44" s="25"/>
     </row>
     <row r="45" spans="1:4">
-      <c r="A45" s="23" t="s">
+      <c r="A45" s="26" t="s">
         <v>157</v>
       </c>
-      <c r="B45" s="24"/>
-      <c r="C45" s="23" t="s">
+      <c r="B45" s="25"/>
+      <c r="C45" s="26" t="s">
         <v>158</v>
       </c>
-      <c r="D45" s="24"/>
+      <c r="D45" s="25"/>
     </row>
     <row r="46" spans="1:4">
-      <c r="A46" s="23" t="s">
+      <c r="A46" s="26" t="s">
         <v>159</v>
       </c>
-      <c r="B46" s="24"/>
-      <c r="C46" s="23" t="s">
+      <c r="B46" s="25"/>
+      <c r="C46" s="26" t="s">
         <v>160</v>
       </c>
-      <c r="D46" s="24"/>
+      <c r="D46" s="25"/>
     </row>
     <row r="47" spans="1:4">
-      <c r="A47" s="23" t="s">
+      <c r="A47" s="26" t="s">
         <v>161</v>
       </c>
-      <c r="B47" s="24"/>
-      <c r="C47" s="23" t="s">
+      <c r="B47" s="25"/>
+      <c r="C47" s="26" t="s">
         <v>162</v>
       </c>
-      <c r="D47" s="24"/>
+      <c r="D47" s="25"/>
     </row>
     <row r="48" spans="1:4">
-      <c r="A48" s="23" t="s">
+      <c r="A48" s="26" t="s">
         <v>163</v>
       </c>
-      <c r="B48" s="24"/>
-      <c r="C48" s="23" t="s">
+      <c r="B48" s="25"/>
+      <c r="C48" s="26" t="s">
         <v>164</v>
       </c>
-      <c r="D48" s="24"/>
+      <c r="D48" s="25"/>
     </row>
     <row r="49" spans="1:4">
-      <c r="A49" s="23" t="s">
+      <c r="A49" s="26" t="s">
         <v>165</v>
       </c>
-      <c r="B49" s="24"/>
-      <c r="C49" s="23" t="s">
+      <c r="B49" s="25"/>
+      <c r="C49" s="26" t="s">
         <v>166</v>
       </c>
-      <c r="D49" s="24"/>
+      <c r="D49" s="25"/>
     </row>
     <row r="50" spans="1:4">
-      <c r="A50" s="23" t="s">
+      <c r="A50" s="26" t="s">
         <v>167</v>
       </c>
-      <c r="B50" s="24"/>
-      <c r="C50" s="23" t="s">
+      <c r="B50" s="25"/>
+      <c r="C50" s="26" t="s">
         <v>168</v>
       </c>
-      <c r="D50" s="24"/>
+      <c r="D50" s="25"/>
     </row>
     <row r="51" spans="1:4">
-      <c r="A51" s="23" t="s">
+      <c r="A51" s="26" t="s">
         <v>169</v>
       </c>
-      <c r="B51" s="24"/>
-      <c r="C51" s="23" t="s">
+      <c r="B51" s="25"/>
+      <c r="C51" s="26" t="s">
         <v>170</v>
       </c>
-      <c r="D51" s="24"/>
+      <c r="D51" s="25"/>
     </row>
     <row r="52" spans="1:4">
-      <c r="A52" s="23" t="s">
+      <c r="A52" s="26" t="s">
         <v>171</v>
       </c>
-      <c r="B52" s="24"/>
-      <c r="C52" s="23" t="s">
+      <c r="B52" s="25"/>
+      <c r="C52" s="26" t="s">
         <v>172</v>
       </c>
-      <c r="D52" s="24"/>
+      <c r="D52" s="25"/>
     </row>
     <row r="53" spans="1:4">
-      <c r="A53" s="23" t="s">
+      <c r="A53" s="26" t="s">
         <v>173</v>
       </c>
-      <c r="B53" s="24"/>
-      <c r="C53" s="23" t="s">
+      <c r="B53" s="25"/>
+      <c r="C53" s="26" t="s">
         <v>174</v>
       </c>
-      <c r="D53" s="24"/>
+      <c r="D53" s="25"/>
     </row>
     <row r="54" spans="1:4">
-      <c r="A54" s="23" t="s">
+      <c r="A54" s="26" t="s">
         <v>175</v>
       </c>
-      <c r="B54" s="24"/>
-      <c r="C54" s="23" t="s">
+      <c r="B54" s="25"/>
+      <c r="C54" s="26" t="s">
         <v>176</v>
       </c>
-      <c r="D54" s="24"/>
+      <c r="D54" s="25"/>
     </row>
     <row r="55" spans="1:4">
-      <c r="A55" s="23" t="s">
+      <c r="A55" s="26" t="s">
         <v>177</v>
       </c>
-      <c r="B55" s="24"/>
-      <c r="C55" s="23" t="s">
+      <c r="B55" s="25"/>
+      <c r="C55" s="26" t="s">
         <v>178</v>
       </c>
-      <c r="D55" s="24"/>
+      <c r="D55" s="25"/>
     </row>
     <row r="56" spans="1:4">
-      <c r="A56" s="23" t="s">
+      <c r="A56" s="26" t="s">
         <v>179</v>
       </c>
-      <c r="B56" s="24"/>
-      <c r="C56" s="23" t="s">
+      <c r="B56" s="25"/>
+      <c r="C56" s="26" t="s">
         <v>180</v>
       </c>
-      <c r="D56" s="24"/>
+      <c r="D56" s="25"/>
     </row>
     <row r="57" spans="1:4">
-      <c r="A57" s="23" t="s">
+      <c r="A57" s="26" t="s">
         <v>181</v>
       </c>
-      <c r="B57" s="24"/>
-      <c r="C57" s="23" t="s">
+      <c r="B57" s="25"/>
+      <c r="C57" s="26" t="s">
         <v>182</v>
       </c>
-      <c r="D57" s="24"/>
+      <c r="D57" s="25"/>
     </row>
     <row r="58" spans="1:4">
-      <c r="A58" s="23" t="s">
+      <c r="A58" s="26" t="s">
         <v>183</v>
       </c>
-      <c r="B58" s="24"/>
-      <c r="C58" s="23" t="s">
+      <c r="B58" s="25"/>
+      <c r="C58" s="26" t="s">
         <v>184</v>
       </c>
-      <c r="D58" s="24"/>
+      <c r="D58" s="25"/>
     </row>
     <row r="59" spans="1:4">
-      <c r="A59" s="23" t="s">
+      <c r="A59" s="26" t="s">
         <v>185</v>
       </c>
-      <c r="B59" s="24"/>
-      <c r="C59" s="23" t="s">
+      <c r="B59" s="25"/>
+      <c r="C59" s="26" t="s">
         <v>150</v>
       </c>
-      <c r="D59" s="24"/>
+      <c r="D59" s="25"/>
     </row>
     <row r="60" spans="1:4">
-      <c r="A60" s="23" t="s">
+      <c r="A60" s="26" t="s">
         <v>186</v>
       </c>
-      <c r="B60" s="24"/>
-      <c r="C60" s="23" t="s">
+      <c r="B60" s="25"/>
+      <c r="C60" s="26" t="s">
         <v>187</v>
       </c>
-      <c r="D60" s="24"/>
+      <c r="D60" s="25"/>
     </row>
     <row r="61" spans="1:4">
-      <c r="A61" s="23" t="s">
+      <c r="A61" s="26" t="s">
         <v>188</v>
       </c>
-      <c r="B61" s="24"/>
-      <c r="C61" s="23" t="s">
+      <c r="B61" s="25"/>
+      <c r="C61" s="26" t="s">
         <v>189</v>
       </c>
-      <c r="D61" s="24"/>
+      <c r="D61" s="25"/>
     </row>
     <row r="62" spans="1:4">
-      <c r="A62" s="23" t="s">
+      <c r="A62" s="26" t="s">
         <v>190</v>
       </c>
-      <c r="B62" s="24"/>
-      <c r="C62" s="23" t="s">
+      <c r="B62" s="25"/>
+      <c r="C62" s="26" t="s">
         <v>191</v>
       </c>
-      <c r="D62" s="24"/>
+      <c r="D62" s="25"/>
     </row>
     <row r="63" spans="1:4">
-      <c r="A63" s="23" t="s">
+      <c r="A63" s="26" t="s">
         <v>192</v>
       </c>
-      <c r="B63" s="24"/>
-      <c r="C63" s="23" t="s">
+      <c r="B63" s="25"/>
+      <c r="C63" s="26" t="s">
         <v>193</v>
       </c>
-      <c r="D63" s="24"/>
+      <c r="D63" s="25"/>
     </row>
     <row r="64" spans="1:4">
-      <c r="A64" s="23" t="s">
+      <c r="A64" s="26" t="s">
         <v>194</v>
       </c>
-      <c r="B64" s="24"/>
-      <c r="C64" s="23" t="s">
+      <c r="B64" s="25"/>
+      <c r="C64" s="26" t="s">
         <v>195</v>
       </c>
-      <c r="D64" s="24"/>
+      <c r="D64" s="25"/>
     </row>
     <row r="65" spans="1:4">
-      <c r="A65" s="23" t="s">
+      <c r="A65" s="26" t="s">
         <v>196</v>
       </c>
-      <c r="B65" s="24"/>
-      <c r="C65" s="23" t="s">
+      <c r="B65" s="25"/>
+      <c r="C65" s="26" t="s">
         <v>197</v>
       </c>
-      <c r="D65" s="24"/>
+      <c r="D65" s="25"/>
     </row>
     <row r="66" spans="1:4">
-      <c r="A66" s="23" t="s">
+      <c r="A66" s="26" t="s">
         <v>198</v>
       </c>
-      <c r="B66" s="24"/>
-      <c r="C66" s="23" t="s">
+      <c r="B66" s="25"/>
+      <c r="C66" s="26" t="s">
         <v>199</v>
       </c>
-      <c r="D66" s="24"/>
+      <c r="D66" s="25"/>
     </row>
     <row r="67" spans="1:4">
-      <c r="A67" s="23" t="s">
+      <c r="A67" s="26" t="s">
         <v>200</v>
       </c>
-      <c r="B67" s="24"/>
-      <c r="C67" s="23" t="s">
+      <c r="B67" s="25"/>
+      <c r="C67" s="26" t="s">
         <v>201</v>
       </c>
-      <c r="D67" s="24"/>
+      <c r="D67" s="25"/>
     </row>
     <row r="68" spans="1:4">
-      <c r="A68" s="23" t="s">
+      <c r="A68" s="26" t="s">
         <v>202</v>
       </c>
-      <c r="B68" s="24"/>
-      <c r="C68" s="23" t="s">
+      <c r="B68" s="25"/>
+      <c r="C68" s="26" t="s">
         <v>203</v>
       </c>
-      <c r="D68" s="24"/>
+      <c r="D68" s="25"/>
     </row>
     <row r="69" spans="1:4">
-      <c r="A69" s="23" t="s">
+      <c r="A69" s="26" t="s">
         <v>204</v>
       </c>
-      <c r="B69" s="24"/>
-      <c r="C69" s="23" t="s">
+      <c r="B69" s="25"/>
+      <c r="C69" s="26" t="s">
         <v>205</v>
       </c>
-      <c r="D69" s="24"/>
+      <c r="D69" s="25"/>
     </row>
     <row r="70" spans="1:4">
-      <c r="A70" s="23" t="s">
+      <c r="A70" s="26" t="s">
         <v>206</v>
       </c>
-      <c r="B70" s="24"/>
-      <c r="C70" s="23" t="s">
+      <c r="B70" s="25"/>
+      <c r="C70" s="26" t="s">
         <v>207</v>
       </c>
-      <c r="D70" s="24"/>
+      <c r="D70" s="25"/>
     </row>
     <row r="71" spans="1:4">
-      <c r="A71" s="25" t="s">
+      <c r="A71" s="27" t="s">
         <v>208</v>
       </c>
-      <c r="B71" s="24"/>
-      <c r="C71" s="23" t="s">
+      <c r="B71" s="25"/>
+      <c r="C71" s="26" t="s">
         <v>209</v>
       </c>
-      <c r="D71" s="24"/>
+      <c r="D71" s="25"/>
     </row>
     <row r="72" spans="1:4">
-      <c r="A72" s="23" t="s">
+      <c r="A72" s="26" t="s">
         <v>210</v>
       </c>
-      <c r="B72" s="24"/>
-      <c r="C72" s="23" t="s">
+      <c r="B72" s="25"/>
+      <c r="C72" s="26" t="s">
         <v>211</v>
       </c>
-      <c r="D72" s="24"/>
+      <c r="D72" s="25"/>
     </row>
     <row r="73" spans="1:4">
-      <c r="A73" s="23" t="s">
+      <c r="A73" s="26" t="s">
         <v>212</v>
       </c>
-      <c r="B73" s="24"/>
-      <c r="C73" s="23" t="s">
+      <c r="B73" s="25"/>
+      <c r="C73" s="26" t="s">
         <v>213</v>
       </c>
-      <c r="D73" s="24"/>
+      <c r="D73" s="25"/>
     </row>
     <row r="74" spans="1:4">
-      <c r="A74" s="23" t="s">
+      <c r="A74" s="26" t="s">
         <v>214</v>
       </c>
-      <c r="B74" s="24"/>
-      <c r="C74" s="23" t="s">
+      <c r="B74" s="25"/>
+      <c r="C74" s="26" t="s">
         <v>215</v>
       </c>
-      <c r="D74" s="24"/>
+      <c r="D74" s="25"/>
     </row>
     <row r="75" spans="1:4">
-      <c r="A75" s="23" t="s">
+      <c r="A75" s="26" t="s">
         <v>216</v>
       </c>
-      <c r="B75" s="24"/>
-      <c r="C75" s="23" t="s">
+      <c r="B75" s="25"/>
+      <c r="C75" s="26" t="s">
         <v>217</v>
       </c>
-      <c r="D75" s="24"/>
+      <c r="D75" s="25"/>
     </row>
     <row r="76" spans="1:4">
-      <c r="A76" s="23" t="s">
+      <c r="A76" s="26" t="s">
         <v>218</v>
       </c>
-      <c r="B76" s="24"/>
-      <c r="C76" s="23" t="s">
+      <c r="B76" s="25"/>
+      <c r="C76" s="26" t="s">
         <v>219</v>
       </c>
-      <c r="D76" s="24"/>
+      <c r="D76" s="25"/>
     </row>
     <row r="77" spans="1:4">
-      <c r="A77" s="23" t="s">
+      <c r="A77" s="26" t="s">
         <v>220</v>
       </c>
-      <c r="B77" s="24"/>
-      <c r="C77" s="23" t="s">
+      <c r="B77" s="25"/>
+      <c r="C77" s="26" t="s">
         <v>221</v>
       </c>
-      <c r="D77" s="24"/>
+      <c r="D77" s="25"/>
     </row>
     <row r="78" spans="1:4">
-      <c r="A78" s="23" t="s">
+      <c r="A78" s="26" t="s">
         <v>222</v>
       </c>
-      <c r="B78" s="24"/>
-      <c r="C78" s="23" t="s">
+      <c r="B78" s="25"/>
+      <c r="C78" s="26" t="s">
         <v>223</v>
       </c>
-      <c r="D78" s="24"/>
+      <c r="D78" s="25"/>
     </row>
     <row r="79" spans="1:4">
-      <c r="A79" s="23" t="s">
+      <c r="A79" s="26" t="s">
         <v>224</v>
       </c>
-      <c r="B79" s="24"/>
-      <c r="C79" s="23" t="s">
+      <c r="B79" s="25"/>
+      <c r="C79" s="26" t="s">
         <v>225</v>
       </c>
-      <c r="D79" s="24"/>
+      <c r="D79" s="25"/>
     </row>
     <row r="80" spans="1:4">
-      <c r="A80" s="23" t="s">
+      <c r="A80" s="26" t="s">
         <v>226</v>
       </c>
-      <c r="B80" s="24"/>
-      <c r="C80" s="23" t="s">
+      <c r="B80" s="25"/>
+      <c r="C80" s="26" t="s">
         <v>227</v>
       </c>
-      <c r="D80" s="24"/>
+      <c r="D80" s="25"/>
     </row>
     <row r="81" spans="1:4">
-      <c r="A81" s="23" t="s">
+      <c r="A81" s="26" t="s">
         <v>228</v>
       </c>
-      <c r="B81" s="24"/>
-      <c r="C81" s="23" t="s">
+      <c r="B81" s="25"/>
+      <c r="C81" s="26" t="s">
         <v>229</v>
       </c>
-      <c r="D81" s="24"/>
+      <c r="D81" s="25"/>
     </row>
     <row r="82" spans="1:4">
-      <c r="A82" s="23" t="s">
+      <c r="A82" s="26" t="s">
         <v>230</v>
       </c>
-      <c r="B82" s="24"/>
-      <c r="C82" s="23" t="s">
+      <c r="B82" s="25"/>
+      <c r="C82" s="26" t="s">
         <v>231</v>
       </c>
-      <c r="D82" s="24"/>
+      <c r="D82" s="25"/>
     </row>
     <row r="83" spans="1:4">
-      <c r="A83" s="23" t="s">
+      <c r="A83" s="26" t="s">
         <v>232</v>
       </c>
-      <c r="B83" s="24"/>
-      <c r="C83" s="23" t="s">
+      <c r="B83" s="25"/>
+      <c r="C83" s="26" t="s">
         <v>233</v>
       </c>
-      <c r="D83" s="24"/>
+      <c r="D83" s="25"/>
     </row>
     <row r="84" spans="1:4">
-      <c r="A84" s="23" t="s">
+      <c r="A84" s="26" t="s">
         <v>234</v>
       </c>
-      <c r="B84" s="24"/>
-      <c r="C84" s="23" t="s">
+      <c r="B84" s="25"/>
+      <c r="C84" s="26" t="s">
         <v>235</v>
       </c>
-      <c r="D84" s="24"/>
+      <c r="D84" s="25"/>
     </row>
     <row r="85" spans="1:4">
-      <c r="A85" s="23" t="s">
+      <c r="A85" s="26" t="s">
         <v>236</v>
       </c>
-      <c r="B85" s="24"/>
-      <c r="C85" s="23" t="s">
+      <c r="B85" s="25"/>
+      <c r="C85" s="26" t="s">
         <v>237</v>
       </c>
-      <c r="D85" s="24"/>
+      <c r="D85" s="25"/>
     </row>
     <row r="86" spans="1:4">
-      <c r="A86" s="23" t="s">
+      <c r="A86" s="26" t="s">
         <v>238</v>
       </c>
-      <c r="B86" s="24"/>
-      <c r="C86" s="23" t="s">
+      <c r="B86" s="25"/>
+      <c r="C86" s="26" t="s">
         <v>239</v>
       </c>
-      <c r="D86" s="24"/>
+      <c r="D86" s="25"/>
     </row>
     <row r="87" spans="1:4">
-      <c r="A87" s="23" t="s">
+      <c r="A87" s="26" t="s">
         <v>240</v>
       </c>
-      <c r="B87" s="24"/>
-      <c r="C87" s="23" t="s">
+      <c r="B87" s="25"/>
+      <c r="C87" s="26" t="s">
         <v>241</v>
       </c>
-      <c r="D87" s="24"/>
+      <c r="D87" s="25"/>
     </row>
     <row r="88" spans="1:4">
-      <c r="A88" s="23" t="s">
+      <c r="A88" s="26" t="s">
         <v>242</v>
       </c>
-      <c r="B88" s="24"/>
-      <c r="C88" s="23" t="s">
+      <c r="B88" s="25"/>
+      <c r="C88" s="26" t="s">
         <v>243</v>
       </c>
-      <c r="D88" s="24"/>
+      <c r="D88" s="25"/>
     </row>
     <row r="89" spans="1:4">
-      <c r="A89" s="23" t="s">
+      <c r="A89" s="26" t="s">
         <v>244</v>
       </c>
-      <c r="B89" s="24"/>
-      <c r="C89" s="23" t="s">
+      <c r="B89" s="25"/>
+      <c r="C89" s="26" t="s">
         <v>245</v>
       </c>
-      <c r="D89" s="24"/>
+      <c r="D89" s="25"/>
     </row>
     <row r="90" spans="1:4">
-      <c r="A90" s="23" t="s">
+      <c r="A90" s="26" t="s">
         <v>246</v>
       </c>
-      <c r="B90" s="24"/>
-      <c r="C90" s="23" t="s">
+      <c r="B90" s="25"/>
+      <c r="C90" s="26" t="s">
         <v>247</v>
       </c>
-      <c r="D90" s="24"/>
+      <c r="D90" s="25"/>
     </row>
     <row r="91" spans="1:4">
-      <c r="A91" s="23" t="s">
+      <c r="A91" s="26" t="s">
         <v>248</v>
       </c>
-      <c r="B91" s="24"/>
-      <c r="C91" s="23" t="s">
+      <c r="B91" s="25"/>
+      <c r="C91" s="26" t="s">
         <v>249</v>
       </c>
-      <c r="D91" s="24"/>
+      <c r="D91" s="25"/>
     </row>
     <row r="92" spans="1:4">
-      <c r="A92" s="23" t="s">
+      <c r="A92" s="26" t="s">
         <v>250</v>
       </c>
-      <c r="B92" s="24"/>
-      <c r="C92" s="23" t="s">
+      <c r="B92" s="25"/>
+      <c r="C92" s="26" t="s">
         <v>251</v>
       </c>
-      <c r="D92" s="24"/>
+      <c r="D92" s="25"/>
     </row>
     <row r="93" spans="1:4">
-      <c r="A93" s="23" t="s">
+      <c r="A93" s="26" t="s">
         <v>252</v>
       </c>
-      <c r="B93" s="24"/>
-      <c r="C93" s="23" t="s">
+      <c r="B93" s="25"/>
+      <c r="C93" s="26" t="s">
         <v>253</v>
       </c>
-      <c r="D93" s="24"/>
+      <c r="D93" s="25"/>
     </row>
     <row r="94" spans="1:4">
-      <c r="A94" s="23" t="s">
+      <c r="A94" s="26" t="s">
         <v>254</v>
       </c>
-      <c r="B94" s="24"/>
-      <c r="C94" s="23" t="s">
+      <c r="B94" s="25"/>
+      <c r="C94" s="26" t="s">
         <v>255</v>
       </c>
-      <c r="D94" s="24"/>
+      <c r="D94" s="25"/>
     </row>
     <row r="95" spans="1:4">
-      <c r="A95" s="23" t="s">
+      <c r="A95" s="26" t="s">
         <v>256</v>
       </c>
-      <c r="B95" s="24"/>
-      <c r="C95" s="23" t="s">
+      <c r="B95" s="25"/>
+      <c r="C95" s="26" t="s">
         <v>257</v>
       </c>
-      <c r="D95" s="24"/>
+      <c r="D95" s="25"/>
     </row>
     <row r="96" spans="1:4">
-      <c r="A96" s="23" t="s">
+      <c r="A96" s="26" t="s">
         <v>258</v>
       </c>
-      <c r="B96" s="24"/>
-      <c r="C96" s="23" t="s">
+      <c r="B96" s="25"/>
+      <c r="C96" s="26" t="s">
         <v>259</v>
       </c>
-      <c r="D96" s="24"/>
+      <c r="D96" s="25"/>
     </row>
     <row r="97" spans="1:4">
-      <c r="A97" s="23" t="s">
+      <c r="A97" s="26" t="s">
         <v>260</v>
       </c>
-      <c r="B97" s="24"/>
-      <c r="C97" s="23" t="s">
+      <c r="B97" s="25"/>
+      <c r="C97" s="26" t="s">
         <v>261</v>
       </c>
-      <c r="D97" s="24"/>
+      <c r="D97" s="25"/>
     </row>
     <row r="98" spans="1:4">
-      <c r="A98" s="23" t="s">
+      <c r="A98" s="26" t="s">
         <v>262</v>
       </c>
-      <c r="B98" s="24"/>
-      <c r="C98" s="23" t="s">
+      <c r="B98" s="25"/>
+      <c r="C98" s="26" t="s">
         <v>263</v>
       </c>
-      <c r="D98" s="24"/>
+      <c r="D98" s="25"/>
     </row>
     <row r="99" spans="1:4">
-      <c r="A99" s="23" t="s">
+      <c r="A99" s="26" t="s">
         <v>264</v>
       </c>
-      <c r="B99" s="24"/>
-      <c r="C99" s="23" t="s">
+      <c r="B99" s="25"/>
+      <c r="C99" s="26" t="s">
         <v>265</v>
       </c>
-      <c r="D99" s="24"/>
+      <c r="D99" s="25"/>
     </row>
     <row r="100" spans="1:4">
-      <c r="A100" s="23" t="s">
+      <c r="A100" s="26" t="s">
         <v>266</v>
       </c>
-      <c r="B100" s="24"/>
-      <c r="C100" s="23" t="s">
+      <c r="B100" s="25"/>
+      <c r="C100" s="26" t="s">
         <v>267</v>
       </c>
-      <c r="D100" s="24"/>
+      <c r="D100" s="25"/>
     </row>
   </sheetData>
   <mergeCells count="197">
-    <mergeCell ref="A2:D2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="C8:D8"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="C9:D9"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="C10:D10"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="A24:B24"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="C25:D25"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="A28:B28"/>
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="A29:B29"/>
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="A30:B30"/>
-    <mergeCell ref="C30:D30"/>
-    <mergeCell ref="A31:B31"/>
-    <mergeCell ref="C31:D31"/>
-    <mergeCell ref="A32:B32"/>
-    <mergeCell ref="C32:D32"/>
-    <mergeCell ref="A33:B33"/>
-    <mergeCell ref="C33:D33"/>
-    <mergeCell ref="A34:B34"/>
-    <mergeCell ref="C34:D34"/>
-    <mergeCell ref="A35:B35"/>
-    <mergeCell ref="C35:D35"/>
-    <mergeCell ref="A36:B36"/>
-    <mergeCell ref="C36:D36"/>
-    <mergeCell ref="A37:B37"/>
-    <mergeCell ref="C37:D37"/>
-    <mergeCell ref="A38:B38"/>
-    <mergeCell ref="C38:D38"/>
-    <mergeCell ref="A39:B39"/>
-    <mergeCell ref="C39:D39"/>
-    <mergeCell ref="A40:B40"/>
-    <mergeCell ref="C40:D40"/>
-    <mergeCell ref="A41:B41"/>
-    <mergeCell ref="C41:D41"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="C42:D42"/>
-    <mergeCell ref="A43:B43"/>
-    <mergeCell ref="C43:D43"/>
-    <mergeCell ref="A44:B44"/>
-    <mergeCell ref="C44:D44"/>
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="C45:D45"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="C46:D46"/>
-    <mergeCell ref="A47:B47"/>
-    <mergeCell ref="C47:D47"/>
-    <mergeCell ref="A48:B48"/>
-    <mergeCell ref="C48:D48"/>
-    <mergeCell ref="A49:B49"/>
-    <mergeCell ref="C49:D49"/>
-    <mergeCell ref="A50:B50"/>
-    <mergeCell ref="C50:D50"/>
-    <mergeCell ref="A51:B51"/>
-    <mergeCell ref="C51:D51"/>
-    <mergeCell ref="A52:B52"/>
-    <mergeCell ref="C52:D52"/>
-    <mergeCell ref="A53:B53"/>
-    <mergeCell ref="C53:D53"/>
-    <mergeCell ref="A54:B54"/>
-    <mergeCell ref="C54:D54"/>
-    <mergeCell ref="A55:B55"/>
-    <mergeCell ref="C55:D55"/>
-    <mergeCell ref="A56:B56"/>
-    <mergeCell ref="C56:D56"/>
-    <mergeCell ref="A57:B57"/>
-    <mergeCell ref="C57:D57"/>
-    <mergeCell ref="A58:B58"/>
-    <mergeCell ref="C58:D58"/>
-    <mergeCell ref="A59:B59"/>
-    <mergeCell ref="C59:D59"/>
-    <mergeCell ref="A60:B60"/>
-    <mergeCell ref="C60:D60"/>
-    <mergeCell ref="A61:B61"/>
-    <mergeCell ref="C61:D61"/>
-    <mergeCell ref="A62:B62"/>
-    <mergeCell ref="C62:D62"/>
-    <mergeCell ref="A63:B63"/>
-    <mergeCell ref="C63:D63"/>
-    <mergeCell ref="A64:B64"/>
-    <mergeCell ref="C64:D64"/>
-    <mergeCell ref="A65:B65"/>
-    <mergeCell ref="C65:D65"/>
-    <mergeCell ref="A66:B66"/>
-    <mergeCell ref="C66:D66"/>
-    <mergeCell ref="A67:B67"/>
-    <mergeCell ref="C67:D67"/>
-    <mergeCell ref="A68:B68"/>
-    <mergeCell ref="C68:D68"/>
-    <mergeCell ref="A69:B69"/>
-    <mergeCell ref="C69:D69"/>
-    <mergeCell ref="A70:B70"/>
-    <mergeCell ref="C70:D70"/>
-    <mergeCell ref="A71:B71"/>
-    <mergeCell ref="C71:D71"/>
-    <mergeCell ref="A72:B72"/>
-    <mergeCell ref="C72:D72"/>
-    <mergeCell ref="A73:B73"/>
-    <mergeCell ref="C73:D73"/>
-    <mergeCell ref="A74:B74"/>
-    <mergeCell ref="C74:D74"/>
-    <mergeCell ref="A75:B75"/>
-    <mergeCell ref="C75:D75"/>
-    <mergeCell ref="A76:B76"/>
-    <mergeCell ref="C76:D76"/>
-    <mergeCell ref="A77:B77"/>
-    <mergeCell ref="C77:D77"/>
-    <mergeCell ref="A78:B78"/>
-    <mergeCell ref="C78:D78"/>
-    <mergeCell ref="A79:B79"/>
-    <mergeCell ref="C79:D79"/>
-    <mergeCell ref="A80:B80"/>
-    <mergeCell ref="C80:D80"/>
-    <mergeCell ref="A81:B81"/>
-    <mergeCell ref="C81:D81"/>
-    <mergeCell ref="A82:B82"/>
-    <mergeCell ref="C82:D82"/>
-    <mergeCell ref="A83:B83"/>
-    <mergeCell ref="C83:D83"/>
-    <mergeCell ref="A84:B84"/>
-    <mergeCell ref="C84:D84"/>
-    <mergeCell ref="A85:B85"/>
-    <mergeCell ref="C85:D85"/>
-    <mergeCell ref="A86:B86"/>
-    <mergeCell ref="C86:D86"/>
-    <mergeCell ref="A87:B87"/>
-    <mergeCell ref="C87:D87"/>
-    <mergeCell ref="A88:B88"/>
-    <mergeCell ref="C88:D88"/>
-    <mergeCell ref="A89:B89"/>
-    <mergeCell ref="C89:D89"/>
-    <mergeCell ref="A90:B90"/>
-    <mergeCell ref="C90:D90"/>
-    <mergeCell ref="A91:B91"/>
-    <mergeCell ref="C91:D91"/>
     <mergeCell ref="A97:B97"/>
     <mergeCell ref="C97:D97"/>
     <mergeCell ref="A98:B98"/>
@@ -7678,6 +7499,185 @@
     <mergeCell ref="C95:D95"/>
     <mergeCell ref="A96:B96"/>
     <mergeCell ref="C96:D96"/>
+    <mergeCell ref="A87:B87"/>
+    <mergeCell ref="C87:D87"/>
+    <mergeCell ref="A88:B88"/>
+    <mergeCell ref="C88:D88"/>
+    <mergeCell ref="A89:B89"/>
+    <mergeCell ref="C89:D89"/>
+    <mergeCell ref="A90:B90"/>
+    <mergeCell ref="C90:D90"/>
+    <mergeCell ref="A91:B91"/>
+    <mergeCell ref="C91:D91"/>
+    <mergeCell ref="A82:B82"/>
+    <mergeCell ref="C82:D82"/>
+    <mergeCell ref="A83:B83"/>
+    <mergeCell ref="C83:D83"/>
+    <mergeCell ref="A84:B84"/>
+    <mergeCell ref="C84:D84"/>
+    <mergeCell ref="A85:B85"/>
+    <mergeCell ref="C85:D85"/>
+    <mergeCell ref="A86:B86"/>
+    <mergeCell ref="C86:D86"/>
+    <mergeCell ref="A77:B77"/>
+    <mergeCell ref="C77:D77"/>
+    <mergeCell ref="A78:B78"/>
+    <mergeCell ref="C78:D78"/>
+    <mergeCell ref="A79:B79"/>
+    <mergeCell ref="C79:D79"/>
+    <mergeCell ref="A80:B80"/>
+    <mergeCell ref="C80:D80"/>
+    <mergeCell ref="A81:B81"/>
+    <mergeCell ref="C81:D81"/>
+    <mergeCell ref="A72:B72"/>
+    <mergeCell ref="C72:D72"/>
+    <mergeCell ref="A73:B73"/>
+    <mergeCell ref="C73:D73"/>
+    <mergeCell ref="A74:B74"/>
+    <mergeCell ref="C74:D74"/>
+    <mergeCell ref="A75:B75"/>
+    <mergeCell ref="C75:D75"/>
+    <mergeCell ref="A76:B76"/>
+    <mergeCell ref="C76:D76"/>
+    <mergeCell ref="A67:B67"/>
+    <mergeCell ref="C67:D67"/>
+    <mergeCell ref="A68:B68"/>
+    <mergeCell ref="C68:D68"/>
+    <mergeCell ref="A69:B69"/>
+    <mergeCell ref="C69:D69"/>
+    <mergeCell ref="A70:B70"/>
+    <mergeCell ref="C70:D70"/>
+    <mergeCell ref="A71:B71"/>
+    <mergeCell ref="C71:D71"/>
+    <mergeCell ref="A62:B62"/>
+    <mergeCell ref="C62:D62"/>
+    <mergeCell ref="A63:B63"/>
+    <mergeCell ref="C63:D63"/>
+    <mergeCell ref="A64:B64"/>
+    <mergeCell ref="C64:D64"/>
+    <mergeCell ref="A65:B65"/>
+    <mergeCell ref="C65:D65"/>
+    <mergeCell ref="A66:B66"/>
+    <mergeCell ref="C66:D66"/>
+    <mergeCell ref="A57:B57"/>
+    <mergeCell ref="C57:D57"/>
+    <mergeCell ref="A58:B58"/>
+    <mergeCell ref="C58:D58"/>
+    <mergeCell ref="A59:B59"/>
+    <mergeCell ref="C59:D59"/>
+    <mergeCell ref="A60:B60"/>
+    <mergeCell ref="C60:D60"/>
+    <mergeCell ref="A61:B61"/>
+    <mergeCell ref="C61:D61"/>
+    <mergeCell ref="A52:B52"/>
+    <mergeCell ref="C52:D52"/>
+    <mergeCell ref="A53:B53"/>
+    <mergeCell ref="C53:D53"/>
+    <mergeCell ref="A54:B54"/>
+    <mergeCell ref="C54:D54"/>
+    <mergeCell ref="A55:B55"/>
+    <mergeCell ref="C55:D55"/>
+    <mergeCell ref="A56:B56"/>
+    <mergeCell ref="C56:D56"/>
+    <mergeCell ref="A47:B47"/>
+    <mergeCell ref="C47:D47"/>
+    <mergeCell ref="A48:B48"/>
+    <mergeCell ref="C48:D48"/>
+    <mergeCell ref="A49:B49"/>
+    <mergeCell ref="C49:D49"/>
+    <mergeCell ref="A50:B50"/>
+    <mergeCell ref="C50:D50"/>
+    <mergeCell ref="A51:B51"/>
+    <mergeCell ref="C51:D51"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="C42:D42"/>
+    <mergeCell ref="A43:B43"/>
+    <mergeCell ref="C43:D43"/>
+    <mergeCell ref="A44:B44"/>
+    <mergeCell ref="C44:D44"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="C45:D45"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="C46:D46"/>
+    <mergeCell ref="A37:B37"/>
+    <mergeCell ref="C37:D37"/>
+    <mergeCell ref="A38:B38"/>
+    <mergeCell ref="C38:D38"/>
+    <mergeCell ref="A39:B39"/>
+    <mergeCell ref="C39:D39"/>
+    <mergeCell ref="A40:B40"/>
+    <mergeCell ref="C40:D40"/>
+    <mergeCell ref="A41:B41"/>
+    <mergeCell ref="C41:D41"/>
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="C32:D32"/>
+    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="C33:D33"/>
+    <mergeCell ref="A34:B34"/>
+    <mergeCell ref="C34:D34"/>
+    <mergeCell ref="A35:B35"/>
+    <mergeCell ref="C35:D35"/>
+    <mergeCell ref="A36:B36"/>
+    <mergeCell ref="C36:D36"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="A29:B29"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="C30:D30"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="C31:D31"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="C6:D6"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="F3" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>

</xml_diff>